<commit_message>
R first painted dashboard
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisfernandoquezada/Documents/GitHub/omrat/src/R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCF721E-0C10-314F-A5E0-AE38CB754228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD040543-7E01-4F4F-9DA9-61E55D1DA8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19380" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="861">
   <si>
     <t>LABEL</t>
   </si>
@@ -1779,18 +1779,6 @@
   </si>
   <si>
     <t>dashboard_title</t>
-  </si>
-  <si>
-    <t>Evaluación del riesgo de sarampión y rubéola</t>
-  </si>
-  <si>
-    <t>Measles and rubella risk assessment</t>
-  </si>
-  <si>
-    <t>Avaliação de risco de sarampo e rubéola</t>
-  </si>
-  <si>
-    <t>Évaluation du risque de la rougeole et de la rubéole</t>
   </si>
   <si>
     <t>dashboard_tab_title</t>
@@ -2646,6 +2634,9 @@
   </si>
   <si>
     <t>Cerrar</t>
+  </si>
+  <si>
+    <t>Evaluación de polio</t>
   </si>
 </sst>
 </file>
@@ -3091,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C7D9D-C4E2-B94C-B003-B8DCE10597B7}">
   <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5758,7 +5749,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>542</v>
       </c>
@@ -5889,7 +5880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5934,29 +5927,20 @@
         <v>576</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>577</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="D3" t="s">
-        <v>580</v>
-      </c>
-      <c r="E3" t="s">
-        <v>581</v>
+        <v>860</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="7"/>
@@ -5964,7 +5948,7 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>224</v>
@@ -5981,19 +5965,19 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>581</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>585</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>586</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6032,10 +6016,10 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="7"/>
@@ -6043,10 +6027,10 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="7"/>
@@ -6054,10 +6038,10 @@
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7"/>
@@ -6065,10 +6049,10 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
@@ -6076,10 +6060,10 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
@@ -6087,10 +6071,10 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="7"/>
@@ -6098,44 +6082,44 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>510</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>512</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7"/>
@@ -6143,10 +6127,10 @@
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="7"/>
@@ -6154,24 +6138,24 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>610</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>614</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>121</v>
@@ -6188,7 +6172,7 @@
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>145</v>
@@ -6205,7 +6189,7 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>164</v>
@@ -6222,7 +6206,7 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>193</v>
@@ -6239,41 +6223,41 @@
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>561</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>121</v>
@@ -6290,7 +6274,7 @@
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>145</v>
@@ -6307,7 +6291,7 @@
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>164</v>
@@ -6324,7 +6308,7 @@
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>193</v>
@@ -6341,61 +6325,61 @@
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>561</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>629</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>633</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>634</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="7"/>
@@ -6403,7 +6387,7 @@
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>306</v>
@@ -6420,10 +6404,10 @@
     </row>
     <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="7"/>
@@ -6431,7 +6415,7 @@
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>306</v>
@@ -6448,7 +6432,7 @@
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>312</v>
@@ -6465,10 +6449,10 @@
     </row>
     <row r="38" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="7"/>
@@ -6476,10 +6460,10 @@
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="7"/>
@@ -6487,10 +6471,10 @@
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="7"/>
@@ -6498,10 +6482,10 @@
     </row>
     <row r="41" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="7"/>
@@ -6509,10 +6493,10 @@
     </row>
     <row r="42" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="7"/>
@@ -6520,36 +6504,36 @@
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>653</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>657</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>658</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6633,10 +6617,10 @@
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="7"/>
@@ -6666,7 +6650,7 @@
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>72</v>
@@ -6697,16 +6681,16 @@
         <v>277</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6779,10 +6763,10 @@
     </row>
     <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="7"/>
@@ -6790,10 +6774,10 @@
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="7"/>
@@ -6801,10 +6785,10 @@
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="7"/>
@@ -6832,7 +6816,7 @@
         <v>310</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="7"/>
@@ -6857,10 +6841,10 @@
     </row>
     <row r="66" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="7"/>
@@ -6868,10 +6852,10 @@
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="7"/>
@@ -6879,44 +6863,44 @@
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>677</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>681</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>682</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="7"/>
@@ -6924,10 +6908,10 @@
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="7"/>
@@ -6935,10 +6919,10 @@
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="7"/>
@@ -6946,10 +6930,10 @@
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="7"/>
@@ -6957,10 +6941,10 @@
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="7"/>
@@ -6968,10 +6952,10 @@
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="7"/>
@@ -6979,10 +6963,10 @@
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="7"/>
@@ -6990,10 +6974,10 @@
     </row>
     <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="7"/>
@@ -7001,10 +6985,10 @@
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="7"/>
@@ -7012,10 +6996,10 @@
     </row>
     <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="7"/>
@@ -7023,10 +7007,10 @@
     </row>
     <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="7"/>
@@ -7034,7 +7018,7 @@
     </row>
     <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>135</v>
@@ -7051,7 +7035,7 @@
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>140</v>
@@ -7068,10 +7052,10 @@
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
@@ -7079,10 +7063,10 @@
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
@@ -7090,27 +7074,27 @@
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>710</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>714</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>715</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>717</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
@@ -7118,10 +7102,10 @@
     </row>
     <row r="87" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
@@ -7129,10 +7113,10 @@
     </row>
     <row r="88" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
@@ -7179,7 +7163,7 @@
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>74</v>
@@ -7207,7 +7191,7 @@
     </row>
     <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>130</v>
@@ -7224,27 +7208,27 @@
     </row>
     <row r="95" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>723</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>727</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>728</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>729</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="7"/>
@@ -7263,10 +7247,10 @@
     </row>
     <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="7"/>
@@ -7274,10 +7258,10 @@
     </row>
     <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="7"/>
@@ -7307,10 +7291,10 @@
     </row>
     <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="7"/>
@@ -7321,16 +7305,16 @@
         <v>327</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -7341,13 +7325,13 @@
         <v>330</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -7358,13 +7342,13 @@
         <v>332</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -7372,7 +7356,7 @@
         <v>333</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
@@ -7468,10 +7452,10 @@
     </row>
     <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="7"/>
@@ -7479,10 +7463,10 @@
     </row>
     <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C116" s="8"/>
       <c r="D116" s="7"/>
@@ -7490,10 +7474,10 @@
     </row>
     <row r="117" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="7"/>
@@ -7501,10 +7485,10 @@
     </row>
     <row r="118" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="7"/>
@@ -7512,27 +7496,27 @@
     </row>
     <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>754</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>758</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>759</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>761</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="7"/>
@@ -7540,27 +7524,27 @@
     </row>
     <row r="121" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>761</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>765</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>766</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
@@ -7568,10 +7552,10 @@
     </row>
     <row r="123" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
@@ -7579,10 +7563,10 @@
     </row>
     <row r="124" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="7"/>
@@ -7747,7 +7731,7 @@
     </row>
     <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>173</v>
@@ -7764,10 +7748,10 @@
     </row>
     <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
@@ -7775,7 +7759,7 @@
     </row>
     <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>178</v>
@@ -7792,10 +7776,10 @@
     </row>
     <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
@@ -7803,10 +7787,10 @@
     </row>
     <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
@@ -7814,10 +7798,10 @@
     </row>
     <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="7"/>
@@ -7825,10 +7809,10 @@
     </row>
     <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="7"/>
@@ -7836,10 +7820,10 @@
     </row>
     <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="7"/>
@@ -7847,10 +7831,10 @@
     </row>
     <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
@@ -7875,10 +7859,10 @@
     </row>
     <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
@@ -7886,7 +7870,7 @@
     </row>
     <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>306</v>
@@ -7903,10 +7887,10 @@
     </row>
     <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
@@ -7914,10 +7898,10 @@
     </row>
     <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="C149" s="8"/>
       <c r="D149" s="7"/>
@@ -7925,10 +7909,10 @@
     </row>
     <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="7"/>
@@ -7936,10 +7920,10 @@
     </row>
     <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="7"/>
@@ -7947,7 +7931,7 @@
     </row>
     <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B152" s="9" t="s">
         <v>395</v>
@@ -7958,10 +7942,10 @@
     </row>
     <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="7"/>
@@ -7969,10 +7953,10 @@
     </row>
     <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="7"/>
@@ -7980,10 +7964,10 @@
     </row>
     <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="7"/>
@@ -8019,7 +8003,7 @@
     </row>
     <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>377</v>
@@ -8036,10 +8020,10 @@
     </row>
     <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C159" s="8"/>
       <c r="D159" s="7"/>
@@ -8047,10 +8031,10 @@
     </row>
     <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="7" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C160" s="8"/>
       <c r="D160" s="7"/>
@@ -8061,7 +8045,7 @@
         <v>384</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C161" s="8"/>
       <c r="D161" s="7"/>
@@ -8157,10 +8141,10 @@
     </row>
     <row r="170" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A170" s="7" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="7"/>
@@ -8168,10 +8152,10 @@
     </row>
     <row r="171" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="7"/>
@@ -8179,10 +8163,10 @@
     </row>
     <row r="172" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -8190,7 +8174,7 @@
     </row>
     <row r="173" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>393</v>
@@ -8201,10 +8185,10 @@
     </row>
     <row r="174" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
@@ -8212,7 +8196,7 @@
     </row>
     <row r="175" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="B175" s="9" t="s">
         <v>397</v>
@@ -8223,10 +8207,10 @@
     </row>
     <row r="176" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
@@ -8234,10 +8218,10 @@
     </row>
     <row r="177" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
@@ -8351,19 +8335,19 @@
     </row>
     <row r="186" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>826</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="E186" s="3" t="s">
         <v>830</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>831</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>832</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>833</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -8423,7 +8407,7 @@
     </row>
     <row r="192" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B192" s="9" t="s">
         <v>423</v>
@@ -8434,10 +8418,10 @@
     </row>
     <row r="193" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
@@ -8445,10 +8429,10 @@
     </row>
     <row r="194" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
@@ -8456,10 +8440,10 @@
     </row>
     <row r="195" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
@@ -8506,90 +8490,90 @@
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -8599,26 +8583,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
-      <UserInfo>
-        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
-        <AccountId>180</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
-        <AccountId>212</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8876,22 +8846,32 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
+      <UserInfo>
+        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
+        <AccountId>180</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
+        <AccountId>212</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
-    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
-    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8917,9 +8897,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
+    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
general bar uses pfa filter
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891F4303-83CC-7943-B552-5CF604030278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D705D030-5B3A-0245-9A27-C374DB92C993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="883">
   <si>
     <t>LABEL</t>
   </si>
@@ -2691,6 +2691,18 @@
   </si>
   <si>
     <t>Brotes de EPV</t>
+  </si>
+  <si>
+    <t>&gt;100000 o con &lt;100000 pero que si haya tenido casos de PFA</t>
+  </si>
+  <si>
+    <t>population_pfa_filter</t>
+  </si>
+  <si>
+    <t>population_pfa_no_filter</t>
+  </si>
+  <si>
+    <t>&lt;100000 que no haya tenido casos de PFA</t>
   </si>
 </sst>
 </file>
@@ -2768,7 +2780,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2776,11 +2788,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2819,6 +2844,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5932,10 +5960,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E208"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C209" sqref="C209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8681,6 +8709,22 @@
       <c r="C208" s="8"/>
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
+    </row>
+    <row r="209" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>880</v>
+      </c>
+      <c r="B209" s="15" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>881</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>882</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E208" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
@@ -8816,6 +8860,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
+      <UserInfo>
+        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
+        <AccountId>180</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
+        <AccountId>212</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -9069,39 +9145,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
-      <UserInfo>
-        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
-        <AccountId>180</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
-        <AccountId>212</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
+    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9119,24 +9183,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
-    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
-    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(immunity): polio coverage map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D705D030-5B3A-0245-9A27-C374DB92C993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2EF345-E45F-E144-885E-0BA0A7368B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$208</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$209</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="885">
   <si>
     <t>LABEL</t>
   </si>
@@ -2703,6 +2703,12 @@
   </si>
   <si>
     <t>&lt;100000 que no haya tenido casos de PFA</t>
+  </si>
+  <si>
+    <t>immunity_polio_cob</t>
+  </si>
+  <si>
+    <t>Cobertura de Polio</t>
   </si>
 </sst>
 </file>
@@ -5960,10 +5966,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7278,95 +7284,95 @@
       <c r="E93" s="7"/>
     </row>
     <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>704</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="A94" s="7" t="s">
+        <v>883</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>884</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>704</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>705</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
-        <v>706</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>707</v>
-      </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
     </row>
     <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
     </row>
     <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="A98" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+    </row>
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>710</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E99" s="3" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B100" s="9" t="s">
         <v>716</v>
-      </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-    </row>
-    <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A100" s="7" t="s">
-        <v>717</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>718</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
@@ -7374,10 +7380,10 @@
     </row>
     <row r="101" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
@@ -7385,122 +7391,122 @@
     </row>
     <row r="102" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+    </row>
+    <row r="103" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B103" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-    </row>
-    <row r="103" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="C103" s="8"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+    </row>
+    <row r="104" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>318</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D104" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
+    <row r="105" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A105" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B104" s="9" t="s">
+      <c r="B105" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="7"/>
-      <c r="E104" s="7"/>
-    </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="C105" s="8"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+    </row>
+    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>721</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C106" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D105" s="4" t="s">
+      <c r="D106" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E105" s="4" t="s">
+      <c r="E106" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
+    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B107" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-    </row>
-    <row r="107" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="C107" s="8"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+    </row>
+    <row r="108" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>722</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D108" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+    <row r="109" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>723</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D109" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="E108" s="3" t="s">
+      <c r="E109" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
+    <row r="110" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A110" s="7" t="s">
         <v>728</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B110" s="9" t="s">
         <v>729</v>
-      </c>
-      <c r="C109" s="8"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="7"/>
-    </row>
-    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>351</v>
       </c>
       <c r="C110" s="8"/>
       <c r="D110" s="7"/>
@@ -7508,10 +7514,10 @@
     </row>
     <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>730</v>
+        <v>350</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>731</v>
+        <v>351</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="7"/>
@@ -7519,10 +7525,10 @@
     </row>
     <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>595</v>
+        <v>731</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="7"/>
@@ -7530,10 +7536,10 @@
     </row>
     <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>321</v>
+        <v>732</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>322</v>
+        <v>595</v>
       </c>
       <c r="C113" s="8"/>
       <c r="D113" s="7"/>
@@ -7541,10 +7547,10 @@
     </row>
     <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C114" s="8"/>
       <c r="D114" s="7"/>
@@ -7552,94 +7558,94 @@
     </row>
     <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>733</v>
+        <v>323</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>734</v>
+        <v>324</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+    </row>
+    <row r="117" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>327</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D117" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="E117" s="3" t="s">
         <v>738</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>329</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>739</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>329</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>331</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D119" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="E119" s="3" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>745</v>
-      </c>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8"/>
     </row>
     <row r="120" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>745</v>
+      </c>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+    </row>
+    <row r="121" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A121" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B120" s="9" t="s">
+      <c r="B121" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="C120" s="8"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-    </row>
-    <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="7"/>
@@ -7647,10 +7653,10 @@
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
@@ -7658,10 +7664,10 @@
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
@@ -7669,21 +7675,21 @@
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="7"/>
@@ -7691,21 +7697,21 @@
     </row>
     <row r="126" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C127" s="8"/>
       <c r="D127" s="7"/>
@@ -7713,10 +7719,10 @@
     </row>
     <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
-        <v>746</v>
+        <v>348</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>747</v>
+        <v>349</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="7"/>
@@ -7724,21 +7730,21 @@
     </row>
     <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="7"/>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="7"/>
@@ -7746,77 +7752,77 @@
     </row>
     <row r="131" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
     </row>
     <row r="132" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="A132" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="C132" s="8"/>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+    </row>
+    <row r="133" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>754</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>755</v>
       </c>
-      <c r="C132" s="3" t="s">
+      <c r="C133" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D133" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="E132" s="3" t="s">
+      <c r="E133" s="3" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A133" s="7" t="s">
+    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A134" s="7" t="s">
         <v>759</v>
       </c>
-      <c r="B133" s="9" t="s">
+      <c r="B134" s="9" t="s">
         <v>760</v>
       </c>
-      <c r="C133" s="8"/>
-      <c r="D133" s="7"/>
-      <c r="E133" s="7"/>
-    </row>
-    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="C134" s="8"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
+    </row>
+    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>761</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="C134" s="3" t="s">
+      <c r="C135" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D135" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="E134" s="3" t="s">
+      <c r="E135" s="3" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
-        <v>766</v>
-      </c>
-      <c r="B135" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="C135" s="8"/>
-      <c r="D135" s="7"/>
-      <c r="E135" s="7"/>
     </row>
     <row r="136" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="7"/>
@@ -7824,10 +7830,10 @@
     </row>
     <row r="137" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
@@ -7835,10 +7841,10 @@
     </row>
     <row r="138" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>352</v>
+        <v>770</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>353</v>
+        <v>771</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
@@ -7846,212 +7852,212 @@
     </row>
     <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>356</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>360</v>
-      </c>
+    <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A140" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C140" s="8"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
     </row>
     <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>356</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>361</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C141" s="3" t="s">
+      <c r="C142" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D141" s="3" t="s">
+      <c r="D142" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="E141" s="3" t="s">
+      <c r="E142" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A142" s="7" t="s">
+    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A143" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B143" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C142" s="8"/>
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
-    </row>
-    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>368</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E143" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="C143" s="8"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
     </row>
     <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>370</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>371</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C147" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D146" s="3" t="s">
+      <c r="D147" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E146" s="3" t="s">
+      <c r="E147" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A147" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="C147" s="8"/>
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
     </row>
     <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
     </row>
     <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="A149" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C149" s="8"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>772</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C149" s="3" t="s">
+      <c r="C150" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D150" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E149" s="3" t="s">
+      <c r="E150" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" s="7" t="s">
+    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" s="7" t="s">
         <v>773</v>
       </c>
-      <c r="B150" s="9" t="s">
+      <c r="B151" s="9" t="s">
         <v>774</v>
       </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-    </row>
-    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="C151" s="8"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+    </row>
+    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>775</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="C152" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D152" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E151" s="3" t="s">
+      <c r="E152" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" s="7" t="s">
-        <v>776</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C152" s="8"/>
-      <c r="D152" s="7"/>
-      <c r="E152" s="7"/>
     </row>
     <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="7"/>
@@ -8059,10 +8065,10 @@
     </row>
     <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="7"/>
@@ -8070,21 +8076,21 @@
     </row>
     <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C156" s="8"/>
       <c r="D156" s="7"/>
@@ -8092,77 +8098,77 @@
     </row>
     <row r="157" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+    <row r="158" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A158" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="C158" s="8"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>376</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C159" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D159" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E159" s="3" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" s="7" t="s">
+    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" s="7" t="s">
         <v>788</v>
       </c>
-      <c r="B159" s="9" t="s">
+      <c r="B160" s="9" t="s">
         <v>789</v>
       </c>
-      <c r="C159" s="8"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-    </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="C160" s="8"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>790</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C161" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D161" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E160" s="3" t="s">
+      <c r="E161" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B161" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="C161" s="8"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="7"/>
     </row>
     <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C162" s="8"/>
       <c r="D162" s="7"/>
@@ -8170,10 +8176,10 @@
     </row>
     <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="7"/>
@@ -8181,10 +8187,10 @@
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="7"/>
@@ -8192,10 +8198,10 @@
     </row>
     <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>395</v>
+        <v>798</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
@@ -8203,10 +8209,10 @@
     </row>
     <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>801</v>
+        <v>395</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="7"/>
@@ -8214,10 +8220,10 @@
     </row>
     <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="7"/>
@@ -8225,46 +8231,40 @@
     </row>
     <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C168" s="8"/>
       <c r="D168" s="7"/>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
-        <v>381</v>
+        <v>804</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>382</v>
+        <v>805</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>383</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>380</v>
-      </c>
+    <row r="170" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A170" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C170" s="8"/>
+      <c r="D170" s="7"/>
+      <c r="E170" s="7"/>
     </row>
     <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>806</v>
+        <v>383</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>377</v>
@@ -8280,44 +8280,50 @@
       </c>
     </row>
     <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A172" s="7" t="s">
-        <v>807</v>
-      </c>
-      <c r="B172" s="9" t="s">
-        <v>808</v>
-      </c>
-      <c r="C172" s="8"/>
-      <c r="D172" s="7"/>
-      <c r="E172" s="7"/>
+      <c r="A172" t="s">
+        <v>806</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C173" s="8"/>
       <c r="D173" s="7"/>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>384</v>
+        <v>809</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>387</v>
+        <v>811</v>
       </c>
       <c r="C175" s="8"/>
       <c r="D175" s="7"/>
@@ -8325,65 +8331,65 @@
     </row>
     <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
       <c r="E176" s="7"/>
     </row>
-    <row r="177" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C180" s="8"/>
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
     </row>
-    <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="7"/>
@@ -8391,87 +8397,87 @@
     </row>
     <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
-        <v>812</v>
+        <v>400</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>813</v>
+        <v>401</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="7"/>
       <c r="E183" s="7"/>
     </row>
-    <row r="184" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>393</v>
+        <v>817</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>820</v>
+        <v>393</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>397</v>
+        <v>820</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>823</v>
+        <v>397</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
@@ -8479,21 +8485,21 @@
     </row>
     <row r="190" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
-        <v>402</v>
+        <v>824</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>403</v>
+        <v>825</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
@@ -8501,133 +8507,133 @@
     </row>
     <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
     </row>
     <row r="193" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>406</v>
-      </c>
-      <c r="B193" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>410</v>
-      </c>
+      <c r="A193" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="B193" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C193" s="8"/>
+      <c r="D193" s="7"/>
+      <c r="E193" s="7"/>
     </row>
     <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>406</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
         <v>411</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B195" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C194" s="3" t="s">
+      <c r="C195" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="D194" s="3" t="s">
+      <c r="D195" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E194" s="3" t="s">
+      <c r="E195" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195" s="7" t="s">
+    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A196" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="B195" s="9" t="s">
+      <c r="B196" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="C195" s="8"/>
-      <c r="D195" s="7"/>
-      <c r="E195" s="7"/>
-    </row>
-    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
+      <c r="C196" s="8"/>
+      <c r="D196" s="7"/>
+      <c r="E196" s="7"/>
+    </row>
+    <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
         <v>417</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B197" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C196" s="3" t="s">
+      <c r="C197" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D196" s="3" t="s">
+      <c r="D197" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E196" s="3" t="s">
+      <c r="E197" s="3" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A197" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B197" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C197" s="8"/>
-      <c r="D197" s="7"/>
-      <c r="E197" s="7"/>
     </row>
     <row r="198" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
     </row>
-    <row r="199" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A199" t="s">
+    <row r="199" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A199" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B199" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C199" s="8"/>
+      <c r="D199" s="7"/>
+      <c r="E199" s="7"/>
+    </row>
+    <row r="200" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
         <v>826</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B200" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="C199" s="3" t="s">
+      <c r="C200" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D199" s="3" t="s">
+      <c r="D200" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="E199" s="3" t="s">
+      <c r="E200" s="3" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A200" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="B200" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="C200" s="8"/>
-      <c r="D200" s="7"/>
-      <c r="E200" s="7"/>
     </row>
     <row r="201" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C201" s="8"/>
       <c r="D201" s="7"/>
@@ -8635,21 +8641,21 @@
     </row>
     <row r="202" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
       <c r="E202" s="7"/>
     </row>
-    <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>403</v>
+        <v>430</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
@@ -8657,21 +8663,21 @@
     </row>
     <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
     </row>
-    <row r="205" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
-        <v>831</v>
+        <v>432</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
@@ -8679,10 +8685,10 @@
     </row>
     <row r="206" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" s="7" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>833</v>
+        <v>423</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="7"/>
@@ -8690,10 +8696,10 @@
     </row>
     <row r="207" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="7"/>
@@ -8701,33 +8707,44 @@
     </row>
     <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C208" s="8"/>
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
     </row>
-    <row r="209" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
+    <row r="209" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A209" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B209" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C209" s="8"/>
+      <c r="D209" s="7"/>
+      <c r="E209" s="7"/>
+    </row>
+    <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
         <v>880</v>
       </c>
-      <c r="B209" s="15" t="s">
+      <c r="B210" s="15" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
         <v>881</v>
       </c>
-      <c r="B210" s="4" t="s">
+      <c r="B211" s="4" t="s">
         <v>882</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E208" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E209" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8869,29 +8886,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
-      <UserInfo>
-        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
-        <AccountId>180</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
-        <AccountId>212</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -9145,6 +9139,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
+      <UserInfo>
+        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
+        <AccountId>180</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
+        <AccountId>212</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
   <ds:schemaRefs>
@@ -9154,18 +9171,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
-    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
-    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9183,4 +9188,16 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
+    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(immunity): ipv2 coverage map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2EF345-E45F-E144-885E-0BA0A7368B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE17676-5D77-2B44-8CEB-0E01EF8650E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$210</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="887">
   <si>
     <t>LABEL</t>
   </si>
@@ -2709,6 +2709,12 @@
   </si>
   <si>
     <t>Cobertura de Polio</t>
+  </si>
+  <si>
+    <t>immunity_ipv2_cob</t>
+  </si>
+  <si>
+    <t>Cobertura de IPV2</t>
   </si>
 </sst>
 </file>
@@ -5966,10 +5972,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7295,95 +7301,95 @@
       <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>704</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="A95" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>886</v>
+      </c>
+      <c r="C95" s="8"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>704</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>705</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D97" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
-        <v>706</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>707</v>
-      </c>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
     </row>
     <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
     </row>
     <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="A99" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>710</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="7" t="s">
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B101" s="9" t="s">
         <v>716</v>
-      </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-    </row>
-    <row r="101" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
-        <v>717</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>718</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
@@ -7391,10 +7397,10 @@
     </row>
     <row r="102" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
@@ -7402,122 +7408,122 @@
     </row>
     <row r="103" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+    </row>
+    <row r="104" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B103" s="9" t="s">
+      <c r="B104" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-    </row>
-    <row r="104" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="C104" s="8"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>318</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E105" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
+    <row r="106" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A106" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B106" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
-    </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="C106" s="8"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>721</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C107" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D107" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E106" s="4" t="s">
+      <c r="E107" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="B108" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
-    </row>
-    <row r="108" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="C108" s="8"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+    </row>
+    <row r="109" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>722</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D109" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E108" s="3" t="s">
+      <c r="E109" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+    <row r="110" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>723</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C110" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D110" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="E110" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
+    <row r="111" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A111" s="7" t="s">
         <v>728</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B111" s="9" t="s">
         <v>729</v>
-      </c>
-      <c r="C110" s="8"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-    </row>
-    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>351</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="7"/>
@@ -7525,10 +7531,10 @@
     </row>
     <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>730</v>
+        <v>350</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>731</v>
+        <v>351</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="7"/>
@@ -7536,10 +7542,10 @@
     </row>
     <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>595</v>
+        <v>731</v>
       </c>
       <c r="C113" s="8"/>
       <c r="D113" s="7"/>
@@ -7547,10 +7553,10 @@
     </row>
     <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>321</v>
+        <v>732</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>322</v>
+        <v>595</v>
       </c>
       <c r="C114" s="8"/>
       <c r="D114" s="7"/>
@@ -7558,10 +7564,10 @@
     </row>
     <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="7"/>
@@ -7569,94 +7575,94 @@
     </row>
     <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>733</v>
+        <v>323</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>734</v>
+        <v>324</v>
       </c>
       <c r="C116" s="8"/>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C117" s="8"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>327</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D118" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E118" s="3" t="s">
         <v>738</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>329</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>739</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>329</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>331</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D120" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E120" s="3" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>745</v>
-      </c>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
     </row>
     <row r="121" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>745</v>
+      </c>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+    </row>
+    <row r="122" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A122" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B121" s="9" t="s">
+      <c r="B122" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="C121" s="8"/>
-      <c r="D121" s="7"/>
-      <c r="E121" s="7"/>
-    </row>
-    <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
@@ -7664,10 +7670,10 @@
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
@@ -7675,10 +7681,10 @@
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="7"/>
@@ -7686,21 +7692,21 @@
     </row>
     <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="7"/>
@@ -7708,21 +7714,21 @@
     </row>
     <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C127" s="8"/>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="7"/>
@@ -7730,10 +7736,10 @@
     </row>
     <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
-        <v>746</v>
+        <v>348</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>747</v>
+        <v>349</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="7"/>
@@ -7741,21 +7747,21 @@
     </row>
     <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="7"/>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="7"/>
@@ -7763,77 +7769,77 @@
     </row>
     <row r="132" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
     </row>
     <row r="133" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="A133" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="C133" s="8"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+    </row>
+    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>754</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>755</v>
       </c>
-      <c r="C133" s="3" t="s">
+      <c r="C134" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="D134" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="E133" s="3" t="s">
+      <c r="E134" s="3" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" s="7" t="s">
+    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A135" s="7" t="s">
         <v>759</v>
       </c>
-      <c r="B134" s="9" t="s">
+      <c r="B135" s="9" t="s">
         <v>760</v>
       </c>
-      <c r="C134" s="8"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
-    </row>
-    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="C135" s="8"/>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>761</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="C135" s="3" t="s">
+      <c r="C136" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="D135" s="3" t="s">
+      <c r="D136" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="E135" s="3" t="s">
+      <c r="E136" s="3" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A136" s="7" t="s">
-        <v>766</v>
-      </c>
-      <c r="B136" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="C136" s="8"/>
-      <c r="D136" s="7"/>
-      <c r="E136" s="7"/>
     </row>
     <row r="137" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
@@ -7841,10 +7847,10 @@
     </row>
     <row r="138" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
@@ -7852,10 +7858,10 @@
     </row>
     <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>352</v>
+        <v>770</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>353</v>
+        <v>771</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
@@ -7863,212 +7869,212 @@
     </row>
     <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>356</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>360</v>
-      </c>
+    <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A141" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C141" s="8"/>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
     </row>
     <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>356</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>361</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C142" s="3" t="s">
+      <c r="C143" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D142" s="3" t="s">
+      <c r="D143" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="E142" s="3" t="s">
+      <c r="E143" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A143" s="7" t="s">
+    <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A144" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="B143" s="9" t="s">
+      <c r="B144" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
-    </row>
-    <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>368</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="C144" s="8"/>
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
     </row>
     <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>370</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>371</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="C148" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D148" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E147" s="3" t="s">
+      <c r="E148" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A148" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B148" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="C148" s="8"/>
-      <c r="D148" s="7"/>
-      <c r="E148" s="7"/>
     </row>
     <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C149" s="8"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
     </row>
     <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="A150" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C150" s="8"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+    </row>
+    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>772</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="C151" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D151" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E150" s="3" t="s">
+      <c r="E151" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" s="7" t="s">
+    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A152" s="7" t="s">
         <v>773</v>
       </c>
-      <c r="B151" s="9" t="s">
+      <c r="B152" s="9" t="s">
         <v>774</v>
       </c>
-      <c r="C151" s="8"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="7"/>
-    </row>
-    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="C152" s="8"/>
+      <c r="D152" s="7"/>
+      <c r="E152" s="7"/>
+    </row>
+    <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>775</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B153" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C152" s="3" t="s">
+      <c r="C153" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D153" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E152" s="3" t="s">
+      <c r="E153" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="7" t="s">
-        <v>776</v>
-      </c>
-      <c r="B153" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C153" s="8"/>
-      <c r="D153" s="7"/>
-      <c r="E153" s="7"/>
     </row>
     <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="7"/>
@@ -8076,10 +8082,10 @@
     </row>
     <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="7"/>
@@ -8087,21 +8093,21 @@
     </row>
     <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C156" s="8"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
@@ -8109,77 +8115,77 @@
     </row>
     <row r="158" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+    <row r="159" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A159" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="C159" s="8"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>376</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C160" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D160" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E160" s="3" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="7" t="s">
+    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" s="7" t="s">
         <v>788</v>
       </c>
-      <c r="B160" s="9" t="s">
+      <c r="B161" s="9" t="s">
         <v>789</v>
       </c>
-      <c r="C160" s="8"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
-    </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+      <c r="C161" s="8"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
+    </row>
+    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>790</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C161" s="3" t="s">
+      <c r="C162" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D162" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E161" s="3" t="s">
+      <c r="E162" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B162" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="C162" s="8"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="7"/>
     </row>
     <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="7"/>
@@ -8187,10 +8193,10 @@
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="7"/>
@@ -8198,10 +8204,10 @@
     </row>
     <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
@@ -8209,10 +8215,10 @@
     </row>
     <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>395</v>
+        <v>798</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="7"/>
@@ -8220,10 +8226,10 @@
     </row>
     <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>801</v>
+        <v>395</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="7"/>
@@ -8231,10 +8237,10 @@
     </row>
     <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C168" s="8"/>
       <c r="D168" s="7"/>
@@ -8242,46 +8248,40 @@
     </row>
     <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="7" t="s">
-        <v>381</v>
+        <v>804</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>382</v>
+        <v>805</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>383</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>380</v>
-      </c>
+    <row r="171" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A171" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C171" s="8"/>
+      <c r="D171" s="7"/>
+      <c r="E171" s="7"/>
     </row>
     <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>806</v>
+        <v>383</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>377</v>
@@ -8297,44 +8297,50 @@
       </c>
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" s="7" t="s">
-        <v>807</v>
-      </c>
-      <c r="B173" s="9" t="s">
-        <v>808</v>
-      </c>
-      <c r="C173" s="8"/>
-      <c r="D173" s="7"/>
-      <c r="E173" s="7"/>
+      <c r="A173" t="s">
+        <v>806</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
-        <v>384</v>
+        <v>809</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C175" s="8"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>387</v>
+        <v>811</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
@@ -8342,65 +8348,65 @@
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C180" s="8"/>
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
     </row>
-    <row r="181" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="7"/>
@@ -8408,87 +8414,87 @@
     </row>
     <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="7"/>
       <c r="E183" s="7"/>
     </row>
-    <row r="184" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
-        <v>812</v>
+        <v>400</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>813</v>
+        <v>401</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>393</v>
+        <v>817</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>820</v>
+        <v>393</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>397</v>
+        <v>820</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>823</v>
+        <v>397</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
@@ -8496,21 +8502,21 @@
     </row>
     <row r="191" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
-        <v>402</v>
+        <v>824</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>403</v>
+        <v>825</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
@@ -8518,133 +8524,133 @@
     </row>
     <row r="193" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
     <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>406</v>
-      </c>
-      <c r="B194" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D194" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E194" s="3" t="s">
-        <v>410</v>
-      </c>
+      <c r="A194" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="B194" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C194" s="8"/>
+      <c r="D194" s="7"/>
+      <c r="E194" s="7"/>
     </row>
     <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>406</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
         <v>411</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B196" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C195" s="3" t="s">
+      <c r="C196" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="D195" s="3" t="s">
+      <c r="D196" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E195" s="3" t="s">
+      <c r="E196" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" s="7" t="s">
+    <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A197" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="B196" s="9" t="s">
+      <c r="B197" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="C196" s="8"/>
-      <c r="D196" s="7"/>
-      <c r="E196" s="7"/>
-    </row>
-    <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
+      <c r="C197" s="8"/>
+      <c r="D197" s="7"/>
+      <c r="E197" s="7"/>
+    </row>
+    <row r="198" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
         <v>417</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B198" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C197" s="3" t="s">
+      <c r="C198" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D197" s="3" t="s">
+      <c r="D198" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E197" s="3" t="s">
+      <c r="E198" s="3" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A198" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B198" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C198" s="8"/>
-      <c r="D198" s="7"/>
-      <c r="E198" s="7"/>
     </row>
     <row r="199" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
+    <row r="200" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A200" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B200" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C200" s="8"/>
+      <c r="D200" s="7"/>
+      <c r="E200" s="7"/>
+    </row>
+    <row r="201" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
         <v>826</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="B201" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="C200" s="3" t="s">
+      <c r="C201" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D200" s="3" t="s">
+      <c r="D201" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="E200" s="3" t="s">
+      <c r="E201" s="3" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A201" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="B201" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="C201" s="8"/>
-      <c r="D201" s="7"/>
-      <c r="E201" s="7"/>
     </row>
     <row r="202" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
@@ -8652,21 +8658,21 @@
     </row>
     <row r="203" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
       <c r="E203" s="7"/>
     </row>
-    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>403</v>
+        <v>430</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="7"/>
@@ -8674,21 +8680,21 @@
     </row>
     <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
     </row>
-    <row r="206" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A206" s="7" t="s">
-        <v>831</v>
+        <v>432</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="7"/>
@@ -8696,10 +8702,10 @@
     </row>
     <row r="207" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>833</v>
+        <v>423</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="7"/>
@@ -8707,10 +8713,10 @@
     </row>
     <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" s="7" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C208" s="8"/>
       <c r="D208" s="7"/>
@@ -8718,33 +8724,44 @@
     </row>
     <row r="209" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C209" s="8"/>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
     </row>
     <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
+      <c r="A210" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B210" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C210" s="8"/>
+      <c r="D210" s="7"/>
+      <c r="E210" s="7"/>
+    </row>
+    <row r="211" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
         <v>880</v>
       </c>
-      <c r="B210" s="15" t="s">
+      <c r="B211" s="15" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
         <v>881</v>
       </c>
-      <c r="B211" s="4" t="s">
+      <c r="B212" s="4" t="s">
         <v>882</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E209" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E210" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(immunity): effective coverage map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE17676-5D77-2B44-8CEB-0E01EF8650E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4244B7A9-AC5C-0B45-A840-14D7150EDF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$210</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$213</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="893">
   <si>
     <t>LABEL</t>
   </si>
@@ -2708,13 +2708,31 @@
     <t>immunity_polio_cob</t>
   </si>
   <si>
-    <t>Cobertura de Polio</t>
-  </si>
-  <si>
     <t>immunity_ipv2_cob</t>
   </si>
   <si>
     <t>Cobertura de IPV2</t>
+  </si>
+  <si>
+    <t>Cobertura de Polio 3</t>
+  </si>
+  <si>
+    <t>immunity_effective_cob</t>
+  </si>
+  <si>
+    <t>Cobertura de Polio 3 exitosa</t>
+  </si>
+  <si>
+    <t>immunity_effective_cob_text</t>
+  </si>
+  <si>
+    <t>¿Si el país llevó a cabo una campaña de vacunación contra la polio en 2019-2023, se alcanzó una cobertura &gt;95% en el municipio?</t>
+  </si>
+  <si>
+    <t>immunity_legend_effective</t>
+  </si>
+  <si>
+    <t>Cobertura efectiva</t>
   </si>
 </sst>
 </file>
@@ -5972,10 +5990,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7294,7 +7312,7 @@
         <v>883</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="7"/>
@@ -7302,261 +7320,261 @@
     </row>
     <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
+        <v>884</v>
+      </c>
+      <c r="B95" s="9" t="s">
         <v>885</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>886</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>704</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>705</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>143</v>
-      </c>
+      <c r="A96" s="7" t="s">
+        <v>887</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>888</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+    </row>
+    <row r="97" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>890</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
     </row>
     <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>706</v>
+        <v>891</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>707</v>
+        <v>892</v>
       </c>
       <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
     </row>
     <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
-        <v>708</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>709</v>
-      </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
+      <c r="A99" t="s">
+        <v>704</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>711</v>
+        <v>140</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>712</v>
+        <v>141</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>713</v>
+        <v>142</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>714</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
     </row>
-    <row r="102" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
       <c r="E102" s="8"/>
     </row>
-    <row r="103" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
+    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>710</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>716</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+    </row>
+    <row r="105" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A105" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
+    </row>
+    <row r="106" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" s="7" t="s">
         <v>719</v>
       </c>
-      <c r="B103" s="9" t="s">
+      <c r="B106" s="9" t="s">
         <v>720</v>
       </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-    </row>
-    <row r="104" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+    </row>
+    <row r="107" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B104" s="9" t="s">
+      <c r="B107" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="7"/>
-      <c r="E104" s="7"/>
-    </row>
-    <row r="105" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="C107" s="8"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+    </row>
+    <row r="108" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>318</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="D108" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
+    <row r="109" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A109" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B109" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-    </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="C109" s="8"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>721</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C110" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D110" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E107" s="4" t="s">
+      <c r="E110" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
+    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B111" s="9" t="s">
         <v>326</v>
-      </c>
-      <c r="C108" s="8"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="7"/>
-    </row>
-    <row r="109" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>722</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>723</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
-        <v>728</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>729</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="C112" s="8"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>731</v>
-      </c>
-      <c r="C113" s="8"/>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-    </row>
-    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>722</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>723</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>595</v>
+        <v>729</v>
       </c>
       <c r="C114" s="8"/>
       <c r="D114" s="7"/>
@@ -7564,10 +7582,10 @@
     </row>
     <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>321</v>
+        <v>350</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>322</v>
+        <v>351</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="7"/>
@@ -7575,10 +7593,10 @@
     </row>
     <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>323</v>
+        <v>730</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>324</v>
+        <v>731</v>
       </c>
       <c r="C116" s="8"/>
       <c r="D116" s="7"/>
@@ -7586,116 +7604,116 @@
     </row>
     <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>734</v>
+        <v>595</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C118" s="8"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+    </row>
+    <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C119" s="8"/>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+    </row>
+    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C120" s="8"/>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>327</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D121" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="E121" s="3" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+    <row r="122" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>329</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D122" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E122" s="3" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+    <row r="123" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>331</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C123" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="D120" s="3" t="s">
+      <c r="D123" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="E120" s="3" t="s">
+      <c r="E123" s="3" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
+    <row r="124" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A124" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="B121" s="9" t="s">
+      <c r="B124" s="9" t="s">
         <v>745</v>
       </c>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
-    </row>
-    <row r="122" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+    </row>
+    <row r="125" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A125" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B122" s="9" t="s">
+      <c r="B125" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="C122" s="8"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
-    </row>
-    <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="C123" s="8"/>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
-    </row>
-    <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="B124" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="C124" s="8"/>
-      <c r="D124" s="7"/>
-      <c r="E124" s="7"/>
-    </row>
-    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>341</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="7"/>
@@ -7703,32 +7721,32 @@
     </row>
     <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="C127" s="8"/>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="7"/>
@@ -7736,143 +7754,143 @@
     </row>
     <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="7"/>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
-        <v>746</v>
+        <v>344</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>747</v>
+        <v>345</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="7"/>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
-        <v>748</v>
+        <v>346</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>749</v>
+        <v>347</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
-        <v>750</v>
+        <v>348</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>751</v>
+        <v>349</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>754</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>758</v>
-      </c>
+    <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A134" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="C134" s="8"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
     </row>
     <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
-        <v>759</v>
+        <v>750</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>760</v>
+        <v>751</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
     </row>
     <row r="136" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>761</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>762</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>765</v>
-      </c>
+      <c r="A136" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="C136" s="8"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
     </row>
     <row r="137" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A137" s="7" t="s">
-        <v>766</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="C137" s="8"/>
-      <c r="D137" s="7"/>
-      <c r="E137" s="7"/>
+      <c r="A137" t="s">
+        <v>754</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="138" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>768</v>
+        <v>759</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
     </row>
     <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A139" s="7" t="s">
-        <v>770</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>771</v>
-      </c>
-      <c r="C139" s="8"/>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
+      <c r="A139" t="s">
+        <v>761</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
-        <v>352</v>
+        <v>766</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>353</v>
+        <v>767</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
@@ -7880,55 +7898,43 @@
     </row>
     <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
-        <v>354</v>
+        <v>768</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>355</v>
+        <v>769</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="7"/>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>356</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>361</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E143" s="3" t="s">
-        <v>365</v>
-      </c>
+    <row r="142" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A142" s="7" t="s">
+        <v>770</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="C142" s="8"/>
+      <c r="D142" s="7"/>
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A143" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C143" s="8"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
     </row>
     <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>171</v>
+        <v>355</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
@@ -7936,289 +7942,301 @@
     </row>
     <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>173</v>
+        <v>357</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>174</v>
+        <v>358</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>175</v>
+        <v>359</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>176</v>
+        <v>360</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>178</v>
+        <v>362</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>179</v>
+        <v>363</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>180</v>
+        <v>364</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>370</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>186</v>
-      </c>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A147" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C147" s="8"/>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
     </row>
     <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A149" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B149" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="C149" s="8"/>
-      <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
+      <c r="A149" t="s">
+        <v>369</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="B150" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
+      <c r="A150" t="s">
+        <v>370</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>772</v>
+        <v>371</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
-        <v>773</v>
+        <v>372</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>774</v>
+        <v>373</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
     </row>
     <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>775</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>181</v>
-      </c>
+      <c r="A153" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C153" s="8"/>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
     </row>
     <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" s="7" t="s">
-        <v>776</v>
-      </c>
-      <c r="B154" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C154" s="8"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
+      <c r="A154" t="s">
+        <v>772</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
     </row>
     <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" s="7" t="s">
-        <v>780</v>
-      </c>
-      <c r="B156" s="9" t="s">
-        <v>781</v>
-      </c>
-      <c r="C156" s="8"/>
-      <c r="D156" s="7"/>
-      <c r="E156" s="7"/>
+      <c r="A156" t="s">
+        <v>775</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="C159" s="8"/>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
     </row>
     <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>376</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E160" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="C160" s="8"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C161" s="8"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>790</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>309</v>
-      </c>
+    <row r="162" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A162" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="C162" s="8"/>
+      <c r="D162" s="7"/>
+      <c r="E162" s="7"/>
     </row>
     <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B163" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="C163" s="8"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="7"/>
+      <c r="A163" t="s">
+        <v>376</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
     </row>
     <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" s="7" t="s">
-        <v>795</v>
-      </c>
-      <c r="B165" s="9" t="s">
-        <v>796</v>
-      </c>
-      <c r="C165" s="8"/>
-      <c r="D165" s="7"/>
-      <c r="E165" s="7"/>
+      <c r="A165" t="s">
+        <v>790</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="7"/>
@@ -8226,10 +8244,10 @@
     </row>
     <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>395</v>
+        <v>794</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="7"/>
@@ -8237,10 +8255,10 @@
     </row>
     <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="C168" s="8"/>
       <c r="D168" s="7"/>
@@ -8248,10 +8266,10 @@
     </row>
     <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
@@ -8259,99 +8277,99 @@
     </row>
     <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="7" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>805</v>
+        <v>395</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
-        <v>381</v>
+        <v>800</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>382</v>
+        <v>801</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="7"/>
       <c r="E171" s="7"/>
     </row>
     <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>383</v>
-      </c>
-      <c r="B172" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D172" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A172" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="B172" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="C172" s="8"/>
+      <c r="D172" s="7"/>
+      <c r="E172" s="7"/>
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>806</v>
-      </c>
-      <c r="B173" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D173" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A173" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="B173" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="C173" s="8"/>
+      <c r="D173" s="7"/>
+      <c r="E173" s="7"/>
+    </row>
+    <row r="174" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>807</v>
+        <v>381</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>808</v>
+        <v>382</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
     </row>
     <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="7" t="s">
-        <v>809</v>
-      </c>
-      <c r="B175" s="9" t="s">
-        <v>810</v>
-      </c>
-      <c r="C175" s="8"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="7"/>
-    </row>
-    <row r="176" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A176" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="B176" s="9" t="s">
-        <v>811</v>
-      </c>
-      <c r="C176" s="8"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="7"/>
+      <c r="A175" t="s">
+        <v>383</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>806</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
-        <v>386</v>
+        <v>807</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>387</v>
+        <v>808</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
@@ -8359,32 +8377,32 @@
     </row>
     <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
-        <v>388</v>
+        <v>809</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>389</v>
+        <v>810</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>391</v>
+        <v>811</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C180" s="8"/>
       <c r="D180" s="7"/>
@@ -8392,32 +8410,32 @@
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="7"/>
@@ -8425,54 +8443,54 @@
     </row>
     <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
-        <v>812</v>
+        <v>396</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>813</v>
+        <v>397</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
-        <v>814</v>
+        <v>398</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>815</v>
+        <v>399</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
-        <v>816</v>
+        <v>400</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>817</v>
+        <v>401</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>393</v>
+        <v>813</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
@@ -8480,110 +8498,98 @@
     </row>
     <row r="189" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>397</v>
+        <v>817</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>823</v>
+        <v>393</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
     </row>
-    <row r="193" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
-        <v>402</v>
+        <v>821</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
-        <v>404</v>
+        <v>822</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>405</v>
+        <v>823</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>406</v>
-      </c>
-      <c r="B195" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>410</v>
-      </c>
+    <row r="195" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A195" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="B195" s="9" t="s">
+        <v>825</v>
+      </c>
+      <c r="C195" s="8"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="7"/>
     </row>
     <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>411</v>
-      </c>
-      <c r="B196" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D196" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>414</v>
-      </c>
+      <c r="A196" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B196" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C196" s="8"/>
+      <c r="D196" s="7"/>
+      <c r="E196" s="7"/>
     </row>
     <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
@@ -8591,66 +8597,72 @@
     </row>
     <row r="198" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A199" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B199" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C199" s="8"/>
-      <c r="D199" s="7"/>
-      <c r="E199" s="7"/>
-    </row>
-    <row r="200" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>411</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
     </row>
-    <row r="201" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>826</v>
+        <v>417</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>827</v>
+        <v>418</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>828</v>
+        <v>419</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>829</v>
+        <v>420</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>830</v>
+        <v>421</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
@@ -8658,43 +8670,49 @@
     </row>
     <row r="203" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
       <c r="E203" s="7"/>
     </row>
-    <row r="204" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A204" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="B204" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="C204" s="8"/>
-      <c r="D204" s="7"/>
-      <c r="E204" s="7"/>
-    </row>
-    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>826</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>403</v>
+        <v>427</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
     </row>
-    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" s="7" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="7"/>
@@ -8702,32 +8720,32 @@
     </row>
     <row r="207" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
-        <v>831</v>
+        <v>429</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="7"/>
       <c r="E207" s="7"/>
     </row>
-    <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A208" s="7" t="s">
-        <v>832</v>
+        <v>431</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>833</v>
+        <v>403</v>
       </c>
       <c r="C208" s="8"/>
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
     </row>
-    <row r="209" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
-        <v>834</v>
+        <v>432</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>835</v>
+        <v>405</v>
       </c>
       <c r="C209" s="8"/>
       <c r="D209" s="7"/>
@@ -8735,33 +8753,66 @@
     </row>
     <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="7" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>837</v>
+        <v>423</v>
       </c>
       <c r="C210" s="8"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
     </row>
     <row r="211" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
+      <c r="A211" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="B211" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="C211" s="8"/>
+      <c r="D211" s="7"/>
+      <c r="E211" s="7"/>
+    </row>
+    <row r="212" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A212" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="B212" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="C212" s="8"/>
+      <c r="D212" s="7"/>
+      <c r="E212" s="7"/>
+    </row>
+    <row r="213" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A213" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B213" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C213" s="8"/>
+      <c r="D213" s="7"/>
+      <c r="E213" s="7"/>
+    </row>
+    <row r="214" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
         <v>880</v>
       </c>
-      <c r="B211" s="15" t="s">
+      <c r="B214" s="15" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
         <v>881</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="B215" s="4" t="s">
         <v>882</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E210" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E213" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fix: semantic changes requested
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E7C94F-3FA1-974E-A632-11E6448E4B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FDCA7E-3EFB-074F-8A9F-3384F3580CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="901">
   <si>
     <t>LABEL</t>
   </si>
@@ -2636,9 +2636,6 @@
     <t>Cerrar</t>
   </si>
   <si>
-    <t>Evaluación de polio</t>
-  </si>
-  <si>
     <t>Año de evaluación</t>
   </si>
   <si>
@@ -2693,39 +2690,24 @@
     <t>Brotes de EPV</t>
   </si>
   <si>
-    <t>&gt;100000 o con &lt;100000 pero que si haya tenido casos de PFA</t>
-  </si>
-  <si>
     <t>population_pfa_filter</t>
   </si>
   <si>
     <t>population_pfa_no_filter</t>
   </si>
   <si>
-    <t>&lt;100000 que no haya tenido casos de PFA</t>
-  </si>
-  <si>
     <t>immunity_polio_cob</t>
   </si>
   <si>
     <t>immunity_ipv2_cob</t>
   </si>
   <si>
-    <t>Cobertura de IPV2</t>
-  </si>
-  <si>
-    <t>Cobertura de Polio 3</t>
-  </si>
-  <si>
     <t>immunity_effective_cob</t>
   </si>
   <si>
     <t>immunity_effective_cob_text</t>
   </si>
   <si>
-    <t>¿Si el país llevó a cabo una campaña de vacunación contra la polio en 2019-2023, se alcanzó una cobertura &gt;95% en el municipio?</t>
-  </si>
-  <si>
     <t>immunity_legend_effective</t>
   </si>
   <si>
@@ -2744,13 +2726,37 @@
     <t>IPV2 (Puntaje)</t>
   </si>
   <si>
-    <t>Cobertura de Polio 3 efectiva</t>
-  </si>
-  <si>
     <t>immunity_effective_score</t>
   </si>
   <si>
-    <t>Cobertura de Polio 3 efectiva (Puntaje)</t>
+    <t>Evaluación de riesgo polio</t>
+  </si>
+  <si>
+    <t>Riesgo alto</t>
+  </si>
+  <si>
+    <t>Riesgo bajo</t>
+  </si>
+  <si>
+    <t>&gt;100 000 menores de 15 años o con &lt;100 000 menores de 15 años, pero que tuvo casos de PFA en el último año</t>
+  </si>
+  <si>
+    <t>&lt;100000 menores de 15 años que no haya tenido casos de PFA en el último año</t>
+  </si>
+  <si>
+    <t>Cobertura con Polio 3</t>
+  </si>
+  <si>
+    <t>Cobertura con IPV2</t>
+  </si>
+  <si>
+    <t>Campaña de polio con cobertura &gt;95%</t>
+  </si>
+  <si>
+    <t>Campaña de polio con cobertura &gt;95% (Puntaje)</t>
+  </si>
+  <si>
+    <t>Campaña de vacunación en los últimos 5 años que alcanzó una cobertura &gt;95%</t>
   </si>
 </sst>
 </file>
@@ -6010,8 +6016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6062,7 +6068,7 @@
         <v>577</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>860</v>
+        <v>891</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6081,7 +6087,7 @@
         <v>580</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>225</v>
@@ -6285,7 +6291,7 @@
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>121</v>
@@ -6302,7 +6308,7 @@
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>145</v>
@@ -6319,20 +6325,20 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>876</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>877</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>878</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -6441,27 +6447,27 @@
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>872</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>873</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>874</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>870</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>871</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>872</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>145</v>
@@ -6478,7 +6484,7 @@
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>121</v>
@@ -6495,7 +6501,7 @@
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>611</v>
@@ -6597,7 +6603,7 @@
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>121</v>
@@ -6614,7 +6620,7 @@
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>145</v>
@@ -6631,20 +6637,20 @@
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>863</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>864</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>865</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>861</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>862</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>863</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -6861,7 +6867,7 @@
         <v>301</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>42</v>
+        <v>893</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>43</v>
@@ -6895,7 +6901,7 @@
         <v>303</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>52</v>
+        <v>892</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>53</v>
@@ -7327,10 +7333,10 @@
     </row>
     <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>886</v>
+        <v>896</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="7"/>
@@ -7338,10 +7344,10 @@
     </row>
     <row r="95" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
@@ -7349,10 +7355,10 @@
     </row>
     <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>885</v>
+        <v>897</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="7"/>
@@ -7360,21 +7366,21 @@
     </row>
     <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="7"/>
@@ -7382,21 +7388,21 @@
     </row>
     <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>897</v>
+        <v>890</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>888</v>
+        <v>883</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>889</v>
+        <v>900</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="7"/>
@@ -7404,10 +7410,10 @@
     </row>
     <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="7"/>
@@ -8846,20 +8852,20 @@
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
     </row>
-    <row r="217" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B217" s="15" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>881</v>
-      </c>
       <c r="B218" s="4" t="s">
-        <v>882</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -9005,6 +9011,29 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
+      <UserInfo>
+        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
+        <AccountId>180</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
+        <AccountId>212</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -9258,29 +9287,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
-      <UserInfo>
-        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
-        <AccountId>180</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
-        <AccountId>212</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
   <ds:schemaRefs>
@@ -9290,6 +9296,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
+    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9307,16 +9325,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
-    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
-    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(immunity): blue for > 100 in maps
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FDCA7E-3EFB-074F-8A9F-3384F3580CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D65D38-4044-134E-BA84-C745AB54C4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$216</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="903">
   <si>
     <t>LABEL</t>
   </si>
@@ -2757,6 +2757,12 @@
   </si>
   <si>
     <t>Campaña de vacunación en los últimos 5 años que alcanzó una cobertura &gt;95%</t>
+  </si>
+  <si>
+    <t>over_100</t>
+  </si>
+  <si>
+    <t>&gt; 100</t>
   </si>
 </sst>
 </file>
@@ -6014,10 +6020,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E218"/>
+  <dimension ref="A1:E219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7009,90 +7015,96 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>282</v>
+      <c r="A69" s="7" t="s">
+        <v>901</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>283</v>
+        <v>902</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>284</v>
+        <v>902</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>285</v>
+        <v>902</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>286</v>
+        <v>902</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>292</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>296</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
-        <v>665</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>666</v>
-      </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="7"/>
@@ -7100,133 +7112,133 @@
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="A76" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+    </row>
+    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>305</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B78" s="9" t="s">
         <v>671</v>
       </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-    </row>
-    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="C78" s="8"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+    </row>
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>311</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E79" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
+    <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B80" s="9" t="s">
         <v>673</v>
-      </c>
-      <c r="C79" s="8"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-    </row>
-    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
-        <v>674</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>675</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>676</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>582</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>585</v>
-      </c>
+      <c r="A81" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="C81" s="8"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>676</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>677</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>680</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="7" t="s">
-        <v>682</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>683</v>
-      </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="7"/>
@@ -7234,10 +7246,10 @@
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="7"/>
@@ -7245,10 +7257,10 @@
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="7"/>
@@ -7256,10 +7268,10 @@
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="7"/>
@@ -7267,10 +7279,10 @@
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="7"/>
@@ -7278,10 +7290,10 @@
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="7"/>
@@ -7289,10 +7301,10 @@
     </row>
     <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="7"/>
@@ -7300,10 +7312,10 @@
     </row>
     <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C91" s="8"/>
       <c r="D91" s="7"/>
@@ -7311,76 +7323,76 @@
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>880</v>
+        <v>702</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>896</v>
+        <v>703</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="C95" s="8"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+    </row>
+    <row r="96" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
         <v>886</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B96" s="9" t="s">
         <v>887</v>
       </c>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-    </row>
-    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
-        <v>881</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>897</v>
-      </c>
       <c r="C96" s="8"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
     </row>
     <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>889</v>
+        <v>897</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>882</v>
+        <v>888</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="7"/>
@@ -7388,127 +7400,127 @@
     </row>
     <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>885</v>
+        <v>900</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
     </row>
     <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>704</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="A102" s="7" t="s">
+        <v>884</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>885</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>704</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>705</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D104" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
-        <v>706</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>707</v>
-      </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
     </row>
     <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="A106" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+    </row>
+    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>710</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D107" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="B108" s="9" t="s">
         <v>716</v>
-      </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-    </row>
-    <row r="108" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
-        <v>717</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>718</v>
       </c>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
@@ -7516,10 +7528,10 @@
     </row>
     <row r="109" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
@@ -7527,122 +7539,122 @@
     </row>
     <row r="110" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+    </row>
+    <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A111" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B111" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C110" s="8"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-    </row>
-    <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="C111" s="8"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+    </row>
+    <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>318</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C112" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D112" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E112" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
+    <row r="113" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A113" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B113" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C112" s="8"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="C113" s="8"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+    </row>
+    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>721</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C114" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D114" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E114" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
+    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B114" s="9" t="s">
+      <c r="B115" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C114" s="8"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-    </row>
-    <row r="115" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="C115" s="8"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+    </row>
+    <row r="116" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>722</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D116" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="E116" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+    <row r="117" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>723</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D117" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="E117" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A117" s="7" t="s">
+    <row r="118" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A118" s="7" t="s">
         <v>728</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B118" s="9" t="s">
         <v>729</v>
-      </c>
-      <c r="C117" s="8"/>
-      <c r="D117" s="7"/>
-      <c r="E117" s="7"/>
-    </row>
-    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>351</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="7"/>
@@ -7650,10 +7662,10 @@
     </row>
     <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
-        <v>730</v>
+        <v>350</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>731</v>
+        <v>351</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="7"/>
@@ -7661,10 +7673,10 @@
     </row>
     <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>595</v>
+        <v>731</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="7"/>
@@ -7672,10 +7684,10 @@
     </row>
     <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
-        <v>321</v>
+        <v>732</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>322</v>
+        <v>595</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="7"/>
@@ -7683,10 +7695,10 @@
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
@@ -7694,94 +7706,94 @@
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>733</v>
+        <v>323</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>734</v>
+        <v>324</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+    <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C124" s="8"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+    </row>
+    <row r="125" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>327</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="C125" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D125" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="E124" s="3" t="s">
+      <c r="E125" s="3" t="s">
         <v>738</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>329</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>739</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>329</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>331</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="C127" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="D127" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="E126" s="3" t="s">
+      <c r="E127" s="3" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A127" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>745</v>
-      </c>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8"/>
     </row>
     <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>745</v>
+      </c>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+    </row>
+    <row r="129" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A129" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B128" s="9" t="s">
+      <c r="B129" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="C128" s="8"/>
-      <c r="D128" s="7"/>
-      <c r="E128" s="7"/>
-    </row>
-    <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B129" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="7"/>
@@ -7789,10 +7801,10 @@
     </row>
     <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="7"/>
@@ -7800,10 +7812,10 @@
     </row>
     <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="7"/>
@@ -7811,21 +7823,21 @@
     </row>
     <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="7"/>
@@ -7833,21 +7845,21 @@
     </row>
     <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="7"/>
@@ -7855,10 +7867,10 @@
     </row>
     <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
-        <v>746</v>
+        <v>348</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>747</v>
+        <v>349</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="7"/>
@@ -7866,21 +7878,21 @@
     </row>
     <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
@@ -7888,77 +7900,77 @@
     </row>
     <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
     <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="A140" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="C140" s="8"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
+    </row>
+    <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>754</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>755</v>
       </c>
-      <c r="C140" s="3" t="s">
+      <c r="C141" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="D141" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="E140" s="3" t="s">
+      <c r="E141" s="3" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A141" s="7" t="s">
+    <row r="142" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A142" s="7" t="s">
         <v>759</v>
       </c>
-      <c r="B141" s="9" t="s">
+      <c r="B142" s="9" t="s">
         <v>760</v>
       </c>
-      <c r="C141" s="8"/>
-      <c r="D141" s="7"/>
-      <c r="E141" s="7"/>
-    </row>
-    <row r="142" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="C142" s="8"/>
+      <c r="D142" s="7"/>
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>761</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="C142" s="3" t="s">
+      <c r="C143" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="D142" s="3" t="s">
+      <c r="D143" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="E142" s="3" t="s">
+      <c r="E143" s="3" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A143" s="7" t="s">
-        <v>766</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
     </row>
     <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
@@ -7966,10 +7978,10 @@
     </row>
     <row r="145" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C145" s="8"/>
       <c r="D145" s="7"/>
@@ -7977,10 +7989,10 @@
     </row>
     <row r="146" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
-        <v>352</v>
+        <v>770</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>353</v>
+        <v>771</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
@@ -7988,212 +8000,212 @@
     </row>
     <row r="147" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C147" s="8"/>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>356</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>360</v>
-      </c>
+    <row r="148" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A148" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C148" s="8"/>
+      <c r="D148" s="7"/>
+      <c r="E148" s="7"/>
     </row>
     <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>356</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>361</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C149" s="3" t="s">
+      <c r="C150" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D150" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="E149" s="3" t="s">
+      <c r="E150" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A150" s="7" t="s">
+    <row r="151" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A151" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="B150" s="9" t="s">
+      <c r="B151" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-    </row>
-    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>368</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D151" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E151" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="C151" s="8"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
     </row>
     <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>370</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>371</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C154" s="3" t="s">
+      <c r="C155" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D155" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E154" s="3" t="s">
+      <c r="E155" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B155" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="C155" s="8"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
     </row>
     <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C156" s="8"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
     </row>
     <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="A157" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C157" s="8"/>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7"/>
+    </row>
+    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>772</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C157" s="3" t="s">
+      <c r="C158" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D158" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E157" s="3" t="s">
+      <c r="E158" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="7" t="s">
+    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A159" s="7" t="s">
         <v>773</v>
       </c>
-      <c r="B158" s="9" t="s">
+      <c r="B159" s="9" t="s">
         <v>774</v>
       </c>
-      <c r="C158" s="8"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+      <c r="C159" s="8"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>775</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C160" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D160" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E160" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="7" t="s">
-        <v>776</v>
-      </c>
-      <c r="B160" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C160" s="8"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
     </row>
     <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C161" s="8"/>
       <c r="D161" s="7"/>
@@ -8201,10 +8213,10 @@
     </row>
     <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C162" s="8"/>
       <c r="D162" s="7"/>
@@ -8212,21 +8224,21 @@
     </row>
     <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="7"/>
@@ -8234,77 +8246,77 @@
     </row>
     <row r="165" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+    <row r="166" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A166" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="C166" s="8"/>
+      <c r="D166" s="7"/>
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>376</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C166" s="3" t="s">
+      <c r="C167" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D166" s="3" t="s">
+      <c r="D167" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E166" s="3" t="s">
+      <c r="E167" s="3" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" s="7" t="s">
+    <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A168" s="7" t="s">
         <v>788</v>
       </c>
-      <c r="B167" s="9" t="s">
+      <c r="B168" s="9" t="s">
         <v>789</v>
       </c>
-      <c r="C167" s="8"/>
-      <c r="D167" s="7"/>
-      <c r="E167" s="7"/>
-    </row>
-    <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
+      <c r="C168" s="8"/>
+      <c r="D168" s="7"/>
+      <c r="E168" s="7"/>
+    </row>
+    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>790</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C168" s="3" t="s">
+      <c r="C169" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="D169" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E168" s="3" t="s">
+      <c r="E169" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A169" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B169" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="C169" s="8"/>
-      <c r="D169" s="7"/>
-      <c r="E169" s="7"/>
     </row>
     <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="7" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="7"/>
@@ -8312,10 +8324,10 @@
     </row>
     <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="7"/>
@@ -8323,10 +8335,10 @@
     </row>
     <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -8334,10 +8346,10 @@
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>395</v>
+        <v>798</v>
       </c>
       <c r="C173" s="8"/>
       <c r="D173" s="7"/>
@@ -8345,10 +8357,10 @@
     </row>
     <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>801</v>
+        <v>395</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
@@ -8356,10 +8368,10 @@
     </row>
     <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C175" s="8"/>
       <c r="D175" s="7"/>
@@ -8367,46 +8379,40 @@
     </row>
     <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
       <c r="E176" s="7"/>
     </row>
-    <row r="177" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
-        <v>381</v>
+        <v>804</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>382</v>
+        <v>805</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>383</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E178" s="3" t="s">
-        <v>380</v>
-      </c>
+    <row r="178" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A178" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C178" s="8"/>
+      <c r="D178" s="7"/>
+      <c r="E178" s="7"/>
     </row>
     <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>806</v>
+        <v>383</v>
       </c>
       <c r="B179" s="4" t="s">
         <v>377</v>
@@ -8422,44 +8428,50 @@
       </c>
     </row>
     <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A180" s="7" t="s">
-        <v>807</v>
-      </c>
-      <c r="B180" s="9" t="s">
-        <v>808</v>
-      </c>
-      <c r="C180" s="8"/>
-      <c r="D180" s="7"/>
-      <c r="E180" s="7"/>
+      <c r="A180" t="s">
+        <v>806</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
-        <v>384</v>
+        <v>809</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>387</v>
+        <v>811</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="7"/>
@@ -8467,65 +8479,65 @@
     </row>
     <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
@@ -8533,87 +8545,87 @@
     </row>
     <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
-        <v>812</v>
+        <v>400</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>813</v>
+        <v>401</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
     </row>
-    <row r="193" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>393</v>
+        <v>817</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>820</v>
+        <v>393</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A196" s="7" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>397</v>
+        <v>820</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
     </row>
-    <row r="197" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>823</v>
+        <v>397</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
@@ -8621,21 +8633,21 @@
     </row>
     <row r="198" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
     </row>
-    <row r="199" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
-        <v>402</v>
+        <v>824</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>403</v>
+        <v>825</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
@@ -8643,133 +8655,133 @@
     </row>
     <row r="200" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
     </row>
     <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
-        <v>406</v>
-      </c>
-      <c r="B201" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D201" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E201" s="3" t="s">
-        <v>410</v>
-      </c>
+      <c r="A201" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C201" s="8"/>
+      <c r="D201" s="7"/>
+      <c r="E201" s="7"/>
     </row>
     <row r="202" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>406</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
         <v>411</v>
       </c>
-      <c r="B202" s="4" t="s">
+      <c r="B203" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C202" s="3" t="s">
+      <c r="C203" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="D202" s="3" t="s">
+      <c r="D203" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E202" s="3" t="s">
+      <c r="E203" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A203" s="7" t="s">
+    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A204" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="B203" s="9" t="s">
+      <c r="B204" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="C203" s="8"/>
-      <c r="D203" s="7"/>
-      <c r="E203" s="7"/>
-    </row>
-    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
+      <c r="C204" s="8"/>
+      <c r="D204" s="7"/>
+      <c r="E204" s="7"/>
+    </row>
+    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
         <v>417</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="B205" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C204" s="3" t="s">
+      <c r="C205" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D204" s="3" t="s">
+      <c r="D205" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E204" s="3" t="s">
+      <c r="E205" s="3" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A205" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B205" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C205" s="8"/>
-      <c r="D205" s="7"/>
-      <c r="E205" s="7"/>
     </row>
     <row r="206" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="7"/>
       <c r="E206" s="7"/>
     </row>
-    <row r="207" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
+    <row r="207" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A207" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B207" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C207" s="8"/>
+      <c r="D207" s="7"/>
+      <c r="E207" s="7"/>
+    </row>
+    <row r="208" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
         <v>826</v>
       </c>
-      <c r="B207" s="4" t="s">
+      <c r="B208" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="C207" s="3" t="s">
+      <c r="C208" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D207" s="3" t="s">
+      <c r="D208" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="E207" s="3" t="s">
+      <c r="E208" s="3" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A208" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="B208" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="C208" s="8"/>
-      <c r="D208" s="7"/>
-      <c r="E208" s="7"/>
     </row>
     <row r="209" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C209" s="8"/>
       <c r="D209" s="7"/>
@@ -8777,21 +8789,21 @@
     </row>
     <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C210" s="8"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
     </row>
-    <row r="211" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>403</v>
+        <v>430</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="7"/>
@@ -8799,21 +8811,21 @@
     </row>
     <row r="212" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C212" s="8"/>
       <c r="D212" s="7"/>
       <c r="E212" s="7"/>
     </row>
-    <row r="213" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="7" t="s">
-        <v>831</v>
+        <v>432</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="7"/>
@@ -8821,10 +8833,10 @@
     </row>
     <row r="214" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A214" s="7" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>833</v>
+        <v>423</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="7"/>
@@ -8832,10 +8844,10 @@
     </row>
     <row r="215" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" s="7" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C215" s="8"/>
       <c r="D215" s="7"/>
@@ -8843,33 +8855,44 @@
     </row>
     <row r="216" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C216" s="8"/>
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
     </row>
-    <row r="217" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
+    <row r="217" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A217" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B217" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C217" s="8"/>
+      <c r="D217" s="7"/>
+      <c r="E217" s="7"/>
+    </row>
+    <row r="218" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
         <v>878</v>
       </c>
-      <c r="B217" s="15" t="s">
+      <c r="B218" s="15" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
+    <row r="219" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
         <v>879</v>
       </c>
-      <c r="B218" s="4" t="s">
+      <c r="B219" s="4" t="s">
         <v>895</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E216" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E217" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9011,29 +9034,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
-      <UserInfo>
-        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
-        <AccountId>180</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
-        <AccountId>212</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -9287,6 +9287,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07d4ffe0-35c4-4630-b07d-57ff54db67ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="3a79588a-61f1-49eb-bf82-c7b2c97b1d12">
+      <UserInfo>
+        <DisplayName>Bravo, Ms. Pamela (WDC)</DisplayName>
+        <AccountId>180</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Silva, Ms. Octavia  (WDC)</DisplayName>
+        <AccountId>212</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
   <ds:schemaRefs>
@@ -9296,18 +9319,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
-    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
-    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9325,4 +9336,16 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+    <ds:schemaRef ds:uri="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
+    <ds:schemaRef ds:uri="3a79588a-61f1-49eb-bf82-c7b2c97b1d12"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(surveillance): added tab item
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D65D38-4044-134E-BA84-C745AB54C4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E72B7D-1103-C444-9A47-CFA60BFD4963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="-38400" yWindow="-2640" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$217</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$218</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="904">
   <si>
     <t>LABEL</t>
   </si>
@@ -2763,6 +2763,9 @@
   </si>
   <si>
     <t>&gt; 100</t>
+  </si>
+  <si>
+    <t>menuitem_surveillance</t>
   </si>
 </sst>
 </file>
@@ -6020,10 +6023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E219"/>
+  <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6643,148 +6646,154 @@
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>863</v>
+        <v>903</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>864</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>629</v>
+        <v>861</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>630</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>633</v>
-      </c>
+        <v>862</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>629</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>634</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>636</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="C47" s="8"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>637</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+    <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
         <v>638</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B49" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>640</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>309</v>
-      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>640</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>641</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+    <row r="52" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B52" s="9" t="s">
         <v>643</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
-        <v>644</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>645</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="7"/>
@@ -6792,21 +6801,21 @@
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="7"/>
@@ -6814,145 +6823,145 @@
     </row>
     <row r="55" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>652</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>652</v>
-      </c>
+    <row r="56" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>652</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>653</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>656</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-    </row>
-    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>301</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>893</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>47</v>
+        <v>893</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>892</v>
+        <v>47</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>303</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>304</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="7" t="s">
-        <v>658</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>659</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>98</v>
+        <v>658</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>99</v>
+        <v>659</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="7"/>
@@ -6960,10 +6969,10 @@
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="7"/>
@@ -6971,151 +6980,149 @@
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>660</v>
+        <v>61</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>272</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>276</v>
-      </c>
+      <c r="A67" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>272</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>277</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
         <v>901</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>902</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>902</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>902</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>282</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>292</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>296</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="7" t="s">
-        <v>665</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>666</v>
-      </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="7"/>
@@ -7123,133 +7130,133 @@
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="A77" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+    </row>
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>305</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
         <v>671</v>
       </c>
-      <c r="C78" s="8"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-    </row>
-    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="C79" s="8"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>311</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D80" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E80" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
+    <row r="81" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B81" s="9" t="s">
         <v>673</v>
-      </c>
-      <c r="C80" s="8"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-    </row>
-    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
-        <v>674</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>675</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>676</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>582</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>585</v>
-      </c>
+      <c r="A82" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>676</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>677</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>680</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
-        <v>682</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>683</v>
-      </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="7"/>
@@ -7257,10 +7264,10 @@
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="7"/>
@@ -7268,10 +7275,10 @@
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="7"/>
@@ -7279,10 +7286,10 @@
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="7"/>
@@ -7290,10 +7297,10 @@
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="7"/>
@@ -7301,10 +7308,10 @@
     </row>
     <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="7"/>
@@ -7312,10 +7319,10 @@
     </row>
     <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C91" s="8"/>
       <c r="D91" s="7"/>
@@ -7323,10 +7330,10 @@
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="7"/>
@@ -7334,76 +7341,76 @@
     </row>
     <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>880</v>
+        <v>702</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>896</v>
+        <v>703</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+    </row>
+    <row r="97" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
         <v>886</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B97" s="9" t="s">
         <v>887</v>
       </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-    </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
-        <v>881</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>897</v>
-      </c>
       <c r="C97" s="8"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
     </row>
     <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>889</v>
+        <v>897</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>882</v>
+        <v>888</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="7"/>
@@ -7411,127 +7418,127 @@
     </row>
     <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>885</v>
+        <v>900</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>704</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="A103" s="7" t="s">
+        <v>884</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>885</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
     </row>
     <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>704</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>705</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E105" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
-        <v>706</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>707</v>
-      </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
     </row>
     <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="A107" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
+    </row>
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>710</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D108" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
+    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B109" s="9" t="s">
         <v>716</v>
-      </c>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-    </row>
-    <row r="109" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
-        <v>717</v>
-      </c>
-      <c r="B109" s="9" t="s">
-        <v>718</v>
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
@@ -7539,10 +7546,10 @@
     </row>
     <row r="110" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
@@ -7550,122 +7557,122 @@
     </row>
     <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
+    </row>
+    <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="B112" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C111" s="8"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
-    </row>
-    <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="C112" s="8"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+    </row>
+    <row r="113" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>318</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D113" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E112" s="3" t="s">
+      <c r="E113" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
+    <row r="114" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A114" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B113" s="9" t="s">
+      <c r="B114" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C113" s="8"/>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-    </row>
-    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="C114" s="8"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+    </row>
+    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>721</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C115" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D115" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E114" s="4" t="s">
+      <c r="E115" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
+    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="B116" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C115" s="8"/>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
-    </row>
-    <row r="116" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="C116" s="8"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+    </row>
+    <row r="117" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>722</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D117" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="E117" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="118" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>723</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D118" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E118" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
+    <row r="119" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A119" s="7" t="s">
         <v>728</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B119" s="9" t="s">
         <v>729</v>
-      </c>
-      <c r="C118" s="8"/>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
-    </row>
-    <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>351</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="7"/>
@@ -7673,10 +7680,10 @@
     </row>
     <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>730</v>
+        <v>350</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>731</v>
+        <v>351</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="7"/>
@@ -7684,10 +7691,10 @@
     </row>
     <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>595</v>
+        <v>731</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="7"/>
@@ -7695,10 +7702,10 @@
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>321</v>
+        <v>732</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>322</v>
+        <v>595</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
@@ -7706,10 +7713,10 @@
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
@@ -7717,94 +7724,94 @@
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>733</v>
+        <v>323</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>734</v>
+        <v>324</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C125" s="8"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+    </row>
+    <row r="126" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>327</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C126" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="D125" s="3" t="s">
+      <c r="D126" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="E125" s="3" t="s">
+      <c r="E126" s="3" t="s">
         <v>738</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>329</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>739</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>329</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>331</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C128" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D128" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="E127" s="3" t="s">
+      <c r="E128" s="3" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A128" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>745</v>
-      </c>
-      <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
-      <c r="E128" s="8"/>
     </row>
     <row r="129" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>745</v>
+      </c>
+      <c r="C129" s="8"/>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8"/>
+    </row>
+    <row r="130" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A130" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B129" s="9" t="s">
+      <c r="B130" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="C129" s="8"/>
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
-    </row>
-    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="7"/>
@@ -7812,10 +7819,10 @@
     </row>
     <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="7"/>
@@ -7823,10 +7830,10 @@
     </row>
     <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="7"/>
@@ -7834,21 +7841,21 @@
     </row>
     <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="7"/>
@@ -7856,21 +7863,21 @@
     </row>
     <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="7"/>
@@ -7878,10 +7885,10 @@
     </row>
     <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>746</v>
+        <v>348</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>747</v>
+        <v>349</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
@@ -7889,21 +7896,21 @@
     </row>
     <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
@@ -7911,77 +7918,77 @@
     </row>
     <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
     </row>
     <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="A141" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="C141" s="8"/>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>754</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>755</v>
       </c>
-      <c r="C141" s="3" t="s">
+      <c r="C142" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="D141" s="3" t="s">
+      <c r="D142" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="E141" s="3" t="s">
+      <c r="E142" s="3" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A142" s="7" t="s">
+    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A143" s="7" t="s">
         <v>759</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B143" s="9" t="s">
         <v>760</v>
       </c>
-      <c r="C142" s="8"/>
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
-    </row>
-    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="C143" s="8"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+    </row>
+    <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>761</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="C143" s="3" t="s">
+      <c r="C144" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D144" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="E143" s="3" t="s">
+      <c r="E144" s="3" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A144" s="7" t="s">
-        <v>766</v>
-      </c>
-      <c r="B144" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="C144" s="8"/>
-      <c r="D144" s="7"/>
-      <c r="E144" s="7"/>
     </row>
     <row r="145" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C145" s="8"/>
       <c r="D145" s="7"/>
@@ -7989,10 +7996,10 @@
     </row>
     <row r="146" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
@@ -8000,10 +8007,10 @@
     </row>
     <row r="147" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
-        <v>352</v>
+        <v>770</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>353</v>
+        <v>771</v>
       </c>
       <c r="C147" s="8"/>
       <c r="D147" s="7"/>
@@ -8011,212 +8018,212 @@
     </row>
     <row r="148" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>356</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>360</v>
-      </c>
+    <row r="149" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A149" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C149" s="8"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
     </row>
     <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
+        <v>356</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>361</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="C151" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D151" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="E150" s="3" t="s">
+      <c r="E151" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A151" s="7" t="s">
+    <row r="152" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A152" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="B151" s="9" t="s">
+      <c r="B152" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C151" s="8"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="7"/>
-    </row>
-    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>368</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D152" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E152" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="C152" s="8"/>
+      <c r="D152" s="7"/>
+      <c r="E152" s="7"/>
     </row>
     <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>370</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>371</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C155" s="3" t="s">
+      <c r="C156" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D156" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E155" s="3" t="s">
+      <c r="E156" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B156" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="C156" s="8"/>
-      <c r="D156" s="7"/>
-      <c r="E156" s="7"/>
     </row>
     <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
     <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+      <c r="A158" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C158" s="8"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>772</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C159" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D159" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E159" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" s="7" t="s">
+    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" s="7" t="s">
         <v>773</v>
       </c>
-      <c r="B159" s="9" t="s">
+      <c r="B160" s="9" t="s">
         <v>774</v>
       </c>
-      <c r="C159" s="8"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-    </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="C160" s="8"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>775</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C161" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D161" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E160" s="3" t="s">
+      <c r="E161" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="7" t="s">
-        <v>776</v>
-      </c>
-      <c r="B161" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C161" s="8"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="7"/>
     </row>
     <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C162" s="8"/>
       <c r="D162" s="7"/>
@@ -8224,10 +8231,10 @@
     </row>
     <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="7"/>
@@ -8235,21 +8242,21 @@
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
@@ -8257,77 +8264,77 @@
     </row>
     <row r="166" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+    <row r="167" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A167" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="C167" s="8"/>
+      <c r="D167" s="7"/>
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>376</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B168" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C168" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D167" s="3" t="s">
+      <c r="D168" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E167" s="3" t="s">
+      <c r="E168" s="3" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" s="7" t="s">
+    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A169" s="7" t="s">
         <v>788</v>
       </c>
-      <c r="B168" s="9" t="s">
+      <c r="B169" s="9" t="s">
         <v>789</v>
       </c>
-      <c r="C168" s="8"/>
-      <c r="D168" s="7"/>
-      <c r="E168" s="7"/>
-    </row>
-    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+      <c r="C169" s="8"/>
+      <c r="D169" s="7"/>
+      <c r="E169" s="7"/>
+    </row>
+    <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>790</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C169" s="3" t="s">
+      <c r="C170" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D169" s="3" t="s">
+      <c r="D170" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E169" s="3" t="s">
+      <c r="E170" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A170" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B170" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="C170" s="8"/>
-      <c r="D170" s="7"/>
-      <c r="E170" s="7"/>
     </row>
     <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="7"/>
@@ -8335,10 +8342,10 @@
     </row>
     <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -8346,10 +8353,10 @@
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C173" s="8"/>
       <c r="D173" s="7"/>
@@ -8357,10 +8364,10 @@
     </row>
     <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>395</v>
+        <v>798</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
@@ -8368,10 +8375,10 @@
     </row>
     <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>801</v>
+        <v>395</v>
       </c>
       <c r="C175" s="8"/>
       <c r="D175" s="7"/>
@@ -8379,10 +8386,10 @@
     </row>
     <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
@@ -8390,46 +8397,40 @@
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
-        <v>381</v>
+        <v>804</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>382</v>
+        <v>805</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>383</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E179" s="3" t="s">
-        <v>380</v>
-      </c>
+    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A179" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B179" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C179" s="8"/>
+      <c r="D179" s="7"/>
+      <c r="E179" s="7"/>
     </row>
     <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>806</v>
+        <v>383</v>
       </c>
       <c r="B180" s="4" t="s">
         <v>377</v>
@@ -8445,44 +8446,50 @@
       </c>
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A181" s="7" t="s">
-        <v>807</v>
-      </c>
-      <c r="B181" s="9" t="s">
-        <v>808</v>
-      </c>
-      <c r="C181" s="8"/>
-      <c r="D181" s="7"/>
-      <c r="E181" s="7"/>
+      <c r="A181" t="s">
+        <v>806</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
-        <v>384</v>
+        <v>809</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="7"/>
       <c r="E183" s="7"/>
     </row>
-    <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>387</v>
+        <v>811</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
@@ -8490,65 +8497,65 @@
     </row>
     <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
@@ -8556,87 +8563,87 @@
     </row>
     <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
-        <v>812</v>
+        <v>400</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>813</v>
+        <v>401</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
     </row>
-    <row r="193" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>393</v>
+        <v>817</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A196" s="7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>820</v>
+        <v>393</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
     </row>
-    <row r="197" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>397</v>
+        <v>820</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
     </row>
-    <row r="198" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>823</v>
+        <v>397</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
@@ -8644,21 +8651,21 @@
     </row>
     <row r="199" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
-        <v>402</v>
+        <v>824</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>403</v>
+        <v>825</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
@@ -8666,133 +8673,133 @@
     </row>
     <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C201" s="8"/>
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
     </row>
     <row r="202" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
-        <v>406</v>
-      </c>
-      <c r="B202" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D202" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E202" s="3" t="s">
-        <v>410</v>
-      </c>
+      <c r="A202" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="B202" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C202" s="8"/>
+      <c r="D202" s="7"/>
+      <c r="E202" s="7"/>
     </row>
     <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
+        <v>406</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
         <v>411</v>
       </c>
-      <c r="B203" s="4" t="s">
+      <c r="B204" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C203" s="3" t="s">
+      <c r="C204" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="D203" s="3" t="s">
+      <c r="D204" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E203" s="3" t="s">
+      <c r="E204" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A204" s="7" t="s">
+    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A205" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="B204" s="9" t="s">
+      <c r="B205" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="C204" s="8"/>
-      <c r="D204" s="7"/>
-      <c r="E204" s="7"/>
-    </row>
-    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A205" t="s">
+      <c r="C205" s="8"/>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
+    </row>
+    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
         <v>417</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B206" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C205" s="3" t="s">
+      <c r="C206" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D205" s="3" t="s">
+      <c r="D206" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E205" s="3" t="s">
+      <c r="E206" s="3" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A206" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B206" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C206" s="8"/>
-      <c r="D206" s="7"/>
-      <c r="E206" s="7"/>
     </row>
     <row r="207" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="7"/>
       <c r="E207" s="7"/>
     </row>
-    <row r="208" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
+    <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A208" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B208" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C208" s="8"/>
+      <c r="D208" s="7"/>
+      <c r="E208" s="7"/>
+    </row>
+    <row r="209" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
         <v>826</v>
       </c>
-      <c r="B208" s="4" t="s">
+      <c r="B209" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="C208" s="3" t="s">
+      <c r="C209" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D208" s="3" t="s">
+      <c r="D209" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="E208" s="3" t="s">
+      <c r="E209" s="3" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A209" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="B209" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="C209" s="8"/>
-      <c r="D209" s="7"/>
-      <c r="E209" s="7"/>
     </row>
     <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C210" s="8"/>
       <c r="D210" s="7"/>
@@ -8800,21 +8807,21 @@
     </row>
     <row r="211" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
     </row>
-    <row r="212" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A212" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>403</v>
+        <v>430</v>
       </c>
       <c r="C212" s="8"/>
       <c r="D212" s="7"/>
@@ -8822,21 +8829,21 @@
     </row>
     <row r="213" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="7"/>
       <c r="E213" s="7"/>
     </row>
-    <row r="214" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A214" s="7" t="s">
-        <v>831</v>
+        <v>432</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="7"/>
@@ -8844,10 +8851,10 @@
     </row>
     <row r="215" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" s="7" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>833</v>
+        <v>423</v>
       </c>
       <c r="C215" s="8"/>
       <c r="D215" s="7"/>
@@ -8855,10 +8862,10 @@
     </row>
     <row r="216" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" s="7" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C216" s="8"/>
       <c r="D216" s="7"/>
@@ -8866,33 +8873,44 @@
     </row>
     <row r="217" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A217" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C217" s="8"/>
       <c r="D217" s="7"/>
       <c r="E217" s="7"/>
     </row>
-    <row r="218" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
+    <row r="218" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A218" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B218" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C218" s="8"/>
+      <c r="D218" s="7"/>
+      <c r="E218" s="7"/>
+    </row>
+    <row r="219" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
         <v>878</v>
       </c>
-      <c r="B218" s="15" t="s">
+      <c r="B219" s="15" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
+    <row r="220" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
         <v>879</v>
       </c>
-      <c r="B219" s="4" t="s">
+      <c r="B220" s="4" t="s">
         <v>895</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E217" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E218" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(surveillance): reporting units map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1CAC7-CF24-A24D-B22F-17D8DE01E423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA6BD05-4D1E-C947-B36C-7B5A9572E42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2640" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$218</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$221</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="911">
   <si>
     <t>LABEL</t>
   </si>
@@ -2769,6 +2769,24 @@
   </si>
   <si>
     <t>surveillance_score</t>
+  </si>
+  <si>
+    <t>Unidades Notificantes</t>
+  </si>
+  <si>
+    <t>surveillance_reporting_units</t>
+  </si>
+  <si>
+    <t>Proporción de unidades notificantes</t>
+  </si>
+  <si>
+    <t>surveillance_prop_reporting_units</t>
+  </si>
+  <si>
+    <t>surveillance_title_map_reporting_units</t>
+  </si>
+  <si>
+    <t>Proporción de unidades notificadoras que enviaron información en todas las semanas</t>
   </si>
 </sst>
 </file>
@@ -2871,7 +2889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2914,6 +2932,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3230,7 +3251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C7D9D-C4E2-B94C-B003-B8DCE10597B7}">
   <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6026,15 +6047,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E220"/>
+  <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="28.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
@@ -6042,7 +6063,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -6059,7 +6080,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="17" t="s">
         <v>572</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -6076,7 +6097,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="17" t="s">
         <v>577</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -6084,7 +6105,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="18" t="s">
         <v>578</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -6095,7 +6116,7 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="17" t="s">
         <v>580</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -6112,7 +6133,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="17" t="s">
         <v>581</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -6129,7 +6150,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -6146,7 +6167,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -6163,7 +6184,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="18" t="s">
         <v>586</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -6174,7 +6195,7 @@
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="18" t="s">
         <v>588</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -6185,7 +6206,7 @@
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="18" t="s">
         <v>590</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -6196,7 +6217,7 @@
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="18" t="s">
         <v>592</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -6207,7 +6228,7 @@
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="18" t="s">
         <v>594</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -6218,7 +6239,7 @@
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="18" t="s">
         <v>596</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -6229,7 +6250,7 @@
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="17" t="s">
         <v>598</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -6246,7 +6267,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="17" t="s">
         <v>602</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -6263,7 +6284,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="18" t="s">
         <v>606</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -6274,7 +6295,7 @@
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="18" t="s">
         <v>608</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -6285,7 +6306,7 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="17" t="s">
         <v>610</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -6302,7 +6323,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="17" t="s">
         <v>873</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -6319,7 +6340,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="17" t="s">
         <v>901</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -6335,8 +6356,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
         <v>903</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -6346,7 +6367,7 @@
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="17" t="s">
         <v>874</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -6356,7 +6377,7 @@
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="17" t="s">
         <v>615</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -6373,7 +6394,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="17" t="s">
         <v>616</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -6390,7 +6411,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="17" t="s">
         <v>617</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -6407,7 +6428,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="17" t="s">
         <v>618</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -6424,7 +6445,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="17" t="s">
         <v>619</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -6441,7 +6462,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="17" t="s">
         <v>623</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -6458,7 +6479,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="17" t="s">
         <v>871</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -6468,7 +6489,7 @@
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="17" t="s">
         <v>869</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -6478,7 +6499,7 @@
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="17" t="s">
         <v>904</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -6495,7 +6516,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="17" t="s">
         <v>868</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -6512,7 +6533,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="17" t="s">
         <v>867</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -6529,7 +6550,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" s="17" t="s">
         <v>624</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -6546,7 +6567,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="17" t="s">
         <v>625</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -6563,7 +6584,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="17" t="s">
         <v>626</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -6580,7 +6601,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" s="17" t="s">
         <v>627</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -6597,7 +6618,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="17" t="s">
         <v>628</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -6614,7 +6635,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="17" t="s">
         <v>865</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -6631,7 +6652,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="17" t="s">
         <v>866</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -6648,7 +6669,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="17" t="s">
         <v>902</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -6665,7 +6686,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="17" t="s">
         <v>863</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -6675,7 +6696,7 @@
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="17" t="s">
         <v>861</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -6685,7 +6706,7 @@
       <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="A45" s="17" t="s">
         <v>629</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -6702,7 +6723,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="17" t="s">
         <v>634</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -6719,7 +6740,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="18" t="s">
         <v>635</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -6730,7 +6751,7 @@
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="17" t="s">
         <v>637</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -6747,7 +6768,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="18" t="s">
         <v>638</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -6758,7 +6779,7 @@
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="A50" s="17" t="s">
         <v>640</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -6775,7 +6796,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="A51" s="17" t="s">
         <v>641</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -6792,7 +6813,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="18" t="s">
         <v>642</v>
       </c>
       <c r="B52" s="9" t="s">
@@ -6803,7 +6824,7 @@
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="18" t="s">
         <v>644</v>
       </c>
       <c r="B53" s="9" t="s">
@@ -6814,7 +6835,7 @@
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="18" t="s">
         <v>646</v>
       </c>
       <c r="B54" s="9" t="s">
@@ -6825,7 +6846,7 @@
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="18" t="s">
         <v>648</v>
       </c>
       <c r="B55" s="9" t="s">
@@ -6836,7 +6857,7 @@
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="18" t="s">
         <v>650</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -6847,7 +6868,7 @@
       <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="17" t="s">
         <v>652</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -6864,7 +6885,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="17" t="s">
         <v>653</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -6881,7 +6902,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -6892,7 +6913,7 @@
       <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" s="17" t="s">
         <v>301</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -6909,7 +6930,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="17" t="s">
         <v>302</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -6926,7 +6947,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="17" t="s">
         <v>303</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -6943,7 +6964,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="17" t="s">
         <v>304</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -6960,7 +6981,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="18" t="s">
         <v>658</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -6971,7 +6992,7 @@
       <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="18" t="s">
         <v>98</v>
       </c>
       <c r="B65" s="9" t="s">
@@ -6982,7 +7003,7 @@
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="18" t="s">
         <v>61</v>
       </c>
       <c r="B66" s="9" t="s">
@@ -6993,7 +7014,7 @@
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="18" t="s">
         <v>660</v>
       </c>
       <c r="B67" s="9" t="s">
@@ -7004,7 +7025,7 @@
       <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="A68" s="17" t="s">
         <v>272</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -7021,7 +7042,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="A69" s="17" t="s">
         <v>277</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -7038,7 +7059,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="18" t="s">
         <v>899</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -7053,7 +7074,7 @@
       <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="A71" s="17" t="s">
         <v>282</v>
       </c>
       <c r="B71" s="4" t="s">
@@ -7070,7 +7091,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="A72" s="17" t="s">
         <v>287</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -7087,7 +7108,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="A73" s="17" t="s">
         <v>292</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -7104,7 +7125,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="A74" s="17" t="s">
         <v>296</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -7121,7 +7142,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="18" t="s">
         <v>665</v>
       </c>
       <c r="B75" s="9" t="s">
@@ -7132,7 +7153,7 @@
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="18" t="s">
         <v>667</v>
       </c>
       <c r="B76" s="9" t="s">
@@ -7143,7 +7164,7 @@
       <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="18" t="s">
         <v>669</v>
       </c>
       <c r="B77" s="9" t="s">
@@ -7154,7 +7175,7 @@
       <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="A78" s="17" t="s">
         <v>305</v>
       </c>
       <c r="B78" s="4" t="s">
@@ -7171,7 +7192,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="18" t="s">
         <v>310</v>
       </c>
       <c r="B79" s="9" t="s">
@@ -7182,7 +7203,7 @@
       <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="A80" s="17" t="s">
         <v>311</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -7199,7 +7220,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="18" t="s">
         <v>672</v>
       </c>
       <c r="B81" s="9" t="s">
@@ -7210,7 +7231,7 @@
       <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="18" t="s">
         <v>674</v>
       </c>
       <c r="B82" s="9" t="s">
@@ -7221,7 +7242,7 @@
       <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="A83" s="17" t="s">
         <v>676</v>
       </c>
       <c r="B83" s="4" t="s">
@@ -7238,7 +7259,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="A84" s="17" t="s">
         <v>677</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -7255,7 +7276,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="18" t="s">
         <v>682</v>
       </c>
       <c r="B85" s="9" t="s">
@@ -7266,7 +7287,7 @@
       <c r="E85" s="7"/>
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="18" t="s">
         <v>684</v>
       </c>
       <c r="B86" s="9" t="s">
@@ -7277,7 +7298,7 @@
       <c r="E86" s="7"/>
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="18" t="s">
         <v>686</v>
       </c>
       <c r="B87" s="9" t="s">
@@ -7288,7 +7309,7 @@
       <c r="E87" s="7"/>
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B88" s="9" t="s">
@@ -7299,7 +7320,7 @@
       <c r="E88" s="7"/>
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="18" t="s">
         <v>690</v>
       </c>
       <c r="B89" s="9" t="s">
@@ -7310,7 +7331,7 @@
       <c r="E89" s="7"/>
     </row>
     <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="18" t="s">
         <v>692</v>
       </c>
       <c r="B90" s="9" t="s">
@@ -7321,7 +7342,7 @@
       <c r="E90" s="7"/>
     </row>
     <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="18" t="s">
         <v>694</v>
       </c>
       <c r="B91" s="9" t="s">
@@ -7332,7 +7353,7 @@
       <c r="E91" s="7"/>
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="18" t="s">
         <v>696</v>
       </c>
       <c r="B92" s="9" t="s">
@@ -7343,7 +7364,7 @@
       <c r="E92" s="7"/>
     </row>
     <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="18" t="s">
         <v>698</v>
       </c>
       <c r="B93" s="9" t="s">
@@ -7354,7 +7375,7 @@
       <c r="E93" s="7"/>
     </row>
     <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="18" t="s">
         <v>700</v>
       </c>
       <c r="B94" s="9" t="s">
@@ -7365,7 +7386,7 @@
       <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="18" t="s">
         <v>702</v>
       </c>
       <c r="B95" s="9" t="s">
@@ -7376,7 +7397,7 @@
       <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="18" t="s">
         <v>878</v>
       </c>
       <c r="B96" s="9" t="s">
@@ -7387,7 +7408,7 @@
       <c r="E96" s="7"/>
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="18" t="s">
         <v>884</v>
       </c>
       <c r="B97" s="9" t="s">
@@ -7398,7 +7419,7 @@
       <c r="E97" s="8"/>
     </row>
     <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="18" t="s">
         <v>879</v>
       </c>
       <c r="B98" s="9" t="s">
@@ -7409,7 +7430,7 @@
       <c r="E98" s="7"/>
     </row>
     <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
+      <c r="A99" s="18" t="s">
         <v>886</v>
       </c>
       <c r="B99" s="9" t="s">
@@ -7420,7 +7441,7 @@
       <c r="E99" s="7"/>
     </row>
     <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A100" s="7" t="s">
+      <c r="A100" s="18" t="s">
         <v>880</v>
       </c>
       <c r="B100" s="9" t="s">
@@ -7431,7 +7452,7 @@
       <c r="E100" s="7"/>
     </row>
     <row r="101" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="18" t="s">
         <v>888</v>
       </c>
       <c r="B101" s="9" t="s">
@@ -7442,7 +7463,7 @@
       <c r="E101" s="7"/>
     </row>
     <row r="102" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A102" s="7" t="s">
+      <c r="A102" s="18" t="s">
         <v>881</v>
       </c>
       <c r="B102" s="9" t="s">
@@ -7453,7 +7474,7 @@
       <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
+      <c r="A103" s="18" t="s">
         <v>882</v>
       </c>
       <c r="B103" s="9" t="s">
@@ -7464,1456 +7485,1489 @@
       <c r="E103" s="7"/>
     </row>
     <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="A104" s="18" t="s">
+        <v>906</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="17" t="s">
         <v>704</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E105" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="17" t="s">
         <v>705</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="D106" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="E106" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
+    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="18" t="s">
         <v>706</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B107" s="9" t="s">
         <v>707</v>
-      </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-    </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
-        <v>708</v>
-      </c>
-      <c r="B107" s="9" t="s">
-        <v>709</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
       <c r="E107" s="8"/>
     </row>
     <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="A108" s="18" t="s">
+        <v>708</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+    </row>
+    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="17" t="s">
         <v>710</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D109" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="E108" s="3" t="s">
+      <c r="E109" s="3" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
+    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="18" t="s">
         <v>715</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B110" s="9" t="s">
         <v>716</v>
-      </c>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
-    </row>
-    <row r="110" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
-        <v>717</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>718</v>
       </c>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
       <c r="E110" s="8"/>
     </row>
     <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
-        <v>719</v>
+      <c r="A111" s="18" t="s">
+        <v>717</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
       <c r="E111" s="8"/>
     </row>
     <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
+      <c r="A112" s="18" t="s">
+        <v>719</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+    </row>
+    <row r="113" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B113" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C112" s="8"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="C113" s="8"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+    </row>
+    <row r="114" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A114" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D114" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E114" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
+    <row r="115" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A115" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="B114" s="9" t="s">
+      <c r="B115" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C114" s="8"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-    </row>
-    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="C115" s="8"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+    </row>
+    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="17" t="s">
         <v>721</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="C116" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D115" s="4" t="s">
+      <c r="D116" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E115" s="4" t="s">
+      <c r="E116" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
+    <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B117" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C116" s="8"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
-    </row>
-    <row r="117" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="C117" s="8"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A118" s="17" t="s">
         <v>722</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D118" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E118" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="119" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A119" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D119" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="E119" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
+    <row r="120" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A120" s="18" t="s">
         <v>728</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B120" s="9" t="s">
         <v>729</v>
-      </c>
-      <c r="C119" s="8"/>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-    </row>
-    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>351</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="7"/>
       <c r="E120" s="7"/>
     </row>
     <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
-        <v>730</v>
+      <c r="A121" s="18" t="s">
+        <v>350</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>731</v>
+        <v>351</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
-        <v>732</v>
+      <c r="A122" s="18" t="s">
+        <v>730</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>595</v>
+        <v>731</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="7" t="s">
-        <v>321</v>
+      <c r="A123" s="18" t="s">
+        <v>732</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>322</v>
+        <v>595</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
       <c r="E123" s="7"/>
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="7" t="s">
-        <v>323</v>
+      <c r="A124" s="18" t="s">
+        <v>321</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
     </row>
     <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="7" t="s">
-        <v>733</v>
+      <c r="A125" s="18" t="s">
+        <v>323</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>734</v>
+        <v>324</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="18" t="s">
+        <v>733</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C126" s="8"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+    </row>
+    <row r="127" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A127" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="C127" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="D127" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="E126" s="3" t="s">
+      <c r="E127" s="3" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+    <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A128" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C128" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D128" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="E127" s="3" t="s">
+      <c r="E128" s="3" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+    <row r="129" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A129" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="C129" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D129" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="E128" s="3" t="s">
+      <c r="E129" s="3" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A129" s="7" t="s">
+    <row r="130" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A130" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="B129" s="9" t="s">
+      <c r="B130" s="9" t="s">
         <v>745</v>
       </c>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
-    </row>
-    <row r="130" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A130" s="7" t="s">
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+    </row>
+    <row r="131" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A131" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="B130" s="9" t="s">
+      <c r="B131" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="C130" s="8"/>
-      <c r="D130" s="7"/>
-      <c r="E130" s="7"/>
-    </row>
-    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
     </row>
     <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="7" t="s">
-        <v>339</v>
+      <c r="A132" s="18" t="s">
+        <v>337</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
     </row>
     <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" s="7" t="s">
-        <v>340</v>
+      <c r="A133" s="18" t="s">
+        <v>339</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A134" s="7" t="s">
-        <v>342</v>
+    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A134" s="18" t="s">
+        <v>908</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>343</v>
+        <v>907</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
-        <v>344</v>
+    <row r="135" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A135" s="18" t="s">
+        <v>909</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>345</v>
+        <v>910</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A136" s="7" t="s">
-        <v>346</v>
+    <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A136" s="18" t="s">
+        <v>340</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
     </row>
     <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="7" t="s">
-        <v>348</v>
+      <c r="A137" s="18" t="s">
+        <v>342</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="7" t="s">
-        <v>746</v>
+    <row r="138" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A138" s="18" t="s">
+        <v>344</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>747</v>
+        <v>345</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="7" t="s">
-        <v>748</v>
+    <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A139" s="18" t="s">
+        <v>346</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>749</v>
+        <v>347</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A140" s="7" t="s">
-        <v>750</v>
+    <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A140" s="18" t="s">
+        <v>348</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>751</v>
+        <v>349</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A141" s="7" t="s">
-        <v>752</v>
+    <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A141" s="18" t="s">
+        <v>746</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="7"/>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>754</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>758</v>
-      </c>
+    <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A142" s="18" t="s">
+        <v>748</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="C142" s="8"/>
+      <c r="D142" s="7"/>
+      <c r="E142" s="7"/>
     </row>
     <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A143" s="7" t="s">
-        <v>759</v>
+      <c r="A143" s="18" t="s">
+        <v>750</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>760</v>
+        <v>751</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
     </row>
     <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>761</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>762</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>765</v>
-      </c>
+      <c r="A144" s="18" t="s">
+        <v>752</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="C144" s="8"/>
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
     </row>
     <row r="145" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A145" s="7" t="s">
-        <v>766</v>
-      </c>
-      <c r="B145" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="C145" s="8"/>
-      <c r="D145" s="7"/>
-      <c r="E145" s="7"/>
+      <c r="A145" s="17" t="s">
+        <v>754</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="146" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A146" s="7" t="s">
-        <v>768</v>
+      <c r="A146" s="18" t="s">
+        <v>759</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
     </row>
     <row r="147" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A147" s="7" t="s">
-        <v>770</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>771</v>
-      </c>
-      <c r="C147" s="8"/>
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
+      <c r="A147" s="17" t="s">
+        <v>761</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="148" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A148" s="7" t="s">
-        <v>352</v>
+      <c r="A148" s="18" t="s">
+        <v>766</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>353</v>
+        <v>767</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
     </row>
     <row r="149" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A149" s="7" t="s">
-        <v>354</v>
+      <c r="A149" s="18" t="s">
+        <v>768</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>355</v>
+        <v>769</v>
       </c>
       <c r="C149" s="8"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>356</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D150" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E150" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>361</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D151" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E151" s="3" t="s">
-        <v>365</v>
-      </c>
+    <row r="150" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A150" s="18" t="s">
+        <v>770</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="C150" s="8"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+    </row>
+    <row r="151" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A151" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C151" s="8"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
     </row>
     <row r="152" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A152" s="7" t="s">
-        <v>366</v>
+      <c r="A152" s="18" t="s">
+        <v>354</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>171</v>
+        <v>355</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
     </row>
     <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="A153" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A154" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A155" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C155" s="8"/>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+    </row>
+    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A156" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C153" s="3" t="s">
+      <c r="C156" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D156" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E153" s="3" t="s">
+      <c r="E156" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A157" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C154" s="3" t="s">
+      <c r="C157" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D157" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E154" s="3" t="s">
+      <c r="E157" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A158" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C155" s="3" t="s">
+      <c r="C158" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D158" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E155" s="3" t="s">
+      <c r="E158" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A159" s="17" t="s">
         <v>371</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C156" s="3" t="s">
+      <c r="C159" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D159" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E156" s="3" t="s">
+      <c r="E159" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" s="7" t="s">
+    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="B157" s="9" t="s">
+      <c r="B160" s="9" t="s">
         <v>373</v>
-      </c>
-      <c r="C157" s="8"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="7"/>
-    </row>
-    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="B158" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C158" s="8"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>772</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="7" t="s">
-        <v>773</v>
-      </c>
-      <c r="B160" s="9" t="s">
-        <v>774</v>
       </c>
       <c r="C160" s="8"/>
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
     </row>
     <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>775</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>181</v>
-      </c>
+      <c r="A161" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C161" s="8"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
     </row>
     <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" s="7" t="s">
-        <v>776</v>
-      </c>
-      <c r="B162" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C162" s="8"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="7"/>
+      <c r="A162" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" s="7" t="s">
-        <v>778</v>
+      <c r="A163" s="18" t="s">
+        <v>773</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A164" s="7" t="s">
-        <v>780</v>
-      </c>
-      <c r="B164" s="9" t="s">
-        <v>781</v>
-      </c>
-      <c r="C164" s="8"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="7"/>
+      <c r="A164" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" s="7" t="s">
-        <v>782</v>
+      <c r="A165" s="18" t="s">
+        <v>776</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A166" s="7" t="s">
-        <v>784</v>
+    <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A166" s="18" t="s">
+        <v>778</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A167" s="7" t="s">
-        <v>786</v>
+    <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A167" s="18" t="s">
+        <v>780</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="7"/>
       <c r="E167" s="7"/>
     </row>
     <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>376</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D168" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A169" s="7" t="s">
-        <v>788</v>
+      <c r="A168" s="18" t="s">
+        <v>782</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="C168" s="8"/>
+      <c r="D168" s="7"/>
+      <c r="E168" s="7"/>
+    </row>
+    <row r="169" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A169" s="18" t="s">
+        <v>784</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>790</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>309</v>
-      </c>
+    <row r="170" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A170" s="18" t="s">
+        <v>786</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="C170" s="8"/>
+      <c r="D170" s="7"/>
+      <c r="E170" s="7"/>
     </row>
     <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A171" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="C171" s="8"/>
-      <c r="D171" s="7"/>
-      <c r="E171" s="7"/>
+      <c r="A171" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A172" s="7" t="s">
-        <v>793</v>
+      <c r="A172" s="18" t="s">
+        <v>788</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" s="7" t="s">
-        <v>795</v>
-      </c>
-      <c r="B173" s="9" t="s">
-        <v>796</v>
-      </c>
-      <c r="C173" s="8"/>
-      <c r="D173" s="7"/>
-      <c r="E173" s="7"/>
+      <c r="A173" s="17" t="s">
+        <v>790</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A174" s="7" t="s">
-        <v>797</v>
+      <c r="A174" s="18" t="s">
+        <v>791</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
     </row>
     <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="7" t="s">
-        <v>799</v>
+      <c r="A175" s="18" t="s">
+        <v>793</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>395</v>
+        <v>794</v>
       </c>
       <c r="C175" s="8"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
     </row>
     <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A176" s="7" t="s">
-        <v>800</v>
+      <c r="A176" s="18" t="s">
+        <v>795</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
       <c r="E176" s="7"/>
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A177" s="7" t="s">
-        <v>802</v>
+      <c r="A177" s="18" t="s">
+        <v>797</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
     <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A178" s="7" t="s">
-        <v>804</v>
+      <c r="A178" s="18" t="s">
+        <v>799</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>805</v>
+        <v>395</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A179" s="7" t="s">
-        <v>381</v>
+    <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A179" s="18" t="s">
+        <v>800</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>382</v>
+        <v>801</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
     </row>
     <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>383</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D180" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E180" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A180" s="18" t="s">
+        <v>802</v>
+      </c>
+      <c r="B180" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="C180" s="8"/>
+      <c r="D180" s="7"/>
+      <c r="E180" s="7"/>
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>806</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E181" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A182" s="7" t="s">
-        <v>807</v>
+      <c r="A181" s="18" t="s">
+        <v>804</v>
+      </c>
+      <c r="B181" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="C181" s="8"/>
+      <c r="D181" s="7"/>
+      <c r="E181" s="7"/>
+    </row>
+    <row r="182" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A182" s="18" t="s">
+        <v>381</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>808</v>
+        <v>382</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
     </row>
     <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" s="7" t="s">
-        <v>809</v>
-      </c>
-      <c r="B183" s="9" t="s">
-        <v>810</v>
-      </c>
-      <c r="C183" s="8"/>
-      <c r="D183" s="7"/>
-      <c r="E183" s="7"/>
-    </row>
-    <row r="184" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A184" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="B184" s="9" t="s">
-        <v>811</v>
-      </c>
-      <c r="C184" s="8"/>
-      <c r="D184" s="7"/>
-      <c r="E184" s="7"/>
+      <c r="A183" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A184" s="17" t="s">
+        <v>806</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A185" s="7" t="s">
-        <v>386</v>
+      <c r="A185" s="18" t="s">
+        <v>807</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>387</v>
+        <v>808</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
     <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A186" s="7" t="s">
-        <v>388</v>
+      <c r="A186" s="18" t="s">
+        <v>809</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>389</v>
+        <v>810</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A187" s="7" t="s">
-        <v>390</v>
+    <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A187" s="18" t="s">
+        <v>384</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>391</v>
+        <v>811</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A188" s="7" t="s">
-        <v>392</v>
+    <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A188" s="18" t="s">
+        <v>386</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
     <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A189" s="7" t="s">
-        <v>394</v>
+      <c r="A189" s="18" t="s">
+        <v>388</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A190" s="7" t="s">
-        <v>396</v>
+    <row r="190" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A190" s="18" t="s">
+        <v>390</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A191" s="7" t="s">
-        <v>398</v>
+    <row r="191" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A191" s="18" t="s">
+        <v>392</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
     <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A192" s="7" t="s">
-        <v>400</v>
+      <c r="A192" s="18" t="s">
+        <v>394</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
     </row>
-    <row r="193" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A193" s="7" t="s">
-        <v>812</v>
+    <row r="193" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A193" s="18" t="s">
+        <v>396</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>813</v>
+        <v>397</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A194" s="7" t="s">
-        <v>814</v>
+    <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A194" s="18" t="s">
+        <v>398</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>815</v>
+        <v>399</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A195" s="7" t="s">
-        <v>816</v>
+    <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A195" s="18" t="s">
+        <v>400</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>817</v>
+        <v>401</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A196" s="7" t="s">
-        <v>818</v>
+    <row r="196" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A196" s="18" t="s">
+        <v>812</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>393</v>
+        <v>813</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
     </row>
     <row r="197" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A197" s="7" t="s">
-        <v>819</v>
+      <c r="A197" s="18" t="s">
+        <v>814</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
     </row>
-    <row r="198" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A198" s="7" t="s">
-        <v>821</v>
+    <row r="198" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A198" s="18" t="s">
+        <v>816</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>397</v>
+        <v>817</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
     </row>
-    <row r="199" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A199" s="7" t="s">
-        <v>822</v>
+    <row r="199" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A199" s="18" t="s">
+        <v>818</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>823</v>
+        <v>393</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A200" s="7" t="s">
-        <v>824</v>
+    <row r="200" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A200" s="18" t="s">
+        <v>819</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
     </row>
-    <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A201" s="7" t="s">
-        <v>402</v>
+    <row r="201" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A201" s="18" t="s">
+        <v>821</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C201" s="8"/>
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
     </row>
-    <row r="202" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A202" s="7" t="s">
-        <v>404</v>
+    <row r="202" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A202" s="18" t="s">
+        <v>822</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>405</v>
+        <v>823</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
       <c r="E202" s="7"/>
     </row>
-    <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>406</v>
-      </c>
-      <c r="B203" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C203" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D203" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E203" s="3" t="s">
-        <v>410</v>
-      </c>
+    <row r="203" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A203" s="18" t="s">
+        <v>824</v>
+      </c>
+      <c r="B203" s="9" t="s">
+        <v>825</v>
+      </c>
+      <c r="C203" s="8"/>
+      <c r="D203" s="7"/>
+      <c r="E203" s="7"/>
     </row>
     <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>411</v>
-      </c>
-      <c r="B204" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="E204" s="3" t="s">
-        <v>414</v>
-      </c>
+      <c r="A204" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="B204" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C204" s="8"/>
+      <c r="D204" s="7"/>
+      <c r="E204" s="7"/>
     </row>
     <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A205" s="7" t="s">
-        <v>415</v>
+      <c r="A205" s="18" t="s">
+        <v>404</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
     </row>
     <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>417</v>
+      <c r="A206" s="17" t="s">
+        <v>406</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="E206" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A207" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B207" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C207" s="8"/>
-      <c r="D207" s="7"/>
-      <c r="E207" s="7"/>
-    </row>
-    <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A208" s="7" t="s">
-        <v>424</v>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A207" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A208" s="18" t="s">
+        <v>415</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="C208" s="8"/>
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
     </row>
-    <row r="209" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
-        <v>826</v>
+    <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A209" s="17" t="s">
+        <v>417</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>827</v>
+        <v>418</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>828</v>
+        <v>419</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>829</v>
+        <v>420</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>830</v>
+        <v>421</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A210" s="7" t="s">
-        <v>426</v>
+      <c r="A210" s="18" t="s">
+        <v>422</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C210" s="8"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
     </row>
     <row r="211" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A211" s="7" t="s">
-        <v>428</v>
+      <c r="A211" s="18" t="s">
+        <v>424</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
     </row>
-    <row r="212" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A212" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="B212" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="C212" s="8"/>
-      <c r="D212" s="7"/>
-      <c r="E212" s="7"/>
-    </row>
-    <row r="213" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A213" s="7" t="s">
-        <v>431</v>
+    <row r="212" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A212" s="17" t="s">
+        <v>826</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A213" s="18" t="s">
+        <v>426</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>403</v>
+        <v>427</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="7"/>
       <c r="E213" s="7"/>
     </row>
-    <row r="214" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A214" s="7" t="s">
-        <v>432</v>
+    <row r="214" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A214" s="18" t="s">
+        <v>428</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="7"/>
       <c r="E214" s="7"/>
     </row>
     <row r="215" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A215" s="7" t="s">
-        <v>831</v>
+      <c r="A215" s="18" t="s">
+        <v>429</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C215" s="8"/>
       <c r="D215" s="7"/>
       <c r="E215" s="7"/>
     </row>
-    <row r="216" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A216" s="7" t="s">
-        <v>832</v>
+    <row r="216" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A216" s="18" t="s">
+        <v>431</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>833</v>
+        <v>403</v>
       </c>
       <c r="C216" s="8"/>
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
     </row>
-    <row r="217" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A217" s="7" t="s">
-        <v>834</v>
+    <row r="217" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A217" s="18" t="s">
+        <v>432</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>835</v>
+        <v>405</v>
       </c>
       <c r="C217" s="8"/>
       <c r="D217" s="7"/>
       <c r="E217" s="7"/>
     </row>
     <row r="218" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A218" s="7" t="s">
-        <v>836</v>
+      <c r="A218" s="18" t="s">
+        <v>831</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>837</v>
+        <v>423</v>
       </c>
       <c r="C218" s="8"/>
       <c r="D218" s="7"/>
       <c r="E218" s="7"/>
     </row>
-    <row r="219" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
+    <row r="219" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A219" s="18" t="s">
+        <v>832</v>
+      </c>
+      <c r="B219" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="C219" s="8"/>
+      <c r="D219" s="7"/>
+      <c r="E219" s="7"/>
+    </row>
+    <row r="220" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A220" s="18" t="s">
+        <v>834</v>
+      </c>
+      <c r="B220" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="C220" s="8"/>
+      <c r="D220" s="7"/>
+      <c r="E220" s="7"/>
+    </row>
+    <row r="221" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A221" s="18" t="s">
+        <v>836</v>
+      </c>
+      <c r="B221" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C221" s="8"/>
+      <c r="D221" s="7"/>
+      <c r="E221" s="7"/>
+    </row>
+    <row r="222" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A222" s="17" t="s">
         <v>876</v>
       </c>
-      <c r="B219" s="15" t="s">
+      <c r="B222" s="15" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
+    <row r="223" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A223" s="17" t="s">
         <v>877</v>
       </c>
-      <c r="B220" s="4" t="s">
+      <c r="B223" s="4" t="s">
         <v>893</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E218" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E221" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(surveillance): pfa rate map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA6BD05-4D1E-C947-B36C-7B5A9572E42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98644FCC-E145-0C46-B1AB-5FE469799A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-2640" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$224</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="916">
   <si>
     <t>LABEL</t>
   </si>
@@ -2787,6 +2787,21 @@
   </si>
   <si>
     <t>Proporción de unidades notificadoras que enviaron información en todas las semanas</t>
+  </si>
+  <si>
+    <t>surveillance_pfa_rate</t>
+  </si>
+  <si>
+    <t>Tasa PFA</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>surveillance_title_map_pfa_rate</t>
   </si>
 </sst>
 </file>
@@ -6047,10 +6062,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E223"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7898,65 +7913,65 @@
     </row>
     <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="18" t="s">
-        <v>340</v>
+        <v>911</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>341</v>
+        <v>912</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="18" t="s">
-        <v>342</v>
+        <v>915</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>343</v>
+        <v>912</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="18" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="18" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="18" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="18" t="s">
-        <v>746</v>
+        <v>346</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>747</v>
+        <v>347</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="7"/>
@@ -7964,60 +7979,54 @@
     </row>
     <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
-        <v>748</v>
+        <v>348</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>749</v>
+        <v>349</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="7"/>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="18" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="18" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
       <c r="E144" s="7"/>
     </row>
     <row r="145" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A145" s="17" t="s">
-        <v>754</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>758</v>
-      </c>
+      <c r="A145" s="18" t="s">
+        <v>750</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>751</v>
+      </c>
+      <c r="C145" s="8"/>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
     </row>
     <row r="146" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="18" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
@@ -8025,49 +8034,55 @@
     </row>
     <row r="147" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="18" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
     </row>
     <row r="149" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A149" s="18" t="s">
-        <v>768</v>
-      </c>
-      <c r="B149" s="9" t="s">
-        <v>769</v>
-      </c>
-      <c r="C149" s="8"/>
-      <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
+      <c r="A149" s="17" t="s">
+        <v>761</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="150" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="18" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="7"/>
@@ -8075,10 +8090,10 @@
     </row>
     <row r="151" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" s="18" t="s">
-        <v>352</v>
+        <v>768</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>353</v>
+        <v>769</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="7"/>
@@ -8086,173 +8101,167 @@
     </row>
     <row r="152" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" s="18" t="s">
-        <v>354</v>
+        <v>770</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>355</v>
+        <v>771</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="17" t="s">
+    <row r="153" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A153" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C153" s="8"/>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
+    </row>
+    <row r="154" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A154" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C154" s="8"/>
+      <c r="D154" s="7"/>
+      <c r="E154" s="7"/>
+    </row>
+    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A155" s="17" t="s">
         <v>356</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="C153" s="3" t="s">
+      <c r="C155" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D155" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="E153" s="3" t="s">
+      <c r="E155" s="3" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A155" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="B155" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C155" s="8"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
     </row>
     <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>173</v>
+        <v>362</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>174</v>
+        <v>363</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>175</v>
+        <v>364</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>181</v>
-      </c>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A157" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C157" s="8"/>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7"/>
     </row>
     <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" s="17" t="s">
         <v>371</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C161" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D161" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E161" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="18" t="s">
+    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A162" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="B160" s="9" t="s">
+      <c r="B162" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="C160" s="8"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
-    </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="B161" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C161" s="8"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="7"/>
-    </row>
-    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" s="17" t="s">
-        <v>772</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="C162" s="8"/>
+      <c r="D162" s="7"/>
+      <c r="E162" s="7"/>
     </row>
     <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="18" t="s">
-        <v>773</v>
+        <v>374</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>774</v>
+        <v>375</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="7"/>
@@ -8260,49 +8269,55 @@
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="18" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
     </row>
     <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" s="18" t="s">
-        <v>778</v>
-      </c>
-      <c r="B166" s="9" t="s">
-        <v>779</v>
-      </c>
-      <c r="C166" s="8"/>
-      <c r="D166" s="7"/>
-      <c r="E166" s="7"/>
+      <c r="A166" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="18" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="7"/>
@@ -8310,60 +8325,54 @@
     </row>
     <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="18" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C168" s="8"/>
       <c r="D168" s="7"/>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="18" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="18" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A171" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A171" s="18" t="s">
+        <v>784</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>785</v>
+      </c>
+      <c r="C171" s="8"/>
+      <c r="D171" s="7"/>
+      <c r="E171" s="7"/>
+    </row>
+    <row r="172" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" s="18" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -8371,49 +8380,55 @@
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>790</v>
+        <v>376</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>306</v>
+        <v>377</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>307</v>
+        <v>378</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>308</v>
+        <v>379</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>309</v>
+        <v>380</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="18" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
     </row>
     <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="18" t="s">
-        <v>793</v>
-      </c>
-      <c r="B175" s="9" t="s">
-        <v>794</v>
-      </c>
-      <c r="C175" s="8"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="7"/>
+      <c r="A175" s="17" t="s">
+        <v>790</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="18" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
@@ -8421,10 +8436,10 @@
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="18" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
@@ -8432,10 +8447,10 @@
     </row>
     <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="18" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>395</v>
+        <v>796</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
@@ -8443,10 +8458,10 @@
     </row>
     <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="18" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="7"/>
@@ -8454,10 +8469,10 @@
     </row>
     <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="18" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>803</v>
+        <v>395</v>
       </c>
       <c r="C180" s="8"/>
       <c r="D180" s="7"/>
@@ -8465,88 +8480,88 @@
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="18" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="18" t="s">
-        <v>381</v>
+        <v>802</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>382</v>
+        <v>803</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
     </row>
     <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" s="17" t="s">
+      <c r="A183" s="18" t="s">
+        <v>804</v>
+      </c>
+      <c r="B183" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="C183" s="8"/>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
+    </row>
+    <row r="184" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A184" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="B184" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C184" s="8"/>
+      <c r="D184" s="7"/>
+      <c r="E184" s="7"/>
+    </row>
+    <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A185" s="17" t="s">
         <v>383</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B185" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C183" s="3" t="s">
+      <c r="C185" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D183" s="3" t="s">
+      <c r="D185" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E183" s="3" t="s">
+      <c r="E185" s="3" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A184" s="17" t="s">
+    <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A186" s="17" t="s">
         <v>806</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B186" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C184" s="3" t="s">
+      <c r="C186" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D184" s="3" t="s">
+      <c r="D186" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E184" s="3" t="s">
+      <c r="E186" s="3" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A185" s="18" t="s">
+    <row r="187" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A187" s="18" t="s">
         <v>807</v>
       </c>
-      <c r="B185" s="9" t="s">
+      <c r="B187" s="9" t="s">
         <v>808</v>
-      </c>
-      <c r="C185" s="8"/>
-      <c r="D185" s="7"/>
-      <c r="E185" s="7"/>
-    </row>
-    <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A186" s="18" t="s">
-        <v>809</v>
-      </c>
-      <c r="B186" s="9" t="s">
-        <v>810</v>
-      </c>
-      <c r="C186" s="8"/>
-      <c r="D186" s="7"/>
-      <c r="E186" s="7"/>
-    </row>
-    <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A187" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="B187" s="9" t="s">
-        <v>811</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
@@ -8554,54 +8569,54 @@
     </row>
     <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="18" t="s">
-        <v>386</v>
+        <v>809</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>387</v>
+        <v>810</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" s="18" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>389</v>
+        <v>811</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="18" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="18" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A192" s="18" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
@@ -8609,10 +8624,10 @@
     </row>
     <row r="193" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="18" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
@@ -8620,76 +8635,76 @@
     </row>
     <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" s="18" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" s="18" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="18" t="s">
-        <v>812</v>
+        <v>398</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>813</v>
+        <v>399</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
     </row>
-    <row r="197" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="18" t="s">
-        <v>814</v>
+        <v>400</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>815</v>
+        <v>401</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
     </row>
-    <row r="198" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A198" s="18" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
     </row>
-    <row r="199" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A199" s="18" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>393</v>
+        <v>815</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
@@ -8697,166 +8712,159 @@
     </row>
     <row r="201" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A201" s="18" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C201" s="8"/>
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
     </row>
-    <row r="202" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A202" s="18" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
       <c r="E202" s="7"/>
     </row>
-    <row r="203" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" s="18" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>825</v>
+        <v>397</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
       <c r="E203" s="7"/>
     </row>
-    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>402</v>
+        <v>822</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>403</v>
+        <v>823</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
     </row>
-    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>404</v>
+        <v>824</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>405</v>
+        <v>825</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
     </row>
     <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A206" s="17" t="s">
+      <c r="A206" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="B206" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C206" s="8"/>
+      <c r="D206" s="7"/>
+      <c r="E206" s="7"/>
+    </row>
+    <row r="207" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A207" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="B207" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C207" s="8"/>
+      <c r="D207" s="7"/>
+      <c r="E207" s="7"/>
+    </row>
+    <row r="208" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A208" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="B206" s="4" t="s">
+      <c r="B208" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="C206" s="3" t="s">
+      <c r="C208" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="D206" s="3" t="s">
+      <c r="D208" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E206" s="3" t="s">
+      <c r="E208" s="3" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A207" s="17" t="s">
-        <v>411</v>
-      </c>
-      <c r="B207" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D207" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="E207" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A208" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="B208" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="C208" s="8"/>
-      <c r="D208" s="7"/>
-      <c r="E208" s="7"/>
     </row>
     <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="17" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A210" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="B210" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C210" s="8"/>
-      <c r="D210" s="7"/>
-      <c r="E210" s="7"/>
-    </row>
-    <row r="211" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>913</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="D210" s="3"/>
+      <c r="E210" s="3"/>
+    </row>
+    <row r="211" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="18" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
     </row>
-    <row r="212" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="17" t="s">
-        <v>826</v>
+        <v>417</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>827</v>
+        <v>418</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>828</v>
+        <v>419</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>829</v>
+        <v>420</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>830</v>
+        <v>421</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A213" s="18" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="7"/>
@@ -8864,43 +8872,49 @@
     </row>
     <row r="214" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A214" s="18" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="7"/>
       <c r="E214" s="7"/>
     </row>
-    <row r="215" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A215" s="18" t="s">
-        <v>429</v>
-      </c>
-      <c r="B215" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="C215" s="8"/>
-      <c r="D215" s="7"/>
-      <c r="E215" s="7"/>
-    </row>
-    <row r="216" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A215" s="17" t="s">
+        <v>826</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" s="18" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>403</v>
+        <v>427</v>
       </c>
       <c r="C216" s="8"/>
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
     </row>
-    <row r="217" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A217" s="18" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="C217" s="8"/>
       <c r="D217" s="7"/>
@@ -8908,32 +8922,32 @@
     </row>
     <row r="218" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A218" s="18" t="s">
-        <v>831</v>
+        <v>429</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C218" s="8"/>
       <c r="D218" s="7"/>
       <c r="E218" s="7"/>
     </row>
-    <row r="219" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A219" s="18" t="s">
-        <v>832</v>
+        <v>431</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>833</v>
+        <v>403</v>
       </c>
       <c r="C219" s="8"/>
       <c r="D219" s="7"/>
       <c r="E219" s="7"/>
     </row>
-    <row r="220" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A220" s="18" t="s">
-        <v>834</v>
+        <v>432</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>835</v>
+        <v>405</v>
       </c>
       <c r="C220" s="8"/>
       <c r="D220" s="7"/>
@@ -8941,33 +8955,66 @@
     </row>
     <row r="221" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" s="18" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>837</v>
+        <v>423</v>
       </c>
       <c r="C221" s="8"/>
       <c r="D221" s="7"/>
       <c r="E221" s="7"/>
     </row>
-    <row r="222" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A222" s="17" t="s">
+    <row r="222" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A222" s="18" t="s">
+        <v>832</v>
+      </c>
+      <c r="B222" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="C222" s="8"/>
+      <c r="D222" s="7"/>
+      <c r="E222" s="7"/>
+    </row>
+    <row r="223" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A223" s="18" t="s">
+        <v>834</v>
+      </c>
+      <c r="B223" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="C223" s="8"/>
+      <c r="D223" s="7"/>
+      <c r="E223" s="7"/>
+    </row>
+    <row r="224" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A224" s="18" t="s">
+        <v>836</v>
+      </c>
+      <c r="B224" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C224" s="8"/>
+      <c r="D224" s="7"/>
+      <c r="E224" s="7"/>
+    </row>
+    <row r="225" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A225" s="17" t="s">
         <v>876</v>
       </c>
-      <c r="B222" s="15" t="s">
+      <c r="B225" s="15" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A223" s="17" t="s">
+    <row r="226" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A226" s="17" t="s">
         <v>877</v>
       </c>
-      <c r="B223" s="4" t="s">
+      <c r="B226" s="4" t="s">
         <v>893</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E221" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E224" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(surveillance): pfa notified and investigated map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98644FCC-E145-0C46-B1AB-5FE469799A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF63F80-F774-124A-8897-8A3C87C9B661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$224</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="929">
   <si>
     <t>LABEL</t>
   </si>
@@ -2802,6 +2802,45 @@
   </si>
   <si>
     <t>surveillance_title_map_pfa_rate</t>
+  </si>
+  <si>
+    <t>surveillance_pfa_population_text</t>
+  </si>
+  <si>
+    <t>Vigilancia de las PFA para municipios con &gt;100000 menores de 15 años O municipios con &lt;100000 menores de 15 años que tuvieron casos de PFA en el 2022</t>
+  </si>
+  <si>
+    <t>surveillance_pfa_notification</t>
+  </si>
+  <si>
+    <t>Notificación oportuna</t>
+  </si>
+  <si>
+    <t>surveillance_title_map_pfa_notification</t>
+  </si>
+  <si>
+    <t>Proporción de casos de PFA con notificación oportuna (antes de 14 días desde el inicio de la parálisis)</t>
+  </si>
+  <si>
+    <t>surveillance_prop_pfa_notification</t>
+  </si>
+  <si>
+    <t>Proporción de notificaciones oportunas</t>
+  </si>
+  <si>
+    <t>surveillance_prop_pfa_cases</t>
+  </si>
+  <si>
+    <t>surveillance_pfa_investigated</t>
+  </si>
+  <si>
+    <t>surveillance_title_map_pfa_investigated</t>
+  </si>
+  <si>
+    <t>Investigación oportuna</t>
+  </si>
+  <si>
+    <t>Proporción de casos de PFA investigados en menos de 48 horas</t>
   </si>
 </sst>
 </file>
@@ -6062,10 +6101,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7933,12 +7972,12 @@
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A138" s="18" t="s">
-        <v>340</v>
+        <v>916</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>341</v>
+        <v>917</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
@@ -7946,21 +7985,21 @@
     </row>
     <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="18" t="s">
-        <v>342</v>
+        <v>918</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>343</v>
+        <v>919</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A140" s="18" t="s">
-        <v>344</v>
+        <v>920</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>345</v>
+        <v>921</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
@@ -7968,10 +8007,10 @@
     </row>
     <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="18" t="s">
-        <v>346</v>
+        <v>922</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>347</v>
+        <v>923</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="7"/>
@@ -7979,21 +8018,21 @@
     </row>
     <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
-        <v>348</v>
+        <v>925</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>349</v>
+        <v>927</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="7"/>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A143" s="18" t="s">
-        <v>746</v>
+        <v>926</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>747</v>
+        <v>928</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="7"/>
@@ -8001,99 +8040,87 @@
     </row>
     <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="18" t="s">
-        <v>748</v>
+        <v>924</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>749</v>
+        <v>324</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="18" t="s">
-        <v>750</v>
+        <v>340</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>751</v>
+        <v>341</v>
       </c>
       <c r="C145" s="8"/>
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="18" t="s">
-        <v>752</v>
+        <v>342</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>753</v>
+        <v>343</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
     </row>
     <row r="147" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A147" s="17" t="s">
-        <v>754</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>758</v>
-      </c>
+      <c r="A147" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="C147" s="8"/>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
     </row>
     <row r="148" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="18" t="s">
-        <v>759</v>
+        <v>346</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>760</v>
+        <v>347</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A149" s="17" t="s">
-        <v>761</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>762</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A149" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C149" s="8"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="18" t="s">
-        <v>766</v>
+        <v>746</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>767</v>
+        <v>747</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="18" t="s">
-        <v>768</v>
+        <v>748</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>769</v>
+        <v>749</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="7"/>
@@ -8101,10 +8128,10 @@
     </row>
     <row r="152" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" s="18" t="s">
-        <v>770</v>
+        <v>750</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>771</v>
+        <v>751</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="7"/>
@@ -8112,192 +8139,180 @@
     </row>
     <row r="153" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="18" t="s">
-        <v>352</v>
+        <v>752</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>353</v>
+        <v>753</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
     </row>
     <row r="154" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A154" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="B154" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="C154" s="8"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-    </row>
-    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A154" s="17" t="s">
+        <v>754</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A155" s="18" t="s">
+        <v>759</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="C155" s="8"/>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+    </row>
+    <row r="156" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>361</v>
+        <v>761</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>362</v>
+        <v>762</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>363</v>
+        <v>763</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>364</v>
+        <v>764</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>365</v>
+        <v>765</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A157" s="18" t="s">
-        <v>366</v>
+        <v>766</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>171</v>
+        <v>767</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="17" t="s">
+    <row r="158" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A158" s="18" t="s">
+        <v>768</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="C158" s="8"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A159" s="18" t="s">
+        <v>770</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="C159" s="8"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A160" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C160" s="8"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A161" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C161" s="8"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
+    </row>
+    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A162" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A163" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A164" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C164" s="8"/>
+      <c r="D164" s="7"/>
+      <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A165" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C165" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D165" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E165" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E160" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="B162" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="C162" s="8"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="7"/>
-    </row>
-    <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="B163" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C163" s="8"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="7"/>
-    </row>
-    <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A164" s="17" t="s">
-        <v>772</v>
-      </c>
-      <c r="B164" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" s="18" t="s">
-        <v>773</v>
-      </c>
-      <c r="B165" s="9" t="s">
-        <v>774</v>
-      </c>
-      <c r="C165" s="8"/>
-      <c r="D165" s="7"/>
-      <c r="E165" s="7"/>
     </row>
     <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>775</v>
+        <v>369</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>178</v>
@@ -8313,33 +8328,45 @@
       </c>
     </row>
     <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" s="18" t="s">
-        <v>776</v>
-      </c>
-      <c r="B167" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C167" s="8"/>
-      <c r="D167" s="7"/>
-      <c r="E167" s="7"/>
+      <c r="A167" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" s="18" t="s">
-        <v>778</v>
-      </c>
-      <c r="B168" s="9" t="s">
-        <v>779</v>
-      </c>
-      <c r="C168" s="8"/>
-      <c r="D168" s="7"/>
-      <c r="E168" s="7"/>
+      <c r="A168" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="18" t="s">
-        <v>780</v>
+        <v>372</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>781</v>
+        <v>373</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
@@ -8347,32 +8374,38 @@
     </row>
     <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="18" t="s">
-        <v>782</v>
+        <v>374</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>783</v>
+        <v>375</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A171" s="18" t="s">
-        <v>784</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>785</v>
-      </c>
-      <c r="C171" s="8"/>
-      <c r="D171" s="7"/>
-      <c r="E171" s="7"/>
-    </row>
-    <row r="172" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A171" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="18" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>787</v>
+        <v>774</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -8380,55 +8413,49 @@
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>376</v>
+        <v>775</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>377</v>
+        <v>178</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>378</v>
+        <v>179</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>379</v>
+        <v>180</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>380</v>
+        <v>181</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="18" t="s">
-        <v>788</v>
+        <v>776</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>789</v>
+        <v>777</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
     </row>
     <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="17" t="s">
-        <v>790</v>
-      </c>
-      <c r="B175" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>309</v>
-      </c>
+      <c r="A175" s="18" t="s">
+        <v>778</v>
+      </c>
+      <c r="B175" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="C175" s="8"/>
+      <c r="D175" s="7"/>
+      <c r="E175" s="7"/>
     </row>
     <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="18" t="s">
-        <v>791</v>
+        <v>780</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>792</v>
+        <v>781</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="7"/>
@@ -8436,132 +8463,132 @@
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="18" t="s">
-        <v>793</v>
+        <v>782</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>794</v>
+        <v>783</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A178" s="18" t="s">
-        <v>795</v>
+        <v>784</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>796</v>
+        <v>785</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" s="18" t="s">
-        <v>797</v>
+        <v>786</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>798</v>
+        <v>787</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
     </row>
     <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A180" s="18" t="s">
-        <v>799</v>
-      </c>
-      <c r="B180" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="C180" s="8"/>
-      <c r="D180" s="7"/>
-      <c r="E180" s="7"/>
+      <c r="A180" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="18" t="s">
-        <v>800</v>
+        <v>788</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>801</v>
+        <v>789</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
     </row>
     <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A182" s="18" t="s">
-        <v>802</v>
-      </c>
-      <c r="B182" s="9" t="s">
-        <v>803</v>
-      </c>
-      <c r="C182" s="8"/>
-      <c r="D182" s="7"/>
-      <c r="E182" s="7"/>
+      <c r="A182" s="17" t="s">
+        <v>790</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="18" t="s">
-        <v>804</v>
+        <v>791</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>805</v>
+        <v>792</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="7"/>
       <c r="E183" s="7"/>
     </row>
-    <row r="184" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="18" t="s">
-        <v>381</v>
+        <v>793</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>382</v>
+        <v>794</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
     <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A185" s="17" t="s">
-        <v>383</v>
-      </c>
-      <c r="B185" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D185" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E185" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A185" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="B185" s="9" t="s">
+        <v>796</v>
+      </c>
+      <c r="C185" s="8"/>
+      <c r="D185" s="7"/>
+      <c r="E185" s="7"/>
     </row>
     <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A186" s="17" t="s">
-        <v>806</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A186" s="18" t="s">
+        <v>797</v>
+      </c>
+      <c r="B186" s="9" t="s">
+        <v>798</v>
+      </c>
+      <c r="C186" s="8"/>
+      <c r="D186" s="7"/>
+      <c r="E186" s="7"/>
     </row>
     <row r="187" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="18" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>808</v>
+        <v>395</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
@@ -8569,21 +8596,21 @@
     </row>
     <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="18" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="18" t="s">
-        <v>384</v>
+        <v>802</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
@@ -8591,76 +8618,88 @@
     </row>
     <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="18" t="s">
-        <v>386</v>
+        <v>804</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>387</v>
+        <v>805</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" s="18" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A192" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="B192" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="C192" s="8"/>
-      <c r="D192" s="7"/>
-      <c r="E192" s="7"/>
-    </row>
-    <row r="193" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A193" s="18" t="s">
-        <v>392</v>
-      </c>
-      <c r="B193" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="C193" s="8"/>
-      <c r="D193" s="7"/>
-      <c r="E193" s="7"/>
+    <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A192" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A193" s="17" t="s">
+        <v>806</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" s="18" t="s">
-        <v>394</v>
+        <v>807</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>395</v>
+        <v>808</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="18" t="s">
-        <v>396</v>
+        <v>809</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>397</v>
+        <v>810</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A196" s="18" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>399</v>
+        <v>811</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="7"/>
@@ -8668,21 +8707,21 @@
     </row>
     <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="18" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
     </row>
-    <row r="198" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="18" t="s">
-        <v>812</v>
+        <v>388</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>813</v>
+        <v>389</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
@@ -8690,65 +8729,65 @@
     </row>
     <row r="199" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A199" s="18" t="s">
-        <v>814</v>
+        <v>390</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>815</v>
+        <v>391</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
-        <v>816</v>
+        <v>392</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>817</v>
+        <v>393</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
     </row>
-    <row r="201" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="18" t="s">
-        <v>818</v>
+        <v>394</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C201" s="8"/>
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
     </row>
-    <row r="202" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" s="18" t="s">
-        <v>819</v>
+        <v>396</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>820</v>
+        <v>397</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
       <c r="E202" s="7"/>
     </row>
-    <row r="203" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="18" t="s">
-        <v>821</v>
+        <v>398</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
       <c r="E203" s="7"/>
     </row>
-    <row r="204" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>822</v>
+        <v>400</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>823</v>
+        <v>401</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="7"/>
@@ -8756,198 +8795,192 @@
     </row>
     <row r="205" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>824</v>
+        <v>812</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>825</v>
+        <v>813</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
     </row>
-    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>402</v>
+        <v>814</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>403</v>
+        <v>815</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="7"/>
       <c r="E206" s="7"/>
     </row>
-    <row r="207" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A207" s="18" t="s">
-        <v>404</v>
+        <v>816</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>405</v>
+        <v>817</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="7"/>
       <c r="E207" s="7"/>
     </row>
-    <row r="208" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A208" s="17" t="s">
-        <v>406</v>
-      </c>
-      <c r="B208" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D208" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E208" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A209" s="17" t="s">
-        <v>411</v>
-      </c>
-      <c r="B209" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D209" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="E209" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A208" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="B208" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C208" s="8"/>
+      <c r="D208" s="7"/>
+      <c r="E208" s="7"/>
+    </row>
+    <row r="209" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A209" s="18" t="s">
+        <v>819</v>
+      </c>
+      <c r="B209" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="C209" s="8"/>
+      <c r="D209" s="7"/>
+      <c r="E209" s="7"/>
+    </row>
+    <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="18" t="s">
-        <v>913</v>
-      </c>
-      <c r="B210" s="4" t="s">
-        <v>914</v>
-      </c>
-      <c r="D210" s="3"/>
-      <c r="E210" s="3"/>
-    </row>
-    <row r="211" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>821</v>
+      </c>
+      <c r="B210" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C210" s="8"/>
+      <c r="D210" s="7"/>
+      <c r="E210" s="7"/>
+    </row>
+    <row r="211" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A211" s="18" t="s">
-        <v>415</v>
+        <v>822</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>416</v>
+        <v>823</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
     </row>
-    <row r="212" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A212" s="17" t="s">
-        <v>417</v>
-      </c>
-      <c r="B212" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D212" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="E212" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A212" s="18" t="s">
+        <v>824</v>
+      </c>
+      <c r="B212" s="9" t="s">
+        <v>825</v>
+      </c>
+      <c r="C212" s="8"/>
+      <c r="D212" s="7"/>
+      <c r="E212" s="7"/>
+    </row>
+    <row r="213" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="18" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="7"/>
       <c r="E213" s="7"/>
     </row>
-    <row r="214" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A214" s="18" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="7"/>
       <c r="E214" s="7"/>
     </row>
-    <row r="215" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A215" s="17" t="s">
-        <v>826</v>
+        <v>406</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>827</v>
+        <v>407</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>828</v>
+        <v>408</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>829</v>
+        <v>409</v>
       </c>
       <c r="E215" s="3" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A216" s="18" t="s">
-        <v>426</v>
-      </c>
-      <c r="B216" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="C216" s="8"/>
-      <c r="D216" s="7"/>
-      <c r="E216" s="7"/>
-    </row>
-    <row r="217" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A216" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="18" t="s">
-        <v>428</v>
-      </c>
-      <c r="B217" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C217" s="8"/>
-      <c r="D217" s="7"/>
-      <c r="E217" s="7"/>
-    </row>
-    <row r="218" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>913</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="D217" s="3"/>
+      <c r="E217" s="3"/>
+    </row>
+    <row r="218" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A218" s="18" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="C218" s="8"/>
       <c r="D218" s="7"/>
       <c r="E218" s="7"/>
     </row>
     <row r="219" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A219" s="18" t="s">
-        <v>431</v>
-      </c>
-      <c r="B219" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="C219" s="8"/>
-      <c r="D219" s="7"/>
-      <c r="E219" s="7"/>
-    </row>
-    <row r="220" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A219" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A220" s="18" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="C220" s="8"/>
       <c r="D220" s="7"/>
@@ -8955,32 +8988,38 @@
     </row>
     <row r="221" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" s="18" t="s">
-        <v>831</v>
+        <v>424</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C221" s="8"/>
       <c r="D221" s="7"/>
       <c r="E221" s="7"/>
     </row>
-    <row r="222" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A222" s="18" t="s">
-        <v>832</v>
-      </c>
-      <c r="B222" s="9" t="s">
-        <v>833</v>
-      </c>
-      <c r="C222" s="8"/>
-      <c r="D222" s="7"/>
-      <c r="E222" s="7"/>
+    <row r="222" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A222" s="17" t="s">
+        <v>826</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="223" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A223" s="18" t="s">
-        <v>834</v>
+        <v>426</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>835</v>
+        <v>427</v>
       </c>
       <c r="C223" s="8"/>
       <c r="D223" s="7"/>
@@ -8988,33 +9027,110 @@
     </row>
     <row r="224" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" s="18" t="s">
-        <v>836</v>
+        <v>428</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>837</v>
+        <v>423</v>
       </c>
       <c r="C224" s="8"/>
       <c r="D224" s="7"/>
       <c r="E224" s="7"/>
     </row>
-    <row r="225" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A225" s="17" t="s">
+    <row r="225" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A225" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="B225" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C225" s="8"/>
+      <c r="D225" s="7"/>
+      <c r="E225" s="7"/>
+    </row>
+    <row r="226" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A226" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="B226" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C226" s="8"/>
+      <c r="D226" s="7"/>
+      <c r="E226" s="7"/>
+    </row>
+    <row r="227" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A227" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="B227" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C227" s="8"/>
+      <c r="D227" s="7"/>
+      <c r="E227" s="7"/>
+    </row>
+    <row r="228" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A228" s="18" t="s">
+        <v>831</v>
+      </c>
+      <c r="B228" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C228" s="8"/>
+      <c r="D228" s="7"/>
+      <c r="E228" s="7"/>
+    </row>
+    <row r="229" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A229" s="18" t="s">
+        <v>832</v>
+      </c>
+      <c r="B229" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="C229" s="8"/>
+      <c r="D229" s="7"/>
+      <c r="E229" s="7"/>
+    </row>
+    <row r="230" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A230" s="18" t="s">
+        <v>834</v>
+      </c>
+      <c r="B230" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="C230" s="8"/>
+      <c r="D230" s="7"/>
+      <c r="E230" s="7"/>
+    </row>
+    <row r="231" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A231" s="18" t="s">
+        <v>836</v>
+      </c>
+      <c r="B231" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C231" s="8"/>
+      <c r="D231" s="7"/>
+      <c r="E231" s="7"/>
+    </row>
+    <row r="232" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A232" s="17" t="s">
         <v>876</v>
       </c>
-      <c r="B225" s="15" t="s">
+      <c r="B232" s="15" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A226" s="17" t="s">
+    <row r="233" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A233" s="17" t="s">
         <v>877</v>
       </c>
-      <c r="B226" s="4" t="s">
+      <c r="B233" s="4" t="s">
         <v>893</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E224" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E231" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(survaillance): suitable samples, followups, active search maps
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF63F80-F774-124A-8897-8A3C87C9B661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242C3B6B-CE25-B84F-9C00-A5C7D5C90F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$231</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$241</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="953">
   <si>
     <t>LABEL</t>
   </si>
@@ -2841,6 +2841,78 @@
   </si>
   <si>
     <t>Proporción de casos de PFA investigados en menos de 48 horas</t>
+  </si>
+  <si>
+    <t>surveillance_suitable_samples</t>
+  </si>
+  <si>
+    <t>surveillance_title_map_suitable_samples</t>
+  </si>
+  <si>
+    <t>Muestras adecuadas</t>
+  </si>
+  <si>
+    <t>Proporción de casos con muestra adecuada de heces</t>
+  </si>
+  <si>
+    <t>surveillance_prop_samples</t>
+  </si>
+  <si>
+    <t>surveillance_followups</t>
+  </si>
+  <si>
+    <t>surveillance_title_map_followups</t>
+  </si>
+  <si>
+    <t>Seguimiento de casos</t>
+  </si>
+  <si>
+    <t>Proporción de casos con seguimiento a los 60 días</t>
+  </si>
+  <si>
+    <t>surveillance_active_search</t>
+  </si>
+  <si>
+    <t>surveillance_title_map_active_search</t>
+  </si>
+  <si>
+    <t>Búsqueda activa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Búsquedas activas institucionales en al menos un establecimiento de salud </t>
+  </si>
+  <si>
+    <t>surveillance_active_search_text</t>
+  </si>
+  <si>
+    <t>¿En los municipios con &lt;100000 menores de 15 años y que no presentaron casos de PFA, se llevaron a cabo búsquedas activas institucionales en al menos un establecimiento de salud del municipio?</t>
+  </si>
+  <si>
+    <t>yes_upper</t>
+  </si>
+  <si>
+    <t>no_upper</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NON</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t>OUI</t>
+  </si>
+  <si>
+    <t>NÃO</t>
   </si>
 </sst>
 </file>
@@ -6101,10 +6173,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A219" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8040,10 +8112,10 @@
     </row>
     <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="18" t="s">
-        <v>924</v>
+        <v>929</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>324</v>
+        <v>931</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
@@ -8051,7 +8123,7 @@
     </row>
     <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="18" t="s">
-        <v>340</v>
+        <v>933</v>
       </c>
       <c r="B145" s="9" t="s">
         <v>341</v>
@@ -8060,23 +8132,23 @@
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="18" t="s">
-        <v>342</v>
+        <v>930</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>343</v>
+        <v>932</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="18" t="s">
-        <v>344</v>
+        <v>934</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>345</v>
+        <v>936</v>
       </c>
       <c r="C147" s="8"/>
       <c r="D147" s="7"/>
@@ -8084,10 +8156,10 @@
     </row>
     <row r="148" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="18" t="s">
-        <v>346</v>
+        <v>935</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>347</v>
+        <v>937</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
@@ -8095,132 +8167,120 @@
     </row>
     <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="18" t="s">
-        <v>348</v>
+        <v>938</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>349</v>
+        <v>940</v>
       </c>
       <c r="C149" s="8"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A150" s="18" t="s">
-        <v>746</v>
+        <v>939</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>747</v>
+        <v>941</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A151" s="18" t="s">
-        <v>748</v>
+        <v>942</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>749</v>
+        <v>943</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="18" t="s">
-        <v>750</v>
+        <v>924</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>751</v>
+        <v>324</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="18" t="s">
-        <v>752</v>
+        <v>340</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>753</v>
+        <v>341</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A154" s="17" t="s">
-        <v>754</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>758</v>
-      </c>
+    <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A154" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C154" s="8"/>
+      <c r="D154" s="7"/>
+      <c r="E154" s="7"/>
     </row>
     <row r="155" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A155" s="18" t="s">
-        <v>759</v>
+        <v>344</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>760</v>
+        <v>345</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
     </row>
     <row r="156" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A156" s="17" t="s">
-        <v>761</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>762</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E156" s="3" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A156" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="C156" s="8"/>
+      <c r="D156" s="7"/>
+      <c r="E156" s="7"/>
+    </row>
+    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="18" t="s">
-        <v>766</v>
+        <v>348</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>767</v>
+        <v>349</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="18" t="s">
-        <v>768</v>
+        <v>746</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>769</v>
+        <v>747</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="18" t="s">
-        <v>770</v>
+        <v>748</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>771</v>
+        <v>749</v>
       </c>
       <c r="C159" s="8"/>
       <c r="D159" s="7"/>
@@ -8228,10 +8288,10 @@
     </row>
     <row r="160" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" s="18" t="s">
-        <v>352</v>
+        <v>750</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>353</v>
+        <v>751</v>
       </c>
       <c r="C160" s="8"/>
       <c r="D160" s="7"/>
@@ -8239,173 +8299,155 @@
     </row>
     <row r="161" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="18" t="s">
-        <v>354</v>
+        <v>752</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>355</v>
+        <v>753</v>
       </c>
       <c r="C161" s="8"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
-        <v>356</v>
+        <v>754</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>357</v>
+        <v>755</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>358</v>
+        <v>756</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>359</v>
+        <v>757</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>365</v>
-      </c>
+        <v>758</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A163" s="18" t="s">
+        <v>759</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="C163" s="8"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
     </row>
     <row r="164" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A164" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="B164" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C164" s="8"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="7"/>
-    </row>
-    <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" s="17" t="s">
-        <v>368</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="B166" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D167" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E167" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D168" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A164" s="17" t="s">
+        <v>761</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A165" s="18" t="s">
+        <v>766</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>767</v>
+      </c>
+      <c r="C165" s="8"/>
+      <c r="D165" s="7"/>
+      <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A166" s="18" t="s">
+        <v>768</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="C166" s="8"/>
+      <c r="D166" s="7"/>
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A167" s="18" t="s">
+        <v>770</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="C167" s="8"/>
+      <c r="D167" s="7"/>
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A168" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C168" s="8"/>
+      <c r="D168" s="7"/>
+      <c r="E168" s="7"/>
+    </row>
+    <row r="169" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" s="18" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
     </row>
     <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A170" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="B170" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C170" s="8"/>
-      <c r="D170" s="7"/>
-      <c r="E170" s="7"/>
+      <c r="A170" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
-        <v>772</v>
+        <v>361</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>173</v>
+        <v>362</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>174</v>
+        <v>363</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>175</v>
+        <v>364</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" s="18" t="s">
-        <v>773</v>
+        <v>366</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>774</v>
+        <v>171</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -8413,138 +8455,156 @@
     </row>
     <row r="173" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>775</v>
+        <v>368</v>
       </c>
       <c r="B173" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A174" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="B174" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C173" s="3" t="s">
+      <c r="C174" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D173" s="3" t="s">
+      <c r="D174" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E173" s="3" t="s">
+      <c r="E174" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A174" s="18" t="s">
-        <v>776</v>
-      </c>
-      <c r="B174" s="9" t="s">
-        <v>777</v>
-      </c>
-      <c r="C174" s="8"/>
-      <c r="D174" s="7"/>
-      <c r="E174" s="7"/>
-    </row>
     <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="18" t="s">
-        <v>778</v>
-      </c>
-      <c r="B175" s="9" t="s">
-        <v>779</v>
-      </c>
-      <c r="C175" s="8"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="7"/>
+      <c r="A175" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A176" s="18" t="s">
-        <v>780</v>
-      </c>
-      <c r="B176" s="9" t="s">
-        <v>781</v>
-      </c>
-      <c r="C176" s="8"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="7"/>
+      <c r="A176" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="18" t="s">
-        <v>782</v>
+        <v>372</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>783</v>
+        <v>373</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="18" t="s">
-        <v>784</v>
+        <v>374</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>785</v>
+        <v>375</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A179" s="18" t="s">
-        <v>786</v>
-      </c>
-      <c r="B179" s="9" t="s">
-        <v>787</v>
-      </c>
-      <c r="C179" s="8"/>
-      <c r="D179" s="7"/>
-      <c r="E179" s="7"/>
+    <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A179" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A180" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D180" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E180" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A180" s="18" t="s">
+        <v>773</v>
+      </c>
+      <c r="B180" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="C180" s="8"/>
+      <c r="D180" s="7"/>
+      <c r="E180" s="7"/>
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A181" s="18" t="s">
-        <v>788</v>
-      </c>
-      <c r="B181" s="9" t="s">
-        <v>789</v>
-      </c>
-      <c r="C181" s="8"/>
-      <c r="D181" s="7"/>
-      <c r="E181" s="7"/>
+      <c r="A181" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A182" s="17" t="s">
-        <v>790</v>
-      </c>
-      <c r="B182" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D182" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E182" s="3" t="s">
-        <v>309</v>
-      </c>
+      <c r="A182" s="18" t="s">
+        <v>776</v>
+      </c>
+      <c r="B182" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="C182" s="8"/>
+      <c r="D182" s="7"/>
+      <c r="E182" s="7"/>
     </row>
     <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="18" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>792</v>
+        <v>779</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="7"/>
@@ -8552,10 +8612,10 @@
     </row>
     <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="18" t="s">
-        <v>793</v>
+        <v>780</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>794</v>
+        <v>781</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
@@ -8563,121 +8623,121 @@
     </row>
     <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="18" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A186" s="18" t="s">
-        <v>797</v>
+        <v>784</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>798</v>
+        <v>785</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" s="18" t="s">
-        <v>799</v>
+        <v>786</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>395</v>
+        <v>787</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
     <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A188" s="18" t="s">
-        <v>800</v>
-      </c>
-      <c r="B188" s="9" t="s">
-        <v>801</v>
-      </c>
-      <c r="C188" s="8"/>
-      <c r="D188" s="7"/>
-      <c r="E188" s="7"/>
+      <c r="A188" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="18" t="s">
-        <v>802</v>
+        <v>788</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>803</v>
+        <v>789</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
     <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A190" s="18" t="s">
-        <v>804</v>
-      </c>
-      <c r="B190" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="C190" s="8"/>
-      <c r="D190" s="7"/>
-      <c r="E190" s="7"/>
-    </row>
-    <row r="191" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A190" s="17" t="s">
+        <v>790</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="18" t="s">
-        <v>381</v>
+        <v>791</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>382</v>
+        <v>792</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
     <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A192" s="17" t="s">
-        <v>383</v>
-      </c>
-      <c r="B192" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E192" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A192" s="18" t="s">
+        <v>793</v>
+      </c>
+      <c r="B192" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="C192" s="8"/>
+      <c r="D192" s="7"/>
+      <c r="E192" s="7"/>
     </row>
     <row r="193" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A193" s="17" t="s">
-        <v>806</v>
-      </c>
-      <c r="B193" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A193" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="B193" s="9" t="s">
+        <v>796</v>
+      </c>
+      <c r="C193" s="8"/>
+      <c r="D193" s="7"/>
+      <c r="E193" s="7"/>
     </row>
     <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" s="18" t="s">
-        <v>807</v>
+        <v>797</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="7"/>
@@ -8685,21 +8745,21 @@
     </row>
     <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="18" t="s">
-        <v>809</v>
+        <v>799</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>810</v>
+        <v>395</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="18" t="s">
-        <v>384</v>
+        <v>800</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="7"/>
@@ -8707,10 +8767,10 @@
     </row>
     <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="18" t="s">
-        <v>386</v>
+        <v>802</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>387</v>
+        <v>803</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
@@ -8718,54 +8778,66 @@
     </row>
     <row r="198" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="18" t="s">
-        <v>388</v>
+        <v>804</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>389</v>
+        <v>805</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
     </row>
-    <row r="199" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A199" s="18" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A200" s="18" t="s">
-        <v>392</v>
-      </c>
-      <c r="B200" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="C200" s="8"/>
-      <c r="D200" s="7"/>
-      <c r="E200" s="7"/>
+    <row r="200" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A200" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A201" s="18" t="s">
-        <v>394</v>
-      </c>
-      <c r="B201" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="C201" s="8"/>
-      <c r="D201" s="7"/>
-      <c r="E201" s="7"/>
-    </row>
-    <row r="202" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A201" s="17" t="s">
+        <v>806</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="18" t="s">
-        <v>396</v>
+        <v>807</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>397</v>
+        <v>808</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
@@ -8773,54 +8845,54 @@
     </row>
     <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="18" t="s">
-        <v>398</v>
+        <v>809</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>399</v>
+        <v>810</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
       <c r="E203" s="7"/>
     </row>
-    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>401</v>
+        <v>811</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
     </row>
-    <row r="205" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>812</v>
+        <v>386</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>813</v>
+        <v>387</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
     </row>
-    <row r="206" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>814</v>
+        <v>388</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>815</v>
+        <v>389</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="7"/>
       <c r="E206" s="7"/>
     </row>
-    <row r="207" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A207" s="18" t="s">
-        <v>816</v>
+        <v>390</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>817</v>
+        <v>391</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="7"/>
@@ -8828,7 +8900,7 @@
     </row>
     <row r="208" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" s="18" t="s">
-        <v>818</v>
+        <v>392</v>
       </c>
       <c r="B208" s="9" t="s">
         <v>393</v>
@@ -8837,12 +8909,12 @@
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
     </row>
-    <row r="209" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="18" t="s">
-        <v>819</v>
+        <v>394</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>820</v>
+        <v>395</v>
       </c>
       <c r="C209" s="8"/>
       <c r="D209" s="7"/>
@@ -8850,7 +8922,7 @@
     </row>
     <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="18" t="s">
-        <v>821</v>
+        <v>396</v>
       </c>
       <c r="B210" s="9" t="s">
         <v>397</v>
@@ -8859,244 +8931,250 @@
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
     </row>
-    <row r="211" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="18" t="s">
-        <v>822</v>
+        <v>398</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>823</v>
+        <v>399</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
     </row>
-    <row r="212" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="18" t="s">
-        <v>824</v>
+        <v>400</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>825</v>
+        <v>401</v>
       </c>
       <c r="C212" s="8"/>
       <c r="D212" s="7"/>
       <c r="E212" s="7"/>
     </row>
-    <row r="213" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A213" s="18" t="s">
-        <v>402</v>
+        <v>812</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>403</v>
+        <v>813</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="7"/>
       <c r="E213" s="7"/>
     </row>
-    <row r="214" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A214" s="18" t="s">
-        <v>404</v>
+        <v>814</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>405</v>
+        <v>815</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="7"/>
       <c r="E214" s="7"/>
     </row>
-    <row r="215" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A215" s="17" t="s">
-        <v>406</v>
-      </c>
-      <c r="B215" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="D215" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E215" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A216" s="17" t="s">
-        <v>411</v>
-      </c>
-      <c r="B216" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D216" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="E216" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A215" s="18" t="s">
+        <v>816</v>
+      </c>
+      <c r="B215" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="C215" s="8"/>
+      <c r="D215" s="7"/>
+      <c r="E215" s="7"/>
+    </row>
+    <row r="216" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A216" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="B216" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C216" s="8"/>
+      <c r="D216" s="7"/>
+      <c r="E216" s="7"/>
+    </row>
+    <row r="217" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A217" s="18" t="s">
-        <v>913</v>
-      </c>
-      <c r="B217" s="4" t="s">
-        <v>914</v>
-      </c>
-      <c r="D217" s="3"/>
-      <c r="E217" s="3"/>
-    </row>
-    <row r="218" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>819</v>
+      </c>
+      <c r="B217" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="C217" s="8"/>
+      <c r="D217" s="7"/>
+      <c r="E217" s="7"/>
+    </row>
+    <row r="218" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A218" s="18" t="s">
-        <v>415</v>
+        <v>821</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="C218" s="8"/>
       <c r="D218" s="7"/>
       <c r="E218" s="7"/>
     </row>
-    <row r="219" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A219" s="17" t="s">
-        <v>417</v>
-      </c>
-      <c r="B219" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D219" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="E219" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A219" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="B219" s="9" t="s">
+        <v>823</v>
+      </c>
+      <c r="C219" s="8"/>
+      <c r="D219" s="7"/>
+      <c r="E219" s="7"/>
+    </row>
+    <row r="220" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A220" s="18" t="s">
-        <v>422</v>
+        <v>824</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>423</v>
+        <v>825</v>
       </c>
       <c r="C220" s="8"/>
       <c r="D220" s="7"/>
       <c r="E220" s="7"/>
     </row>
-    <row r="221" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A221" s="18" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
       <c r="C221" s="8"/>
       <c r="D221" s="7"/>
       <c r="E221" s="7"/>
     </row>
-    <row r="222" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A222" s="17" t="s">
-        <v>826</v>
-      </c>
-      <c r="B222" s="4" t="s">
-        <v>827</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>828</v>
-      </c>
-      <c r="D222" s="3" t="s">
-        <v>829</v>
-      </c>
-      <c r="E222" s="3" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A223" s="18" t="s">
-        <v>426</v>
-      </c>
-      <c r="B223" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="C223" s="8"/>
-      <c r="D223" s="7"/>
-      <c r="E223" s="7"/>
-    </row>
-    <row r="224" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A224" s="18" t="s">
-        <v>428</v>
-      </c>
-      <c r="B224" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="C224" s="8"/>
-      <c r="D224" s="7"/>
-      <c r="E224" s="7"/>
-    </row>
-    <row r="225" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A225" s="18" t="s">
-        <v>429</v>
-      </c>
-      <c r="B225" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="C225" s="8"/>
-      <c r="D225" s="7"/>
-      <c r="E225" s="7"/>
+    <row r="222" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A222" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="B222" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C222" s="8"/>
+      <c r="D222" s="7"/>
+      <c r="E222" s="7"/>
+    </row>
+    <row r="223" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A223" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A224" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A225" s="17" t="s">
+        <v>944</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="226" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A226" s="18" t="s">
-        <v>431</v>
-      </c>
-      <c r="B226" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="C226" s="8"/>
-      <c r="D226" s="7"/>
-      <c r="E226" s="7"/>
+      <c r="A226" s="17" t="s">
+        <v>945</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>947</v>
+      </c>
     </row>
     <row r="227" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A227" s="18" t="s">
-        <v>432</v>
-      </c>
-      <c r="B227" s="9" t="s">
-        <v>405</v>
-      </c>
-      <c r="C227" s="8"/>
-      <c r="D227" s="7"/>
-      <c r="E227" s="7"/>
-    </row>
-    <row r="228" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>913</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="D227" s="3"/>
+      <c r="E227" s="3"/>
+    </row>
+    <row r="228" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A228" s="18" t="s">
-        <v>831</v>
+        <v>415</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C228" s="8"/>
       <c r="D228" s="7"/>
       <c r="E228" s="7"/>
     </row>
-    <row r="229" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A229" s="18" t="s">
-        <v>832</v>
-      </c>
-      <c r="B229" s="9" t="s">
-        <v>833</v>
-      </c>
-      <c r="C229" s="8"/>
-      <c r="D229" s="7"/>
-      <c r="E229" s="7"/>
+    <row r="229" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A229" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="230" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A230" s="18" t="s">
-        <v>834</v>
+        <v>422</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>835</v>
+        <v>423</v>
       </c>
       <c r="C230" s="8"/>
       <c r="D230" s="7"/>
@@ -9104,33 +9182,149 @@
     </row>
     <row r="231" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A231" s="18" t="s">
-        <v>836</v>
+        <v>424</v>
       </c>
       <c r="B231" s="9" t="s">
-        <v>837</v>
+        <v>425</v>
       </c>
       <c r="C231" s="8"/>
       <c r="D231" s="7"/>
       <c r="E231" s="7"/>
     </row>
-    <row r="232" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A232" s="17" t="s">
+        <v>826</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A233" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="B233" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C233" s="8"/>
+      <c r="D233" s="7"/>
+      <c r="E233" s="7"/>
+    </row>
+    <row r="234" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A234" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="B234" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C234" s="8"/>
+      <c r="D234" s="7"/>
+      <c r="E234" s="7"/>
+    </row>
+    <row r="235" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A235" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="B235" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C235" s="8"/>
+      <c r="D235" s="7"/>
+      <c r="E235" s="7"/>
+    </row>
+    <row r="236" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A236" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="B236" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C236" s="8"/>
+      <c r="D236" s="7"/>
+      <c r="E236" s="7"/>
+    </row>
+    <row r="237" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A237" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="B237" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C237" s="8"/>
+      <c r="D237" s="7"/>
+      <c r="E237" s="7"/>
+    </row>
+    <row r="238" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A238" s="18" t="s">
+        <v>831</v>
+      </c>
+      <c r="B238" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C238" s="8"/>
+      <c r="D238" s="7"/>
+      <c r="E238" s="7"/>
+    </row>
+    <row r="239" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A239" s="18" t="s">
+        <v>832</v>
+      </c>
+      <c r="B239" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="C239" s="8"/>
+      <c r="D239" s="7"/>
+      <c r="E239" s="7"/>
+    </row>
+    <row r="240" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A240" s="18" t="s">
+        <v>834</v>
+      </c>
+      <c r="B240" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="C240" s="8"/>
+      <c r="D240" s="7"/>
+      <c r="E240" s="7"/>
+    </row>
+    <row r="241" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A241" s="18" t="s">
+        <v>836</v>
+      </c>
+      <c r="B241" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C241" s="8"/>
+      <c r="D241" s="7"/>
+      <c r="E241" s="7"/>
+    </row>
+    <row r="242" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A242" s="17" t="s">
         <v>876</v>
       </c>
-      <c r="B232" s="15" t="s">
+      <c r="B242" s="15" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A233" s="17" t="s">
+    <row r="243" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A243" s="17" t="s">
         <v>877</v>
       </c>
-      <c r="B233" s="4" t="s">
+      <c r="B243" s="4" t="s">
         <v>893</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E231" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E241" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(determinants): drinking water map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED9C6D5-02E2-2146-A8DE-4946BAD755FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6982E49-41B3-904D-8B5B-5AE9FBB014B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="990">
   <si>
     <t>LABEL</t>
   </si>
@@ -3006,6 +3006,24 @@
   </si>
   <si>
     <t>Cobertura &gt;95%</t>
+  </si>
+  <si>
+    <t>determinants_drinking_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceso a agua potable </t>
+  </si>
+  <si>
+    <t>determinants_population_legend</t>
+  </si>
+  <si>
+    <t>% de la población</t>
+  </si>
+  <si>
+    <t>Proporción de la población con acceso a servicios básicos de agua potable</t>
+  </si>
+  <si>
+    <t>determinants_title_map_water</t>
   </si>
 </sst>
 </file>
@@ -6263,10 +6281,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E259"/>
+  <dimension ref="A1:E262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B259" sqref="B259"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C257" sqref="C257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9563,6 +9581,30 @@
       </c>
       <c r="B259" s="4" t="s">
         <v>983</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>984</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>986</v>
+      </c>
+      <c r="B261" s="4" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>989</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(determinants): sanitation services map
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6982E49-41B3-904D-8B5B-5AE9FBB014B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E74BAA-D830-724E-90FE-225F8FEBAADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="994">
   <si>
     <t>LABEL</t>
   </si>
@@ -3020,10 +3020,22 @@
     <t>% de la población</t>
   </si>
   <si>
-    <t>Proporción de la población con acceso a servicios básicos de agua potable</t>
-  </si>
-  <si>
     <t>determinants_title_map_water</t>
+  </si>
+  <si>
+    <t>determinants_sanitation_services</t>
+  </si>
+  <si>
+    <t>Acceso a servicios básicos de saneamiento</t>
+  </si>
+  <si>
+    <t>determinants_title_map_sanitation</t>
+  </si>
+  <si>
+    <t>Población con acceso a servicios básicos de agua potable</t>
+  </si>
+  <si>
+    <t>Población con acceso a servicios básicos de saneamiento</t>
   </si>
 </sst>
 </file>
@@ -6281,10 +6293,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E262"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A250" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257"/>
+      <selection activeCell="B264" sqref="B264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9599,12 +9611,28 @@
         <v>987</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
+        <v>988</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
         <v>989</v>
       </c>
-      <c r="B262" s="4" t="s">
-        <v>988</v>
+      <c r="B263" s="4" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>991</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(outbreaks): complete section working
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5261F3-7847-934F-881C-2E04BB722DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359AD1E0-B9BA-5040-B82B-414505A33B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="MSG" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$248</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$247</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="1003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="1033">
   <si>
     <t>LABEL</t>
   </si>
@@ -3063,6 +3063,96 @@
   </si>
   <si>
     <t>Búsquedas activas realizadas</t>
+  </si>
+  <si>
+    <t>outbreaks_title</t>
+  </si>
+  <si>
+    <t>outbreaks_title_map_total_pr</t>
+  </si>
+  <si>
+    <t>Evaluación de riesgo para los casos y brotes de EPV</t>
+  </si>
+  <si>
+    <t>outbreaks_title_map_disease</t>
+  </si>
+  <si>
+    <t>Presencia de brotes de</t>
+  </si>
+  <si>
+    <t>outbreaks_polio</t>
+  </si>
+  <si>
+    <t>outbreaks_polio_score</t>
+  </si>
+  <si>
+    <t>outbreaks_measles</t>
+  </si>
+  <si>
+    <t>outbreaks_measles_score</t>
+  </si>
+  <si>
+    <t>outbreaks_rubella</t>
+  </si>
+  <si>
+    <t>outbreaks_rubella_score</t>
+  </si>
+  <si>
+    <t>outbreaks_diphtheria</t>
+  </si>
+  <si>
+    <t>outbreaks_diphtheria_score</t>
+  </si>
+  <si>
+    <t>outbreaks_yellow_fever</t>
+  </si>
+  <si>
+    <t>outbreaks_yellow_fever_score</t>
+  </si>
+  <si>
+    <t>outbreaks_tetanus</t>
+  </si>
+  <si>
+    <t>outbreaks_tetanus_score</t>
+  </si>
+  <si>
+    <t>Polio</t>
+  </si>
+  <si>
+    <t>Puntaje polio</t>
+  </si>
+  <si>
+    <t>Sarampión</t>
+  </si>
+  <si>
+    <t>Puntaje Sarampión</t>
+  </si>
+  <si>
+    <t>Rubéola</t>
+  </si>
+  <si>
+    <t>Puntaje Rubéola</t>
+  </si>
+  <si>
+    <t>Difteria</t>
+  </si>
+  <si>
+    <t>Puntaje Difteria</t>
+  </si>
+  <si>
+    <t>Fiebre amarilla</t>
+  </si>
+  <si>
+    <t>Puntaje Fiebre amarilla</t>
+  </si>
+  <si>
+    <t>Tétanos neonatal</t>
+  </si>
+  <si>
+    <t>Puntaje tétanos neonatal</t>
+  </si>
+  <si>
+    <t>outbreaks_disease_legend</t>
   </si>
 </sst>
 </file>
@@ -3165,7 +3255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3208,6 +3298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6320,10 +6411,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
-  <dimension ref="A1:E268"/>
+  <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D268" sqref="D268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6960,127 +7051,128 @@
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>863</v>
+        <v>629</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>864</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+        <v>630</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>630</v>
+        <v>582</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>631</v>
+        <v>583</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>632</v>
+        <v>584</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>633</v>
+        <v>585</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>634</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>582</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>585</v>
-      </c>
+      <c r="A45" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>636</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A46" t="s">
         <v>637</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+    <row r="47" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
         <v>638</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>640</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>641</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="E50" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="7"/>
@@ -7088,21 +7180,21 @@
     </row>
     <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="7"/>
@@ -7110,145 +7202,145 @@
     </row>
     <row r="54" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
-        <v>650</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>652</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>653</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>654</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>657</v>
-      </c>
+      <c r="A57" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
+      <c r="A58" t="s">
+        <v>301</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>891</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>891</v>
+        <v>999</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>999</v>
+        <v>890</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>890</v>
+        <v>57</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>304</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A62" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>658</v>
+        <v>98</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>659</v>
+        <v>99</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="7"/>
@@ -7256,10 +7348,10 @@
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="7"/>
@@ -7267,149 +7359,149 @@
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>61</v>
+        <v>660</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="7" t="s">
-        <v>660</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
+      <c r="A66" t="s">
+        <v>272</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>273</v>
+        <v>661</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>274</v>
+        <v>662</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>275</v>
+        <v>663</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>276</v>
+        <v>664</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>277</v>
+      <c r="A68" s="7" t="s">
+        <v>899</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>661</v>
+        <v>1000</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>662</v>
+        <v>1000</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>664</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
-        <v>899</v>
+      <c r="A69" t="s">
+        <v>282</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>1000</v>
+        <v>283</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>1000</v>
+        <v>284</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E69" s="3"/>
+        <v>285</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>296</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>300</v>
-      </c>
+      <c r="A73" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="7"/>
@@ -7417,133 +7509,133 @@
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
-        <v>669</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>670</v>
-      </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
+      <c r="A76" t="s">
+        <v>305</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>305</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>309</v>
-      </c>
+      <c r="A77" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>671</v>
-      </c>
-      <c r="C78" s="8"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-    </row>
-    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="A78" t="s">
         <v>311</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
-        <v>674</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>675</v>
-      </c>
-      <c r="C81" s="8"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
+      <c r="A81" t="s">
+        <v>676</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>582</v>
+        <v>678</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>583</v>
+        <v>679</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>584</v>
+        <v>680</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>585</v>
+        <v>681</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>677</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>678</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>681</v>
-      </c>
+      <c r="A83" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="7"/>
@@ -7551,10 +7643,10 @@
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="7"/>
@@ -7562,10 +7654,10 @@
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="7"/>
@@ -7573,10 +7665,10 @@
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="7"/>
@@ -7584,10 +7676,10 @@
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="7"/>
@@ -7595,10 +7687,10 @@
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="7"/>
@@ -7606,10 +7698,10 @@
     </row>
     <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="7"/>
@@ -7617,10 +7709,10 @@
     </row>
     <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="C91" s="8"/>
       <c r="D91" s="7"/>
@@ -7628,76 +7720,76 @@
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>702</v>
+        <v>878</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>703</v>
+        <v>894</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>894</v>
+        <v>885</v>
       </c>
       <c r="C95" s="8"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-    </row>
-    <row r="96" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>885</v>
+        <v>895</v>
       </c>
       <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
     </row>
     <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>879</v>
+        <v>886</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>887</v>
+        <v>896</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="7"/>
@@ -7705,32 +7797,32 @@
     </row>
     <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>880</v>
+        <v>888</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>898</v>
+        <v>883</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="7"/>
@@ -7738,10 +7830,10 @@
     </row>
     <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>882</v>
+        <v>904</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>883</v>
+        <v>1001</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="7"/>
@@ -7749,116 +7841,116 @@
     </row>
     <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
-        <v>904</v>
+        <v>950</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>1001</v>
+        <v>951</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
-        <v>952</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>953</v>
-      </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>704</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>705</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>143</v>
-      </c>
+      <c r="A107" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>707</v>
+      </c>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
     </row>
     <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="8"/>
     </row>
     <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
-        <v>708</v>
-      </c>
-      <c r="B109" s="9" t="s">
-        <v>709</v>
-      </c>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
+      <c r="A109" t="s">
+        <v>710</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>710</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>711</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>712</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>713</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>716</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+    </row>
+    <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -7866,10 +7958,10 @@
     </row>
     <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
@@ -7877,122 +7969,122 @@
     </row>
     <row r="113" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>719</v>
+        <v>316</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>720</v>
+        <v>317</v>
       </c>
       <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
     </row>
     <row r="114" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="C114" s="8"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-    </row>
-    <row r="115" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="A114" t="s">
         <v>318</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D114" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="E114" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
+    <row r="115" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A115" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B115" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C116" s="8"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+    </row>
+    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>721</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>721</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
+      <c r="A117" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B117" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C118" s="8"/>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
-    </row>
-    <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="C117" s="8"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>722</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>130</v>
+        <v>724</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>131</v>
+        <v>725</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>132</v>
+        <v>726</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>723</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="E120" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A120" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>729</v>
+      </c>
+      <c r="C120" s="8"/>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
-        <v>728</v>
+        <v>350</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>729</v>
+        <v>351</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="7"/>
@@ -8000,10 +8092,10 @@
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>350</v>
+        <v>730</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>351</v>
+        <v>731</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
@@ -8011,10 +8103,10 @@
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>731</v>
+        <v>595</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
@@ -8022,10 +8114,10 @@
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>732</v>
+        <v>321</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>595</v>
+        <v>322</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="7"/>
@@ -8033,10 +8125,10 @@
     </row>
     <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="7"/>
@@ -8044,94 +8136,94 @@
     </row>
     <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>323</v>
+        <v>733</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>324</v>
+        <v>734</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="7" t="s">
-        <v>733</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>734</v>
-      </c>
-      <c r="C127" s="8"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
-    </row>
-    <row r="128" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>327</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>735</v>
+        <v>330</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>331</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>742</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="E130" s="3" t="s">
-        <v>744</v>
-      </c>
+      <c r="A130" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>745</v>
+      </c>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
     </row>
     <row r="131" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>745</v>
+        <v>336</v>
       </c>
       <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
-    </row>
-    <row r="132" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+    </row>
+    <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="7"/>
@@ -8139,43 +8231,43 @@
     </row>
     <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
-        <v>339</v>
+        <v>906</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>324</v>
+        <v>905</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="7"/>
@@ -8183,10 +8275,10 @@
     </row>
     <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>909</v>
+        <v>954</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>910</v>
+        <v>955</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
@@ -8194,32 +8286,32 @@
     </row>
     <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>954</v>
+        <v>913</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>955</v>
+        <v>910</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
@@ -8227,43 +8319,43 @@
     </row>
     <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
-        <v>916</v>
+        <v>965</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>917</v>
+        <v>956</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="7"/>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
-        <v>965</v>
+        <v>918</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>956</v>
+        <v>919</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="7"/>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
@@ -8271,153 +8363,153 @@
     </row>
     <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
-        <v>923</v>
+        <v>957</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>925</v>
+        <v>958</v>
       </c>
       <c r="C145" s="8"/>
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
-        <v>957</v>
+        <v>924</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>958</v>
+        <v>926</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="C147" s="8"/>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
-        <v>927</v>
+        <v>959</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>929</v>
+        <v>960</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
-        <v>959</v>
+        <v>931</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>960</v>
+        <v>341</v>
       </c>
       <c r="C149" s="8"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>341</v>
+        <v>930</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
-        <v>932</v>
+        <v>962</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>934</v>
+        <v>961</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
-        <v>962</v>
+        <v>933</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>961</v>
+        <v>935</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>935</v>
+        <v>1002</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
-        <v>936</v>
+        <v>963</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>1002</v>
+        <v>964</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
-        <v>963</v>
+        <v>937</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>964</v>
+        <v>938</v>
       </c>
       <c r="C156" s="8"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
-        <v>939</v>
+        <v>922</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>940</v>
+        <v>324</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="7"/>
@@ -8425,10 +8517,10 @@
     </row>
     <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
-        <v>922</v>
+        <v>340</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="C159" s="8"/>
       <c r="D159" s="7"/>
@@ -8436,21 +8528,21 @@
     </row>
     <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="7" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C160" s="8"/>
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C161" s="8"/>
       <c r="D161" s="7"/>
@@ -8458,21 +8550,21 @@
     </row>
     <row r="162" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C162" s="8"/>
       <c r="D162" s="7"/>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="7"/>
@@ -8480,10 +8572,10 @@
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>348</v>
+        <v>746</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>349</v>
+        <v>747</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="7"/>
@@ -8491,21 +8583,21 @@
     </row>
     <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="7"/>
@@ -8513,77 +8605,77 @@
     </row>
     <row r="167" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="7"/>
       <c r="E167" s="7"/>
     </row>
     <row r="168" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A168" s="7" t="s">
-        <v>752</v>
-      </c>
-      <c r="B168" s="9" t="s">
-        <v>753</v>
-      </c>
-      <c r="C168" s="8"/>
-      <c r="D168" s="7"/>
-      <c r="E168" s="7"/>
+      <c r="A168" t="s">
+        <v>754</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="169" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>754</v>
-      </c>
-      <c r="B169" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D169" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>758</v>
-      </c>
+      <c r="A169" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="C169" s="8"/>
+      <c r="D169" s="7"/>
+      <c r="E169" s="7"/>
     </row>
     <row r="170" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A170" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="B170" s="9" t="s">
-        <v>760</v>
-      </c>
-      <c r="C170" s="8"/>
-      <c r="D170" s="7"/>
-      <c r="E170" s="7"/>
+      <c r="A170" t="s">
+        <v>761</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="171" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>761</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>762</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>765</v>
-      </c>
+      <c r="A171" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>767</v>
+      </c>
+      <c r="C171" s="8"/>
+      <c r="D171" s="7"/>
+      <c r="E171" s="7"/>
     </row>
     <row r="172" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -8591,10 +8683,10 @@
     </row>
     <row r="173" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C173" s="8"/>
       <c r="D173" s="7"/>
@@ -8602,10 +8694,10 @@
     </row>
     <row r="174" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>770</v>
+        <v>352</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>771</v>
+        <v>353</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="7"/>
@@ -8613,212 +8705,212 @@
     </row>
     <row r="175" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C175" s="8"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A176" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="B176" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="C176" s="8"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="7"/>
+    <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>356</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="177" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>361</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E178" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A179" s="7" t="s">
+    <row r="178" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A178" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="B179" s="9" t="s">
+      <c r="B178" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C179" s="8"/>
-      <c r="D179" s="7"/>
-      <c r="E179" s="7"/>
+      <c r="C178" s="8"/>
+      <c r="D178" s="7"/>
+      <c r="E178" s="7"/>
+    </row>
+    <row r="179" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>368</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="180" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>371</v>
-      </c>
-      <c r="B183" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E183" s="3" t="s">
-        <v>191</v>
-      </c>
+      <c r="A183" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B183" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="C183" s="8"/>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
     </row>
     <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
     <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A185" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="B185" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C185" s="8"/>
-      <c r="D185" s="7"/>
-      <c r="E185" s="7"/>
+      <c r="A185" t="s">
+        <v>772</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
-        <v>772</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="A186" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="B186" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="C186" s="8"/>
+      <c r="D186" s="7"/>
+      <c r="E186" s="7"/>
     </row>
     <row r="187" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A187" s="7" t="s">
-        <v>773</v>
-      </c>
-      <c r="B187" s="9" t="s">
-        <v>774</v>
-      </c>
-      <c r="C187" s="8"/>
-      <c r="D187" s="7"/>
-      <c r="E187" s="7"/>
+      <c r="A187" t="s">
+        <v>775</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>775</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>181</v>
-      </c>
+      <c r="A188" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="B188" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="C188" s="8"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7"/>
     </row>
     <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
@@ -8826,10 +8918,10 @@
     </row>
     <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
@@ -8837,21 +8929,21 @@
     </row>
     <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
@@ -8859,77 +8951,77 @@
     </row>
     <row r="193" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A194" s="7" t="s">
-        <v>786</v>
-      </c>
-      <c r="B194" s="9" t="s">
-        <v>787</v>
-      </c>
-      <c r="C194" s="8"/>
-      <c r="D194" s="7"/>
-      <c r="E194" s="7"/>
+    <row r="194" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>376</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>376</v>
-      </c>
-      <c r="B195" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A195" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="B195" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="C195" s="8"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="7"/>
     </row>
     <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" s="7" t="s">
-        <v>788</v>
-      </c>
-      <c r="B196" s="9" t="s">
-        <v>789</v>
-      </c>
-      <c r="C196" s="8"/>
-      <c r="D196" s="7"/>
-      <c r="E196" s="7"/>
+      <c r="A196" t="s">
+        <v>790</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
-        <v>790</v>
-      </c>
-      <c r="B197" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E197" s="3" t="s">
-        <v>309</v>
-      </c>
+      <c r="A197" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="B197" s="9" t="s">
+        <v>792</v>
+      </c>
+      <c r="C197" s="8"/>
+      <c r="D197" s="7"/>
+      <c r="E197" s="7"/>
     </row>
     <row r="198" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
@@ -8937,10 +9029,10 @@
     </row>
     <row r="199" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
@@ -8948,10 +9040,10 @@
     </row>
     <row r="200" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
@@ -8959,10 +9051,10 @@
     </row>
     <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>798</v>
+        <v>395</v>
       </c>
       <c r="C201" s="8"/>
       <c r="D201" s="7"/>
@@ -8970,10 +9062,10 @@
     </row>
     <row r="202" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>395</v>
+        <v>801</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
@@ -8981,10 +9073,10 @@
     </row>
     <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
@@ -8992,40 +9084,46 @@
     </row>
     <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="7" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
     </row>
-    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
-        <v>804</v>
+        <v>381</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>805</v>
+        <v>382</v>
       </c>
       <c r="C205" s="8"/>
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
     </row>
-    <row r="206" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A206" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="B206" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="C206" s="8"/>
-      <c r="D206" s="7"/>
-      <c r="E206" s="7"/>
+    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>383</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="207" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>383</v>
+        <v>806</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>377</v>
@@ -9041,50 +9139,44 @@
       </c>
     </row>
     <row r="208" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>806</v>
-      </c>
-      <c r="B208" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D208" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E208" s="3" t="s">
-        <v>380</v>
-      </c>
+      <c r="A208" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="B208" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="C208" s="8"/>
+      <c r="D208" s="7"/>
+      <c r="E208" s="7"/>
     </row>
     <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="C209" s="8"/>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
     </row>
-    <row r="210" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="7" t="s">
-        <v>809</v>
+        <v>384</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C210" s="8"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
     </row>
-    <row r="211" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>811</v>
+        <v>387</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="7"/>
@@ -9092,65 +9184,65 @@
     </row>
     <row r="212" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="7" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C212" s="8"/>
       <c r="D212" s="7"/>
       <c r="E212" s="7"/>
     </row>
-    <row r="213" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A213" s="7" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="7"/>
       <c r="E213" s="7"/>
     </row>
-    <row r="214" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A214" s="7" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="7"/>
       <c r="E214" s="7"/>
     </row>
-    <row r="215" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A215" s="7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C215" s="8"/>
       <c r="D215" s="7"/>
       <c r="E215" s="7"/>
     </row>
-    <row r="216" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C216" s="8"/>
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
     </row>
-    <row r="217" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="7" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C217" s="8"/>
       <c r="D217" s="7"/>
@@ -9158,87 +9250,87 @@
     </row>
     <row r="218" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A218" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C218" s="8"/>
       <c r="D218" s="7"/>
       <c r="E218" s="7"/>
     </row>
-    <row r="219" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A219" s="7" t="s">
-        <v>400</v>
+        <v>812</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>401</v>
+        <v>813</v>
       </c>
       <c r="C219" s="8"/>
       <c r="D219" s="7"/>
       <c r="E219" s="7"/>
     </row>
-    <row r="220" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A220" s="7" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="C220" s="8"/>
       <c r="D220" s="7"/>
       <c r="E220" s="7"/>
     </row>
-    <row r="221" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A221" s="7" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C221" s="8"/>
       <c r="D221" s="7"/>
       <c r="E221" s="7"/>
     </row>
-    <row r="222" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" s="7" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>817</v>
+        <v>393</v>
       </c>
       <c r="C222" s="8"/>
       <c r="D222" s="7"/>
       <c r="E222" s="7"/>
     </row>
-    <row r="223" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A223" s="7" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>393</v>
+        <v>820</v>
       </c>
       <c r="C223" s="8"/>
       <c r="D223" s="7"/>
       <c r="E223" s="7"/>
     </row>
-    <row r="224" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" s="7" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>820</v>
+        <v>397</v>
       </c>
       <c r="C224" s="8"/>
       <c r="D224" s="7"/>
       <c r="E224" s="7"/>
     </row>
-    <row r="225" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A225" s="7" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B225" s="9" t="s">
-        <v>397</v>
+        <v>823</v>
       </c>
       <c r="C225" s="8"/>
       <c r="D225" s="7"/>
@@ -9246,21 +9338,21 @@
     </row>
     <row r="226" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A226" s="7" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B226" s="9" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C226" s="8"/>
       <c r="D226" s="7"/>
       <c r="E226" s="7"/>
     </row>
-    <row r="227" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A227" s="7" t="s">
-        <v>824</v>
+        <v>402</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>825</v>
+        <v>403</v>
       </c>
       <c r="C227" s="8"/>
       <c r="D227" s="7"/>
@@ -9268,177 +9360,177 @@
     </row>
     <row r="228" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A228" s="7" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C228" s="8"/>
       <c r="D228" s="7"/>
       <c r="E228" s="7"/>
     </row>
     <row r="229" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A229" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="B229" s="9" t="s">
-        <v>405</v>
-      </c>
-      <c r="C229" s="8"/>
-      <c r="D229" s="7"/>
-      <c r="E229" s="7"/>
+      <c r="A229" t="s">
+        <v>406</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="230" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>411</v>
+        <v>941</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>412</v>
+        <v>945</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>412</v>
+        <v>946</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>413</v>
+        <v>947</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>414</v>
+        <v>948</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E232" s="3" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A233" t="s">
-        <v>942</v>
+      <c r="A233" s="7" t="s">
+        <v>911</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>943</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>943</v>
-      </c>
-      <c r="D233" s="3" t="s">
-        <v>949</v>
-      </c>
-      <c r="E233" s="3" t="s">
-        <v>944</v>
-      </c>
+        <v>912</v>
+      </c>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
     </row>
     <row r="234" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A234" s="7" t="s">
-        <v>911</v>
-      </c>
-      <c r="B234" s="4" t="s">
-        <v>912</v>
-      </c>
-      <c r="D234" s="3"/>
-      <c r="E234" s="3"/>
+        <v>415</v>
+      </c>
+      <c r="B234" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C234" s="8"/>
+      <c r="D234" s="7"/>
+      <c r="E234" s="7"/>
     </row>
     <row r="235" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A235" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="B235" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="C235" s="8"/>
-      <c r="D235" s="7"/>
-      <c r="E235" s="7"/>
-    </row>
-    <row r="236" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A236" t="s">
+      <c r="A235" t="s">
         <v>417</v>
       </c>
-      <c r="B236" s="4" t="s">
+      <c r="B235" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C236" s="3" t="s">
+      <c r="C235" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D236" s="3" t="s">
+      <c r="D235" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E236" s="3" t="s">
+      <c r="E235" s="3" t="s">
         <v>421</v>
       </c>
+    </row>
+    <row r="236" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A236" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="B236" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C236" s="8"/>
+      <c r="D236" s="7"/>
+      <c r="E236" s="7"/>
     </row>
     <row r="237" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A237" s="7" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C237" s="8"/>
       <c r="D237" s="7"/>
       <c r="E237" s="7"/>
     </row>
-    <row r="238" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A238" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="B238" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="C238" s="8"/>
-      <c r="D238" s="7"/>
-      <c r="E238" s="7"/>
-    </row>
-    <row r="239" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A239" t="s">
+    <row r="238" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
         <v>826</v>
       </c>
-      <c r="B239" s="4" t="s">
+      <c r="B238" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="C239" s="3" t="s">
+      <c r="C238" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D239" s="3" t="s">
+      <c r="D238" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="E239" s="3" t="s">
+      <c r="E238" s="3" t="s">
         <v>830</v>
       </c>
+    </row>
+    <row r="239" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A239" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B239" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C239" s="8"/>
+      <c r="D239" s="7"/>
+      <c r="E239" s="7"/>
     </row>
     <row r="240" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A240" s="7" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C240" s="8"/>
       <c r="D240" s="7"/>
@@ -9446,21 +9538,21 @@
     </row>
     <row r="241" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A241" s="7" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C241" s="8"/>
       <c r="D241" s="7"/>
       <c r="E241" s="7"/>
     </row>
-    <row r="242" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
       <c r="C242" s="8"/>
       <c r="D242" s="7"/>
@@ -9468,21 +9560,21 @@
     </row>
     <row r="243" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A243" s="7" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C243" s="8"/>
       <c r="D243" s="7"/>
       <c r="E243" s="7"/>
     </row>
-    <row r="244" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A244" s="7" t="s">
-        <v>432</v>
+        <v>831</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="C244" s="8"/>
       <c r="D244" s="7"/>
@@ -9490,10 +9582,10 @@
     </row>
     <row r="245" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A245" s="7" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>423</v>
+        <v>833</v>
       </c>
       <c r="C245" s="8"/>
       <c r="D245" s="7"/>
@@ -9501,10 +9593,10 @@
     </row>
     <row r="246" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A246" s="7" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C246" s="8"/>
       <c r="D246" s="7"/>
@@ -9512,190 +9604,315 @@
     </row>
     <row r="247" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A247" s="7" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C247" s="8"/>
       <c r="D247" s="7"/>
       <c r="E247" s="7"/>
     </row>
-    <row r="248" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A248" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="B248" s="9" t="s">
-        <v>837</v>
-      </c>
-      <c r="C248" s="8"/>
-      <c r="D248" s="7"/>
-      <c r="E248" s="7"/>
-    </row>
-    <row r="249" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>876</v>
+      </c>
+      <c r="B248" s="15" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>876</v>
-      </c>
-      <c r="B249" s="15" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>877</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>877</v>
+        <v>966</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>893</v>
+        <v>967</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>969</v>
+        <v>996</v>
       </c>
     </row>
     <row r="253" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A254" t="s">
-        <v>971</v>
-      </c>
-      <c r="B254" s="4" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="255" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A255" s="7" t="s">
+    <row r="254" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A254" s="7" t="s">
         <v>972</v>
       </c>
-      <c r="B255" s="9" t="s">
+      <c r="B254" s="9" t="s">
         <v>998</v>
       </c>
+    </row>
+    <row r="255" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>861</v>
+      </c>
+      <c r="B255" s="4" t="s">
+        <v>870</v>
+      </c>
+      <c r="D255" s="3"/>
+      <c r="E255" s="3"/>
     </row>
     <row r="256" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>861</v>
+        <v>973</v>
       </c>
       <c r="B256" s="4" t="s">
         <v>870</v>
       </c>
-      <c r="D256" s="3"/>
-      <c r="E256" s="3"/>
-    </row>
-    <row r="257" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="257" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>986</v>
+        <v>992</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>989</v>
+        <v>994</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>990</v>
+        <v>863</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>991</v>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B269" s="4" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B270" s="4" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B275" s="4" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B276" s="4" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B277" s="4" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B279" s="4" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B282" s="4" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B283" s="4" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A284" s="16" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B284" s="4" t="s">
+        <v>1007</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E248" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
+  <autoFilter ref="A1:E247" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
refactor: update country template and translations
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359AD1E0-B9BA-5040-B82B-414505A33B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F702EB0-B7A8-AC4B-96B8-C2681896E9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
-    <sheet name="REPORT" sheetId="1" r:id="rId1"/>
-    <sheet name="QA_REPORT" sheetId="2" r:id="rId2"/>
-    <sheet name="DASHBOARD" sheetId="3" r:id="rId3"/>
-    <sheet name="MSG" sheetId="4" r:id="rId4"/>
+    <sheet name="REPORT_reference" sheetId="1" r:id="rId1"/>
+    <sheet name="REPORT" sheetId="5" r:id="rId2"/>
+    <sheet name="QA_REPORT" sheetId="6" r:id="rId3"/>
+    <sheet name="QA_REPORT_reference" sheetId="2" r:id="rId4"/>
+    <sheet name="DASHBOARD" sheetId="3" r:id="rId5"/>
+    <sheet name="MSG" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$247</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">QA_REPORT!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT!$A$1:$E$169</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DASHBOARD!$A$1:$E$247</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MSG!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">QA_REPORT_reference!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REPORT_reference!$A$1:$E$169</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="1037">
   <si>
     <t>LABEL</t>
   </si>
@@ -3154,12 +3156,24 @@
   <si>
     <t>outbreaks_disease_legend</t>
   </si>
+  <si>
+    <t>Resultados del análisis de riesgo para polio del nivel municipal</t>
+  </si>
+  <si>
+    <t>Este informe muestra los resultados del análisis de riesgo para polio del nivel municipal que incluye indicadores de inmunidad, vigilancia epidemiológica, determinantes sociales y la presencia de eventos o brotes de enfermedades prevenibles por vacunación. El objetivo de realizar el análisis de riesgo es encaminar las decisiones hacia la mitigación del riesgo total y por componente. Además, el resultado servirá de insumo para el Informe Anual sobre la documentación del estatus de la erradicación de la polio.</t>
+  </si>
+  <si>
+    <t>La herramienta para el análisis de riesgo ha sido elaborada por la Organización Panamericana de la Salud para disposición de los países.</t>
+  </si>
+  <si>
+    <t>Herramienta de evaluación de riesgo polio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3211,6 +3225,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3298,7 +3319,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3615,8 +3638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C7D9D-C4E2-B94C-B003-B8DCE10597B7}">
   <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A101" zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108:B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4995,7 +5018,7 @@
         <v>301</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>42</v>
+        <v>891</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>43</v>
@@ -5029,7 +5052,7 @@
         <v>303</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>52</v>
+        <v>890</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>53</v>
@@ -5794,11 +5817,714 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="5" width="38.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>891</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>282</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>287</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>292</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>296</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="150" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DBD2-0F3F-5E4C-83A2-49E17C536753}">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>441</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>443</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>445</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>447</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>451</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>453</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>455</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>457</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>459</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>461</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>463</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>465</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>467</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>469</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>471</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>473</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>475</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>477</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>479</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>481</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>483</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>485</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>487</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>489</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>491</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>495</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>497</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>499</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>501</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>503</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>505</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>507</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>513</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>515</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>517</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>519</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>524</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>526</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>564</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>566</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>568</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>570</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F5FF65-00C6-6F47-9553-2E4604D763C3}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6282,7 +7008,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>542</v>
       </c>
@@ -6409,11 +7135,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A45" zoomScale="150" workbookViewId="0">
       <selection activeCell="D268" sqref="D268"/>
     </sheetView>
   </sheetViews>
@@ -9904,7 +10630,7 @@
       </c>
     </row>
     <row r="284" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A284" s="16" t="s">
+      <c r="A284" t="s">
         <v>1032</v>
       </c>
       <c r="B284" s="4" t="s">
@@ -9919,7 +10645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1088E479-CA72-964B-98C9-FB941DEE85DA}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -10068,6 +10794,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -10321,15 +11056,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
   <ds:schemaRefs>
@@ -10343,6 +11069,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10360,12 +11094,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: immunity numeric QA
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F702EB0-B7A8-AC4B-96B8-C2681896E9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37A852F-C5A5-FA43-B892-42505F8A401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="1042">
   <si>
     <t>LABEL</t>
   </si>
@@ -3167,6 +3167,21 @@
   </si>
   <si>
     <t>Herramienta de evaluación de riesgo polio</t>
+  </si>
+  <si>
+    <t>immunity_populations_and_pfa</t>
+  </si>
+  <si>
+    <t>¿Si la población &lt;15 años de edad es &lt;100000, se presentaron casos de PFA en el 2022?</t>
+  </si>
+  <si>
+    <t>immunity_polio</t>
+  </si>
+  <si>
+    <t>immunity_ipv_coverage</t>
+  </si>
+  <si>
+    <t>immunity_polio_coverage</t>
   </si>
 </sst>
 </file>
@@ -3276,7 +3291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3318,6 +3333,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -6082,7 +6101,7 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>1034</v>
       </c>
     </row>
@@ -6090,7 +6109,7 @@
       <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="18" t="s">
         <v>1035</v>
       </c>
     </row>
@@ -6101,10 +6120,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DBD2-0F3F-5E4C-83A2-49E17C536753}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6514,6 +6533,46 @@
         <v>571</v>
       </c>
     </row>
+    <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="16" t="s">
+        <v>880</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>896</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6521,10 +6580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F5FF65-00C6-6F47-9553-2E4604D763C3}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A64" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7128,6 +7187,10 @@
         <v>571</v>
       </c>
     </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="16"/>
+      <c r="B77" s="17"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{94F5FF65-00C6-6F47-9553-2E4604D763C3}"/>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7139,8 +7202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D268" sqref="D268"/>
+    <sheetView topLeftCell="A95" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B98" sqref="A98:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat(QA): surveillance NA count
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37A852F-C5A5-FA43-B892-42505F8A401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D841958-CAB4-4C41-9C95-28935300AC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="30540" yWindow="-580" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT_reference" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="1055">
   <si>
     <t>LABEL</t>
   </si>
@@ -3182,6 +3182,45 @@
   </si>
   <si>
     <t>immunity_polio_coverage</t>
+  </si>
+  <si>
+    <t>title_surveillance</t>
+  </si>
+  <si>
+    <t>surveillance_reporting_units_var</t>
+  </si>
+  <si>
+    <t>% de unidades notificadoras que enviaron información en todas las semanas durante el periodo evaluado (2022)</t>
+  </si>
+  <si>
+    <t>surveillance_pfa_rate_var</t>
+  </si>
+  <si>
+    <t>surveillance_pfa_notified_var</t>
+  </si>
+  <si>
+    <t>surveillance_pfa_investigated_var</t>
+  </si>
+  <si>
+    <t>surveillance_suitable_samples_var</t>
+  </si>
+  <si>
+    <t>surveillance_followups_var</t>
+  </si>
+  <si>
+    <t>% de casos con seguimiento a los 60 días</t>
+  </si>
+  <si>
+    <t>% de casos con muestra adecuada de heces</t>
+  </si>
+  <si>
+    <t>% de casos de PFA investigados en menos de 48 horas</t>
+  </si>
+  <si>
+    <t>%  de casos de PFA con notificación oportuna (antes de 14 días desde el inicio de la parálisis)</t>
+  </si>
+  <si>
+    <t>surveillance_active_search_var</t>
   </si>
 </sst>
 </file>
@@ -6120,16 +6159,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DBD2-0F3F-5E4C-83A2-49E17C536753}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="2" max="2" width="47" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6525,7 +6564,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>570</v>
       </c>
@@ -6533,7 +6572,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>1037</v>
       </c>
@@ -6541,7 +6580,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>1039</v>
       </c>
@@ -6549,7 +6588,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>1041</v>
       </c>
@@ -6557,7 +6596,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>1040</v>
       </c>
@@ -6565,12 +6604,110 @@
         <v>895</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
         <v>880</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>896</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="16" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>406</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>411</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="16" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="16" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="16" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="16" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="16" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A64" s="16" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -7202,8 +7339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B98" sqref="A98:B98"/>
+    <sheetView topLeftCell="A145" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B157" sqref="A157:B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat(QA): outbreaks done! all QA is done
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2899B4E6-3B65-2F47-A92F-949205244ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC9D8D0-E591-024D-AD8E-E7D305F73B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="1061">
   <si>
     <t>LABEL</t>
   </si>
@@ -3236,6 +3236,9 @@
   </si>
   <si>
     <t>% de la población con acceso a servicios básicos de saneamiento</t>
+  </si>
+  <si>
+    <t>tilte_outbreaks</t>
   </si>
 </sst>
 </file>
@@ -6174,10 +6177,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DBD2-0F3F-5E4C-83A2-49E17C536753}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6749,6 +6752,62 @@
         <v>1059</v>
       </c>
     </row>
+    <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>1030</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6759,7 +6818,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView topLeftCell="A64" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7378,8 +7437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView topLeftCell="A254" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A267" sqref="A267:B267"/>
+    <sheetView topLeftCell="A265" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B282" activeCellId="6" sqref="A269:B269 A272:B272 A274:B274 A276:B276 A278:B278 A280:B280 A282:B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat(report): background section + total risks
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABCE148-CCE6-DE45-A089-69F3E3EC6F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1986828-3120-3A4B-86A6-00FEDCB72F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25460" windowHeight="18880" activeTab="1" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT_reference" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="1069">
   <si>
     <t>LABEL</t>
   </si>
@@ -3245,6 +3245,24 @@
   </si>
   <si>
     <t>Datos generales</t>
+  </si>
+  <si>
+    <t>A cada municipio del país se le asigna una categoría programática de riesgo: bajo, medio, alto o muy algo, en base a la puntación final obtenida. El puntaje para cada indicador fue realizado por consenso de expertos. El rango de puntajes posibles va de 0 a 100 puntos de riesgo, según la siguiente tabla:</t>
+  </si>
+  <si>
+    <t>background_par_3</t>
+  </si>
+  <si>
+    <t>fueron categorizados en riesgo muy alto</t>
+  </si>
+  <si>
+    <t>fueron categorizados en riesgo alto</t>
+  </si>
+  <si>
+    <t>fueron categorizados en riesgo bajo</t>
+  </si>
+  <si>
+    <t>Perfil de país</t>
   </si>
 </sst>
 </file>
@@ -3354,7 +3372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3402,7 +3420,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3720,8 +3744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C7D9D-C4E2-B94C-B003-B8DCE10597B7}">
   <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108:B111"/>
+    <sheetView topLeftCell="A34" zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5900,10 +5924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6168,12 +6192,229 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="3" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>1035</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+    </row>
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>406</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>411</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>1068</v>
       </c>
     </row>
   </sheetData>
@@ -6185,7 +6426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DBD2-0F3F-5E4C-83A2-49E17C536753}">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -6629,15 +6870,15 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="16" t="s">
+      <c r="A54" t="s">
         <v>880</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="4" t="s">
         <v>896</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="16" t="s">
+      <c r="A55" t="s">
         <v>1042</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -6687,55 +6928,55 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
+      <c r="A59" t="s">
         <v>1045</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="4" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
+      <c r="A60" t="s">
         <v>1046</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="4" t="s">
         <v>1053</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="16" t="s">
+      <c r="A61" t="s">
         <v>1047</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="4" t="s">
         <v>1052</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="16" t="s">
+      <c r="A62" t="s">
         <v>1048</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="4" t="s">
         <v>1051</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="16" t="s">
+      <c r="A63" t="s">
         <v>1049</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="4" t="s">
         <v>1050</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A64" s="16" t="s">
+      <c r="A64" t="s">
         <v>1054</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="4" t="s">
         <v>940</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="16" t="s">
+      <c r="A65" t="s">
         <v>1055</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -6821,7 +7062,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F5FF65-00C6-6F47-9553-2E4604D763C3}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A64" zoomScale="150" workbookViewId="0">
       <selection activeCell="B80" sqref="B80"/>
@@ -7428,10 +7669,6 @@
         <v>571</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="16"/>
-      <c r="B77" s="17"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{94F5FF65-00C6-6F47-9553-2E4604D763C3}"/>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7443,8 +7680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView topLeftCell="A265" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B282" activeCellId="6" sqref="A269:B269 A272:B272 A274:B274 A276:B276 A278:B278 A280:B280 A282:B282"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11098,15 +11335,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -11360,6 +11588,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
   <ds:schemaRefs>
@@ -11373,14 +11610,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11398,4 +11627,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(report): tabla 1. perfil de país
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1986828-3120-3A4B-86A6-00FEDCB72F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAAF4D6-625E-0C41-820F-C37492C7EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25460" windowHeight="18880" activeTab="1" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15880" windowHeight="18880" activeTab="1" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT_reference" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="1085">
   <si>
     <t>LABEL</t>
   </si>
@@ -3263,6 +3263,54 @@
   </si>
   <si>
     <t>Perfil de país</t>
+  </si>
+  <si>
+    <t>table_1a_pob</t>
+  </si>
+  <si>
+    <t>Población total para el año de evaluación</t>
+  </si>
+  <si>
+    <t>table_1a_pob1</t>
+  </si>
+  <si>
+    <t>Población &lt;1 año para el año de evaluación</t>
+  </si>
+  <si>
+    <t>table_1a_pob5</t>
+  </si>
+  <si>
+    <t>Población &lt;5 año para el año de evaluación</t>
+  </si>
+  <si>
+    <t>table_1a_pob15</t>
+  </si>
+  <si>
+    <t>Población &lt;15 año para el año de evaluación</t>
+  </si>
+  <si>
+    <t>table_1a_admin2</t>
+  </si>
+  <si>
+    <t>Número de municipios en el país</t>
+  </si>
+  <si>
+    <t>table_1a_polio_scheme</t>
+  </si>
+  <si>
+    <t>Esquema de vacunación contra la polio</t>
+  </si>
+  <si>
+    <t>table_1a_polio_coverage</t>
+  </si>
+  <si>
+    <t>Cobertura de polio 3</t>
+  </si>
+  <si>
+    <t>table_1a_pfa_rate</t>
+  </si>
+  <si>
+    <t>Tasa de PFA nacional del último año</t>
   </si>
 </sst>
 </file>
@@ -5924,10 +5972,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6417,6 +6465,78 @@
         <v>1068</v>
       </c>
     </row>
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>441</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>1084</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6427,7 +6547,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: general data report
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAAF4D6-625E-0C41-820F-C37492C7EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4808DA3-9085-F943-A60B-8E21D387350E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15880" windowHeight="18880" activeTab="1" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="1102">
   <si>
     <t>LABEL</t>
   </si>
@@ -3311,6 +3311,57 @@
   </si>
   <si>
     <t>Tasa de PFA nacional del último año</t>
+  </si>
+  <si>
+    <t>table_1a_colname1</t>
+  </si>
+  <si>
+    <t>table_1a_colname2</t>
+  </si>
+  <si>
+    <t>table_1b_title</t>
+  </si>
+  <si>
+    <t>Resultados del análisis de riesgo municipal</t>
+  </si>
+  <si>
+    <t>table_1b_pob1</t>
+  </si>
+  <si>
+    <t>table_1b_pob5</t>
+  </si>
+  <si>
+    <t>table_1b_pob15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población &lt;1 (%)* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población &lt;5 (%)* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población &lt;15 (%)* </t>
+  </si>
+  <si>
+    <t>table_1b_footnote</t>
+  </si>
+  <si>
+    <t>*Respecto a la población total de ese grupo de edad</t>
+  </si>
+  <si>
+    <t>figure_1a_title</t>
+  </si>
+  <si>
+    <t>figure_1b_title</t>
+  </si>
+  <si>
+    <t>Resultados del análisis de riesgo municipal para los municipios con ≥100,000 menores de 15 años</t>
+  </si>
+  <si>
+    <t>figure_1c_title</t>
+  </si>
+  <si>
+    <t>Resultados del análisis de riesgo municipal para los municipios con &lt;100 000 menores de 15 años</t>
   </si>
 </sst>
 </file>
@@ -3420,7 +3471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3474,6 +3525,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3793,7 +3847,7 @@
   <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="133" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:B41"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5972,10 +6026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6411,130 +6465,401 @@
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>101</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>103</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>1065</v>
+        <v>108</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>109</v>
+        <v>112</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>1067</v>
+      <c r="A43" t="s">
+        <v>441</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>112</v>
+      <c r="A44" t="s">
+        <v>1069</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>441</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>442</v>
+        <v>1071</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>1072</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1069</v>
+        <v>1073</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1070</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1072</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1075</v>
+        <v>1079</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1077</v>
+        <v>1081</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1079</v>
+        <v>1083</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1084</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>968</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>970</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>971</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>277</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="16" t="s">
+        <v>899</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>305</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>301</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>891</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>302</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>303</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>304</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>671</v>
+      </c>
+      <c r="C70" s="19"/>
+    </row>
+    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>311</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="16" t="s">
+        <v>667</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="16" t="s">
+        <v>658</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>1101</v>
       </c>
     </row>
   </sheetData>
@@ -7800,8 +8125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A48" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: word report. Some errors have to been fixed
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FF260E-E3D5-E749-8189-FB1A82BDA31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3447E6-D303-5C42-9C07-95DFA41BFDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="1420" windowWidth="15880" windowHeight="18880" activeTab="1" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="1115">
   <si>
     <t>LABEL</t>
   </si>
@@ -3389,6 +3389,18 @@
   </si>
   <si>
     <t>Vigilancia</t>
+  </si>
+  <si>
+    <t>figure_3a_title</t>
+  </si>
+  <si>
+    <t>Resultados del análisis de riesgo para el componente de vigilancia</t>
+  </si>
+  <si>
+    <t>figure_3b_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultados del análisis de riesgo para el componente de vigilancia para municipios con &gt;100 000 menores de 15 años </t>
   </si>
 </sst>
 </file>
@@ -3498,7 +3510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3540,6 +3552,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6057,10 +6072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6321,7 +6336,7 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
         <v>1034</v>
       </c>
     </row>
@@ -6337,122 +6352,122 @@
       <c r="A22" t="s">
         <v>1064</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="18" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -6479,55 +6494,55 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="18" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="18" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="18" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="18" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="18" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="17" t="s">
         <v>112</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -6721,7 +6736,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>899</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -6819,14 +6834,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="16" t="s">
+    <row r="70" spans="1:5" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="18" t="s">
         <v>671</v>
       </c>
-      <c r="C70" s="19"/>
+      <c r="C70" s="20"/>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -6854,23 +6869,23 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="17" t="s">
         <v>665</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="18" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="17" t="s">
         <v>667</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="18" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="17" t="s">
         <v>658</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -6889,7 +6904,7 @@
       <c r="A77" t="s">
         <v>1100</v>
       </c>
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="22" t="s">
         <v>1101</v>
       </c>
     </row>
@@ -6929,7 +6944,7 @@
       <c r="A82" t="s">
         <v>876</v>
       </c>
-      <c r="B82" s="22" t="s">
+      <c r="B82" s="23" t="s">
         <v>1109</v>
       </c>
     </row>
@@ -6942,15 +6957,15 @@
       </c>
     </row>
     <row r="84" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="17" t="s">
         <v>911</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="18" t="s">
         <v>912</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="23" t="s">
+      <c r="A85" s="24" t="s">
         <v>144</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -6958,72 +6973,84 @@
       </c>
     </row>
     <row r="86" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="16" t="s">
+      <c r="A86" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="18" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A87" s="16" t="s">
+      <c r="A87" s="17" t="s">
         <v>907</v>
       </c>
-      <c r="B87" s="17" t="s">
+      <c r="B87" s="18" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="16" t="s">
+      <c r="A88" s="17" t="s">
         <v>913</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="18" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A89" s="16" t="s">
+      <c r="A89" s="17" t="s">
         <v>918</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="18" t="s">
         <v>919</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A90" s="16" t="s">
+      <c r="A90" s="17" t="s">
         <v>924</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="18" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A91" s="16" t="s">
+      <c r="A91" s="17" t="s">
         <v>928</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="18" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A92" s="16" t="s">
+      <c r="A92" s="17" t="s">
         <v>933</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="18" t="s">
         <v>935</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A93" s="16" t="s">
+      <c r="A93" s="17" t="s">
         <v>937</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="18" t="s">
         <v>938</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="16"/>
-      <c r="B94" s="19"/>
+    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A94" s="17" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A95" s="17" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>1114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: download reports from dashboard
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3447E6-D303-5C42-9C07-95DFA41BFDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCDC435-BAD1-F74A-902C-5C6ADB7D861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1420" windowWidth="15880" windowHeight="18880" activeTab="1" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT_reference" sheetId="1" r:id="rId1"/>
@@ -1828,9 +1828,6 @@
     <t>report_filename</t>
   </si>
   <si>
-    <t>Informe evaluación de riesgo sarampión y rubéola</t>
-  </si>
-  <si>
     <t>button_map</t>
   </si>
   <si>
@@ -3401,6 +3398,9 @@
   </si>
   <si>
     <t xml:space="preserve">Resultados del análisis de riesgo para el componente de vigilancia para municipios con &gt;100 000 menores de 15 años </t>
+  </si>
+  <si>
+    <t>Informe evaluación de riesgo  polio</t>
   </si>
 </sst>
 </file>
@@ -3510,7 +3510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3556,17 +3556,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3575,7 +3568,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5272,7 +5264,7 @@
         <v>301</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>43</v>
@@ -5306,7 +5298,7 @@
         <v>303</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>53</v>
@@ -6074,8 +6066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6111,7 +6103,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6185,7 +6177,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>43</v>
@@ -6219,7 +6211,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>53</v>
@@ -6336,8 +6328,8 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>1034</v>
+      <c r="B20" s="17" t="s">
+        <v>1033</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="136" x14ac:dyDescent="0.2">
@@ -6345,136 +6337,112 @@
         <v>39</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1064</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>1035</v>
+        <v>1063</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>1034</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="A26" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
+      <c r="A27" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
+      <c r="A28" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
+      <c r="A30" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
+      <c r="A31" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+      <c r="A32" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>94</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -6494,59 +6462,59 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
+      <c r="A36" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="A37" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
+      <c r="A38" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="4" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B39" s="18" t="s">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>1066</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="18" t="s">
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>1067</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -6559,71 +6527,71 @@
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>1069</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>1071</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>1073</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>1074</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>1075</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>1077</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>1078</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>1079</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>1080</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>1081</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>1082</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>1083</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>440</v>
@@ -6631,7 +6599,7 @@
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>220</v>
@@ -6639,66 +6607,66 @@
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>1087</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>1095</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>967</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>968</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6723,30 +6691,30 @@
         <v>277</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>664</v>
-      </c>
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
-        <v>899</v>
+      <c r="A64" t="s">
+        <v>898</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6771,7 +6739,7 @@
         <v>301</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>43</v>
@@ -6788,7 +6756,7 @@
         <v>302</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>48</v>
@@ -6805,7 +6773,7 @@
         <v>303</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>53</v>
@@ -6834,14 +6802,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>310</v>
       </c>
-      <c r="B70" s="18" t="s">
-        <v>671</v>
-      </c>
-      <c r="C70" s="20"/>
+      <c r="B70" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="D70"/>
+      <c r="E70"/>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -6862,50 +6831,50 @@
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
+      <c r="A73" t="s">
+        <v>664</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="B73" s="18" t="s">
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
+      <c r="B74" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="B74" s="18" t="s">
-        <v>668</v>
-      </c>
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
+      <c r="A75" t="s">
+        <v>657</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>658</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>1098</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B77" s="19" t="s">
         <v>1100</v>
-      </c>
-      <c r="B77" s="22" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6913,143 +6882,143 @@
         <v>120</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>1103</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>1104</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>876</v>
-      </c>
-      <c r="B82" s="23" t="s">
-        <v>1109</v>
+        <v>875</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>1108</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="17" t="s">
+      <c r="A84" t="s">
+        <v>910</v>
+      </c>
+      <c r="B84" s="4" t="s">
         <v>911</v>
       </c>
-      <c r="B84" s="18" t="s">
+    </row>
+    <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>335</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>906</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="B85" s="3" t="s">
+      <c r="B88" s="4" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>917</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>923</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>927</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>932</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>936</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>1110</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="B86" s="18" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A87" s="17" t="s">
-        <v>907</v>
-      </c>
-      <c r="B87" s="18" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="17" t="s">
-        <v>913</v>
-      </c>
-      <c r="B88" s="18" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A89" s="17" t="s">
-        <v>918</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A90" s="17" t="s">
-        <v>924</v>
-      </c>
-      <c r="B90" s="18" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A91" s="17" t="s">
-        <v>928</v>
-      </c>
-      <c r="B91" s="18" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A92" s="17" t="s">
-        <v>933</v>
-      </c>
-      <c r="B92" s="18" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
-        <v>937</v>
-      </c>
-      <c r="B93" s="18" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A94" s="17" t="s">
+      <c r="B94" s="16" t="s">
         <v>1111</v>
       </c>
-      <c r="B94" s="16" t="s">
+    </row>
+    <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>1112</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A95" s="17" t="s">
+      <c r="B95" s="16" t="s">
         <v>1113</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -7101,7 +7070,7 @@
         <v>435</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7309,7 +7278,7 @@
         <v>485</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -7357,7 +7326,7 @@
         <v>499</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -7474,47 +7443,47 @@
     </row>
     <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>1037</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>145</v>
@@ -7556,138 +7525,138 @@
     </row>
     <row r="58" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>1043</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>1049</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>1056</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>1057</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>1058</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>
@@ -8315,8 +8284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A156" activeCellId="6" sqref="A135:B135 A138:B138 A142:B142 A146:B146 A150:B150 A153:B153 A156:B156"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8367,7 +8336,7 @@
         <v>577</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -8386,7 +8355,7 @@
         <v>580</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>225</v>
@@ -8487,7 +8456,7 @@
         <v>592</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>593</v>
+        <v>1114</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
@@ -8495,10 +8464,10 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>594</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>595</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
@@ -8506,10 +8475,10 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>596</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>597</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="7"/>
@@ -8517,44 +8486,44 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>510</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>600</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>512</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>604</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>606</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>607</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7"/>
@@ -8562,10 +8531,10 @@
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>608</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>609</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="7"/>
@@ -8573,24 +8542,24 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>609</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>613</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>121</v>
@@ -8607,7 +8576,7 @@
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>145</v>
@@ -8624,27 +8593,27 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>873</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>874</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>875</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>121</v>
@@ -8661,7 +8630,7 @@
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>145</v>
@@ -8678,7 +8647,7 @@
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>164</v>
@@ -8695,7 +8664,7 @@
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>193</v>
@@ -8712,61 +8681,61 @@
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>561</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>621</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>613</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>870</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>871</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>872</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>868</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>869</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>870</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>145</v>
@@ -8783,7 +8752,7 @@
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>121</v>
@@ -8800,24 +8769,24 @@
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>613</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>121</v>
@@ -8834,7 +8803,7 @@
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>145</v>
@@ -8851,7 +8820,7 @@
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>164</v>
@@ -8868,7 +8837,7 @@
     </row>
     <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>193</v>
@@ -8885,24 +8854,24 @@
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>561</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>621</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>121</v>
@@ -8919,7 +8888,7 @@
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>145</v>
@@ -8936,7 +8905,7 @@
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>145</v>
@@ -8953,24 +8922,24 @@
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>628</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>632</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>582</v>
@@ -8987,10 +8956,10 @@
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>635</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>636</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="7"/>
@@ -8998,7 +8967,7 @@
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>306</v>
@@ -9015,10 +8984,10 @@
     </row>
     <row r="47" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>638</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>639</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="7"/>
@@ -9026,7 +8995,7 @@
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>306</v>
@@ -9043,7 +9012,7 @@
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>312</v>
@@ -9060,10 +9029,10 @@
     </row>
     <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>642</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>643</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="7"/>
@@ -9071,10 +9040,10 @@
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="B51" s="9" t="s">
         <v>644</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>645</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="7"/>
@@ -9082,10 +9051,10 @@
     </row>
     <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="B52" s="9" t="s">
         <v>646</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>647</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="7"/>
@@ -9093,10 +9062,10 @@
     </row>
     <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="B53" s="9" t="s">
         <v>648</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>649</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="7"/>
@@ -9104,10 +9073,10 @@
     </row>
     <row r="54" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>650</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>651</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="7"/>
@@ -9115,36 +9084,36 @@
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>652</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>656</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -9163,7 +9132,7 @@
         <v>301</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>43</v>
@@ -9180,7 +9149,7 @@
         <v>302</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>48</v>
@@ -9197,7 +9166,7 @@
         <v>303</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>53</v>
@@ -9228,10 +9197,10 @@
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="B62" s="9" t="s">
         <v>658</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>659</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="7"/>
@@ -9261,7 +9230,7 @@
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>72</v>
@@ -9292,30 +9261,30 @@
         <v>277</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>663</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E68" s="3"/>
     </row>
@@ -9389,10 +9358,10 @@
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="B73" s="9" t="s">
         <v>665</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>666</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="7"/>
@@ -9400,10 +9369,10 @@
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="B74" s="9" t="s">
         <v>667</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>668</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="7"/>
@@ -9411,10 +9380,10 @@
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="B75" s="9" t="s">
         <v>669</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>670</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="7"/>
@@ -9442,7 +9411,7 @@
         <v>310</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="7"/>
@@ -9467,10 +9436,10 @@
     </row>
     <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="B79" s="9" t="s">
         <v>672</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>673</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="7"/>
@@ -9478,10 +9447,10 @@
     </row>
     <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="B80" s="9" t="s">
         <v>674</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>675</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="7"/>
@@ -9489,7 +9458,7 @@
     </row>
     <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>582</v>
@@ -9506,27 +9475,27 @@
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>676</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="C82" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="E82" s="3" t="s">
         <v>680</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="B83" s="9" t="s">
         <v>682</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>683</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="7"/>
@@ -9534,10 +9503,10 @@
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="B84" s="9" t="s">
         <v>684</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>685</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="7"/>
@@ -9545,10 +9514,10 @@
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="B85" s="9" t="s">
         <v>686</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>687</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="7"/>
@@ -9556,10 +9525,10 @@
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="B86" s="9" t="s">
         <v>688</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>689</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="7"/>
@@ -9567,10 +9536,10 @@
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="B87" s="9" t="s">
         <v>690</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>691</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="7"/>
@@ -9578,10 +9547,10 @@
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="B88" s="9" t="s">
         <v>692</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>693</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="7"/>
@@ -9589,10 +9558,10 @@
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="B89" s="9" t="s">
         <v>694</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>695</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="7"/>
@@ -9600,10 +9569,10 @@
     </row>
     <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="B90" s="9" t="s">
         <v>696</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>697</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="7"/>
@@ -9611,10 +9580,10 @@
     </row>
     <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>698</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>699</v>
       </c>
       <c r="C91" s="8"/>
       <c r="D91" s="7"/>
@@ -9622,10 +9591,10 @@
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="B92" s="9" t="s">
         <v>700</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>701</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="7"/>
@@ -9633,10 +9602,10 @@
     </row>
     <row r="93" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="B93" s="9" t="s">
         <v>702</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>703</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="7"/>
@@ -9644,10 +9613,10 @@
     </row>
     <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="7"/>
@@ -9655,10 +9624,10 @@
     </row>
     <row r="95" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
+        <v>883</v>
+      </c>
+      <c r="B95" s="9" t="s">
         <v>884</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>885</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
@@ -9666,10 +9635,10 @@
     </row>
     <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="7"/>
@@ -9677,10 +9646,10 @@
     </row>
     <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>886</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>887</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="7"/>
@@ -9688,10 +9657,10 @@
     </row>
     <row r="98" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="7"/>
@@ -9699,10 +9668,10 @@
     </row>
     <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="7"/>
@@ -9710,10 +9679,10 @@
     </row>
     <row r="100" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="7"/>
@@ -9721,10 +9690,10 @@
     </row>
     <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="B101" s="9" t="s">
         <v>882</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>883</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="7"/>
@@ -9732,10 +9701,10 @@
     </row>
     <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="7"/>
@@ -9743,21 +9712,21 @@
     </row>
     <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
+        <v>949</v>
+      </c>
+      <c r="B103" s="9" t="s">
         <v>950</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>951</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
+        <v>951</v>
+      </c>
+      <c r="B104" s="9" t="s">
         <v>952</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>953</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="7"/>
@@ -9765,7 +9734,7 @@
     </row>
     <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>135</v>
@@ -9782,7 +9751,7 @@
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>140</v>
@@ -9799,10 +9768,10 @@
     </row>
     <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="B107" s="9" t="s">
         <v>706</v>
-      </c>
-      <c r="B107" s="9" t="s">
-        <v>707</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
@@ -9810,10 +9779,10 @@
     </row>
     <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="B108" s="9" t="s">
         <v>708</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>709</v>
       </c>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
@@ -9821,27 +9790,27 @@
     </row>
     <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>709</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="C109" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="D109" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="E109" s="3" t="s">
         <v>713</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="B110" s="9" t="s">
         <v>715</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>716</v>
       </c>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
@@ -9849,10 +9818,10 @@
     </row>
     <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="B111" s="9" t="s">
         <v>717</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>718</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -9860,10 +9829,10 @@
     </row>
     <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="B112" s="9" t="s">
         <v>719</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>720</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
@@ -9910,7 +9879,7 @@
     </row>
     <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>74</v>
@@ -9938,7 +9907,7 @@
     </row>
     <row r="118" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>130</v>
@@ -9955,27 +9924,27 @@
     </row>
     <row r="119" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>722</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="C119" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="D119" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="E119" s="3" t="s">
         <v>726</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="B120" s="9" t="s">
         <v>728</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>729</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="7"/>
@@ -9994,10 +9963,10 @@
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="B122" s="9" t="s">
         <v>730</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>731</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="7"/>
@@ -10005,10 +9974,10 @@
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="7"/>
@@ -10038,10 +10007,10 @@
     </row>
     <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="B126" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="B126" s="9" t="s">
-        <v>734</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="7"/>
@@ -10052,16 +10021,16 @@
         <v>327</v>
       </c>
       <c r="B127" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="D127" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="E127" s="3" t="s">
         <v>737</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -10072,13 +10041,13 @@
         <v>330</v>
       </c>
       <c r="C128" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="D128" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="E128" s="3" t="s">
         <v>740</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -10089,13 +10058,13 @@
         <v>332</v>
       </c>
       <c r="C129" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="D129" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="D129" s="3" t="s">
+      <c r="E129" s="3" t="s">
         <v>743</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -10103,7 +10072,7 @@
         <v>333</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
@@ -10144,10 +10113,10 @@
     </row>
     <row r="134" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="7"/>
@@ -10155,10 +10124,10 @@
     </row>
     <row r="135" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="B135" s="9" t="s">
         <v>907</v>
-      </c>
-      <c r="B135" s="9" t="s">
-        <v>908</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="7"/>
@@ -10166,10 +10135,10 @@
     </row>
     <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="B136" s="9" t="s">
         <v>909</v>
-      </c>
-      <c r="B136" s="9" t="s">
-        <v>910</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="7"/>
@@ -10177,10 +10146,10 @@
     </row>
     <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
+        <v>953</v>
+      </c>
+      <c r="B137" s="9" t="s">
         <v>954</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>955</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="7"/>
@@ -10188,10 +10157,10 @@
     </row>
     <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="7"/>
@@ -10199,10 +10168,10 @@
     </row>
     <row r="139" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
+        <v>913</v>
+      </c>
+      <c r="B139" s="9" t="s">
         <v>914</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>915</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="7"/>
@@ -10210,10 +10179,10 @@
     </row>
     <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="B140" s="9" t="s">
         <v>916</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>917</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="7"/>
@@ -10221,10 +10190,10 @@
     </row>
     <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="7"/>
@@ -10232,10 +10201,10 @@
     </row>
     <row r="142" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="B142" s="9" t="s">
         <v>918</v>
-      </c>
-      <c r="B142" s="9" t="s">
-        <v>919</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="7"/>
@@ -10243,10 +10212,10 @@
     </row>
     <row r="143" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="B143" s="9" t="s">
         <v>920</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>921</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="7"/>
@@ -10254,10 +10223,10 @@
     </row>
     <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="7"/>
@@ -10265,10 +10234,10 @@
     </row>
     <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B145" s="9" t="s">
         <v>957</v>
-      </c>
-      <c r="B145" s="9" t="s">
-        <v>958</v>
       </c>
       <c r="C145" s="8"/>
       <c r="D145" s="7"/>
@@ -10276,10 +10245,10 @@
     </row>
     <row r="146" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="7"/>
@@ -10287,21 +10256,21 @@
     </row>
     <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C147" s="8"/>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="B148" s="9" t="s">
         <v>959</v>
-      </c>
-      <c r="B148" s="9" t="s">
-        <v>960</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="7"/>
@@ -10309,7 +10278,7 @@
     </row>
     <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B149" s="9" t="s">
         <v>341</v>
@@ -10320,10 +10289,10 @@
     </row>
     <row r="150" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="7"/>
@@ -10331,21 +10300,21 @@
     </row>
     <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="7"/>
@@ -10353,10 +10322,10 @@
     </row>
     <row r="153" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="7"/>
@@ -10364,21 +10333,21 @@
     </row>
     <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="B155" s="9" t="s">
         <v>963</v>
-      </c>
-      <c r="B155" s="9" t="s">
-        <v>964</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="7"/>
@@ -10386,10 +10355,10 @@
     </row>
     <row r="156" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
+        <v>936</v>
+      </c>
+      <c r="B156" s="9" t="s">
         <v>937</v>
-      </c>
-      <c r="B156" s="9" t="s">
-        <v>938</v>
       </c>
       <c r="C156" s="8"/>
       <c r="D156" s="7"/>
@@ -10397,10 +10366,10 @@
     </row>
     <row r="157" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="B157" s="9" t="s">
         <v>939</v>
-      </c>
-      <c r="B157" s="9" t="s">
-        <v>940</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="7"/>
@@ -10408,7 +10377,7 @@
     </row>
     <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B158" s="9" t="s">
         <v>324</v>
@@ -10474,10 +10443,10 @@
     </row>
     <row r="164" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="B164" s="9" t="s">
         <v>746</v>
-      </c>
-      <c r="B164" s="9" t="s">
-        <v>747</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="7"/>
@@ -10485,10 +10454,10 @@
     </row>
     <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="B165" s="9" t="s">
         <v>748</v>
-      </c>
-      <c r="B165" s="9" t="s">
-        <v>749</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="7"/>
@@ -10496,10 +10465,10 @@
     </row>
     <row r="166" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="B166" s="9" t="s">
         <v>750</v>
-      </c>
-      <c r="B166" s="9" t="s">
-        <v>751</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="7"/>
@@ -10507,10 +10476,10 @@
     </row>
     <row r="167" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="B167" s="9" t="s">
         <v>752</v>
-      </c>
-      <c r="B167" s="9" t="s">
-        <v>753</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="7"/>
@@ -10518,27 +10487,27 @@
     </row>
     <row r="168" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>753</v>
+      </c>
+      <c r="B168" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="C168" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="C168" s="3" t="s">
+      <c r="D168" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="E168" s="3" t="s">
         <v>757</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="B169" s="9" t="s">
         <v>759</v>
-      </c>
-      <c r="B169" s="9" t="s">
-        <v>760</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="7"/>
@@ -10546,27 +10515,27 @@
     </row>
     <row r="170" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>760</v>
+      </c>
+      <c r="B170" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="C170" s="3" t="s">
         <v>762</v>
       </c>
-      <c r="C170" s="3" t="s">
+      <c r="D170" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="D170" s="3" t="s">
+      <c r="E170" s="3" t="s">
         <v>764</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="B171" s="9" t="s">
         <v>766</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>767</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="7"/>
@@ -10574,10 +10543,10 @@
     </row>
     <row r="172" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="B172" s="9" t="s">
         <v>768</v>
-      </c>
-      <c r="B172" s="9" t="s">
-        <v>769</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="7"/>
@@ -10585,10 +10554,10 @@
     </row>
     <row r="173" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
+        <v>769</v>
+      </c>
+      <c r="B173" s="9" t="s">
         <v>770</v>
-      </c>
-      <c r="B173" s="9" t="s">
-        <v>771</v>
       </c>
       <c r="C173" s="8"/>
       <c r="D173" s="7"/>
@@ -10753,7 +10722,7 @@
     </row>
     <row r="185" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B185" s="4" t="s">
         <v>173</v>
@@ -10770,10 +10739,10 @@
     </row>
     <row r="186" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="B186" s="9" t="s">
         <v>773</v>
-      </c>
-      <c r="B186" s="9" t="s">
-        <v>774</v>
       </c>
       <c r="C186" s="8"/>
       <c r="D186" s="7"/>
@@ -10781,7 +10750,7 @@
     </row>
     <row r="187" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B187" s="4" t="s">
         <v>178</v>
@@ -10798,10 +10767,10 @@
     </row>
     <row r="188" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="B188" s="9" t="s">
         <v>776</v>
-      </c>
-      <c r="B188" s="9" t="s">
-        <v>777</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="7"/>
@@ -10809,10 +10778,10 @@
     </row>
     <row r="189" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="B189" s="9" t="s">
         <v>778</v>
-      </c>
-      <c r="B189" s="9" t="s">
-        <v>779</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="7"/>
@@ -10820,10 +10789,10 @@
     </row>
     <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="B190" s="9" t="s">
         <v>780</v>
-      </c>
-      <c r="B190" s="9" t="s">
-        <v>781</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="7"/>
@@ -10831,10 +10800,10 @@
     </row>
     <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="B191" s="9" t="s">
         <v>782</v>
-      </c>
-      <c r="B191" s="9" t="s">
-        <v>783</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="7"/>
@@ -10842,10 +10811,10 @@
     </row>
     <row r="192" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
+        <v>783</v>
+      </c>
+      <c r="B192" s="9" t="s">
         <v>784</v>
-      </c>
-      <c r="B192" s="9" t="s">
-        <v>785</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="7"/>
@@ -10853,10 +10822,10 @@
     </row>
     <row r="193" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="B193" s="9" t="s">
         <v>786</v>
-      </c>
-      <c r="B193" s="9" t="s">
-        <v>787</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="7"/>
@@ -10881,10 +10850,10 @@
     </row>
     <row r="195" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="B195" s="9" t="s">
         <v>788</v>
-      </c>
-      <c r="B195" s="9" t="s">
-        <v>789</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="7"/>
@@ -10892,7 +10861,7 @@
     </row>
     <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>306</v>
@@ -10909,10 +10878,10 @@
     </row>
     <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="B197" s="9" t="s">
         <v>791</v>
-      </c>
-      <c r="B197" s="9" t="s">
-        <v>792</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="7"/>
@@ -10920,10 +10889,10 @@
     </row>
     <row r="198" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="B198" s="9" t="s">
         <v>793</v>
-      </c>
-      <c r="B198" s="9" t="s">
-        <v>794</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="7"/>
@@ -10931,10 +10900,10 @@
     </row>
     <row r="199" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
+        <v>794</v>
+      </c>
+      <c r="B199" s="9" t="s">
         <v>795</v>
-      </c>
-      <c r="B199" s="9" t="s">
-        <v>796</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="7"/>
@@ -10942,10 +10911,10 @@
     </row>
     <row r="200" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="B200" s="9" t="s">
         <v>797</v>
-      </c>
-      <c r="B200" s="9" t="s">
-        <v>798</v>
       </c>
       <c r="C200" s="8"/>
       <c r="D200" s="7"/>
@@ -10953,7 +10922,7 @@
     </row>
     <row r="201" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B201" s="9" t="s">
         <v>395</v>
@@ -10964,10 +10933,10 @@
     </row>
     <row r="202" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="B202" s="9" t="s">
         <v>800</v>
-      </c>
-      <c r="B202" s="9" t="s">
-        <v>801</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="7"/>
@@ -10975,10 +10944,10 @@
     </row>
     <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="B203" s="9" t="s">
         <v>802</v>
-      </c>
-      <c r="B203" s="9" t="s">
-        <v>803</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="7"/>
@@ -10986,10 +10955,10 @@
     </row>
     <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="B204" s="9" t="s">
         <v>804</v>
-      </c>
-      <c r="B204" s="9" t="s">
-        <v>805</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="7"/>
@@ -11025,7 +10994,7 @@
     </row>
     <row r="207" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>377</v>
@@ -11042,10 +11011,10 @@
     </row>
     <row r="208" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A208" s="7" t="s">
+        <v>806</v>
+      </c>
+      <c r="B208" s="9" t="s">
         <v>807</v>
-      </c>
-      <c r="B208" s="9" t="s">
-        <v>808</v>
       </c>
       <c r="C208" s="8"/>
       <c r="D208" s="7"/>
@@ -11053,10 +11022,10 @@
     </row>
     <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
+        <v>808</v>
+      </c>
+      <c r="B209" s="9" t="s">
         <v>809</v>
-      </c>
-      <c r="B209" s="9" t="s">
-        <v>810</v>
       </c>
       <c r="C209" s="8"/>
       <c r="D209" s="7"/>
@@ -11067,7 +11036,7 @@
         <v>384</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C210" s="8"/>
       <c r="D210" s="7"/>
@@ -11163,10 +11132,10 @@
     </row>
     <row r="219" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A219" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="B219" s="9" t="s">
         <v>812</v>
-      </c>
-      <c r="B219" s="9" t="s">
-        <v>813</v>
       </c>
       <c r="C219" s="8"/>
       <c r="D219" s="7"/>
@@ -11174,10 +11143,10 @@
     </row>
     <row r="220" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A220" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="B220" s="9" t="s">
         <v>814</v>
-      </c>
-      <c r="B220" s="9" t="s">
-        <v>815</v>
       </c>
       <c r="C220" s="8"/>
       <c r="D220" s="7"/>
@@ -11185,10 +11154,10 @@
     </row>
     <row r="221" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A221" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="B221" s="9" t="s">
         <v>816</v>
-      </c>
-      <c r="B221" s="9" t="s">
-        <v>817</v>
       </c>
       <c r="C221" s="8"/>
       <c r="D221" s="7"/>
@@ -11196,7 +11165,7 @@
     </row>
     <row r="222" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" s="7" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B222" s="9" t="s">
         <v>393</v>
@@ -11207,10 +11176,10 @@
     </row>
     <row r="223" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A223" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="B223" s="9" t="s">
         <v>819</v>
-      </c>
-      <c r="B223" s="9" t="s">
-        <v>820</v>
       </c>
       <c r="C223" s="8"/>
       <c r="D223" s="7"/>
@@ -11218,7 +11187,7 @@
     </row>
     <row r="224" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" s="7" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B224" s="9" t="s">
         <v>397</v>
@@ -11229,10 +11198,10 @@
     </row>
     <row r="225" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A225" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="B225" s="9" t="s">
         <v>822</v>
-      </c>
-      <c r="B225" s="9" t="s">
-        <v>823</v>
       </c>
       <c r="C225" s="8"/>
       <c r="D225" s="7"/>
@@ -11240,10 +11209,10 @@
     </row>
     <row r="226" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A226" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="B226" s="9" t="s">
         <v>824</v>
-      </c>
-      <c r="B226" s="9" t="s">
-        <v>825</v>
       </c>
       <c r="C226" s="8"/>
       <c r="D226" s="7"/>
@@ -11307,44 +11276,44 @@
     </row>
     <row r="231" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B231" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="C231" s="3" t="s">
         <v>945</v>
       </c>
-      <c r="C231" s="3" t="s">
+      <c r="D231" s="3" t="s">
         <v>946</v>
       </c>
-      <c r="D231" s="3" t="s">
+      <c r="E231" s="3" t="s">
         <v>947</v>
-      </c>
-      <c r="E231" s="3" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
+        <v>941</v>
+      </c>
+      <c r="B232" s="4" t="s">
         <v>942</v>
       </c>
-      <c r="B232" s="4" t="s">
+      <c r="C232" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="E232" s="3" t="s">
         <v>943</v>
-      </c>
-      <c r="C232" s="3" t="s">
-        <v>943</v>
-      </c>
-      <c r="D232" s="3" t="s">
-        <v>949</v>
-      </c>
-      <c r="E232" s="3" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A233" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="B233" s="4" t="s">
         <v>911</v>
-      </c>
-      <c r="B233" s="4" t="s">
-        <v>912</v>
       </c>
       <c r="D233" s="3"/>
       <c r="E233" s="3"/>
@@ -11401,19 +11370,19 @@
     </row>
     <row r="238" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
+        <v>825</v>
+      </c>
+      <c r="B238" s="4" t="s">
         <v>826</v>
       </c>
-      <c r="B238" s="4" t="s">
+      <c r="C238" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="C238" s="3" t="s">
+      <c r="D238" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D238" s="3" t="s">
+      <c r="E238" s="3" t="s">
         <v>829</v>
-      </c>
-      <c r="E238" s="3" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -11473,7 +11442,7 @@
     </row>
     <row r="244" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A244" s="7" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B244" s="9" t="s">
         <v>423</v>
@@ -11484,10 +11453,10 @@
     </row>
     <row r="245" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A245" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="B245" s="9" t="s">
         <v>832</v>
-      </c>
-      <c r="B245" s="9" t="s">
-        <v>833</v>
       </c>
       <c r="C245" s="8"/>
       <c r="D245" s="7"/>
@@ -11495,10 +11464,10 @@
     </row>
     <row r="246" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A246" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="B246" s="9" t="s">
         <v>834</v>
-      </c>
-      <c r="B246" s="9" t="s">
-        <v>835</v>
       </c>
       <c r="C246" s="8"/>
       <c r="D246" s="7"/>
@@ -11506,10 +11475,10 @@
     </row>
     <row r="247" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A247" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="B247" s="9" t="s">
         <v>836</v>
-      </c>
-      <c r="B247" s="9" t="s">
-        <v>837</v>
       </c>
       <c r="C247" s="8"/>
       <c r="D247" s="7"/>
@@ -11517,300 +11486,300 @@
     </row>
     <row r="248" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="249" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="250" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
+        <v>965</v>
+      </c>
+      <c r="B250" s="4" t="s">
         <v>966</v>
-      </c>
-      <c r="B250" s="4" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
+        <v>967</v>
+      </c>
+      <c r="B251" s="4" t="s">
         <v>968</v>
-      </c>
-      <c r="B251" s="4" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="253" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="254" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A254" s="7" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D255" s="3"/>
       <c r="E255" s="3"/>
     </row>
     <row r="256" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
+        <v>973</v>
+      </c>
+      <c r="B257" s="4" t="s">
         <v>974</v>
-      </c>
-      <c r="B257" s="4" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
+        <v>975</v>
+      </c>
+      <c r="B258" s="4" t="s">
         <v>976</v>
-      </c>
-      <c r="B258" s="4" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
+        <v>977</v>
+      </c>
+      <c r="B259" s="4" t="s">
         <v>978</v>
-      </c>
-      <c r="B259" s="4" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
+        <v>979</v>
+      </c>
+      <c r="B260" s="4" t="s">
         <v>980</v>
-      </c>
-      <c r="B260" s="4" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
+        <v>983</v>
+      </c>
+      <c r="B262" s="4" t="s">
         <v>984</v>
-      </c>
-      <c r="B262" s="4" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
+        <v>991</v>
+      </c>
+      <c r="B264" s="4" t="s">
         <v>992</v>
-      </c>
-      <c r="B264" s="4" t="s">
-        <v>993</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
+        <v>993</v>
+      </c>
+      <c r="B266" s="4" t="s">
         <v>994</v>
-      </c>
-      <c r="B266" s="4" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
+        <v>989</v>
+      </c>
+      <c r="B267" s="4" t="s">
         <v>990</v>
-      </c>
-      <c r="B267" s="4" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
+        <v>862</v>
+      </c>
+      <c r="B268" s="4" t="s">
         <v>863</v>
       </c>
-      <c r="B268" s="4" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="269" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B270" s="4" t="s">
         <v>1004</v>
-      </c>
-      <c r="B270" s="4" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B271" s="4" t="s">
         <v>1006</v>
-      </c>
-      <c r="B271" s="4" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
   </sheetData>
@@ -11854,90 +11823,90 @@
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>837</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>838</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>840</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>841</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>842</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>843</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>844</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>845</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>846</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>847</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>848</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>849</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>850</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>851</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>852</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>853</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>854</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>855</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>856</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>857</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>858</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -11970,6 +11939,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -12223,15 +12201,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
   <ds:schemaRefs>
@@ -12245,6 +12214,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12262,12 +12239,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: QA modal done
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17820EF1-01BF-EF4E-B120-084CB0BD65D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA2BC5B-156E-EB4B-A4D6-D59B8976FFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35400" yWindow="-600" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="-38280" yWindow="-600" windowWidth="24180" windowHeight="18880" activeTab="1" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT_reference" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="1129">
   <si>
     <t>LABEL</t>
   </si>
@@ -3419,6 +3419,30 @@
   </si>
   <si>
     <t>Presencia de casos o brotes de</t>
+  </si>
+  <si>
+    <t>quality_title</t>
+  </si>
+  <si>
+    <t>Completitud del dato</t>
+  </si>
+  <si>
+    <t>Municipios para los que se incluyó información</t>
+  </si>
+  <si>
+    <t>Municipios para los que se incluyó información completa</t>
+  </si>
+  <si>
+    <t>Municipios del país</t>
+  </si>
+  <si>
+    <t>quality_admin2_total</t>
+  </si>
+  <si>
+    <t>quality_admin2_included</t>
+  </si>
+  <si>
+    <t>quality_admin2_complete</t>
   </si>
 </sst>
 </file>
@@ -6090,10 +6114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7047,6 +7071,78 @@
         <v>1106</v>
       </c>
     </row>
+    <row r="96" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>487</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>489</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>491</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>495</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>497</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>1124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7056,8 +7152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DBD2-0F3F-5E4C-83A2-49E17C536753}">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:B7"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8310,7 +8406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A279" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A279" zoomScale="150" workbookViewId="0">
       <selection activeCell="B287" sqref="B287"/>
     </sheetView>
   </sheetViews>
@@ -11989,6 +12085,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004BF2CC58B4B21249B9847CAE6C292121" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20382285bea758b172f195e70f01161d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07d4ffe0-35c4-4630-b07d-57ff54db67ac" xmlns:ns3="3a79588a-61f1-49eb-bf82-c7b2c97b1d12" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6472e07e44c21502ea15ef197acea5c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="07d4ffe0-35c4-4630-b07d-57ff54db67ac"/>
@@ -12242,15 +12347,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9D65FF-F2FD-4C20-A5A5-187B450DED94}">
   <ds:schemaRefs>
@@ -12264,6 +12360,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E63CBD55-76B1-4172-879F-D383FAB08852}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12281,12 +12385,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F89B1EF0-638A-46E6-AC33-5AA4149722BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: footnotes in HTML report
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4CE1FA-B926-1E41-B7D5-003CDD21F1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE59F1F1-444E-2740-9434-A9AD5E16A62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="760" windowWidth="24180" windowHeight="18880" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="5" r:id="rId1"/>
-    <sheet name="QA_REPORT" sheetId="6" r:id="rId2"/>
-    <sheet name="DASHBOARD" sheetId="3" r:id="rId3"/>
-    <sheet name="MSG" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="QA_REPORT" sheetId="6" r:id="rId3"/>
+    <sheet name="DASHBOARD" sheetId="3" r:id="rId4"/>
+    <sheet name="MSG" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DASHBOARD!$A$1:$E$251</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MSG!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">DASHBOARD!$A$1:$E$251</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">MSG!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="964">
   <si>
     <t>LABEL</t>
   </si>
@@ -2905,6 +2906,45 @@
   </si>
   <si>
     <t>&lt;100000 hábitantes menores de 15 años que no haya tenido casos de PFA en el último año</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a^a </t>
+  </si>
+  <si>
+    <t>Población &lt;1 año para el año de evaluación*</t>
+  </si>
+  <si>
+    <t>Población &lt;5 año para el año de evaluación*</t>
+  </si>
+  <si>
+    <t>Población &lt;15 año para el año de evaluación*</t>
+  </si>
+  <si>
+    <t>table_1a_pob1_html</t>
+  </si>
+  <si>
+    <t>table_1a_pob5_html</t>
+  </si>
+  <si>
+    <t>table_1a_pob15_html</t>
+  </si>
+  <si>
+    <t>table_1b_pob1_html</t>
+  </si>
+  <si>
+    <t>table_1b_pob5_html</t>
+  </si>
+  <si>
+    <t>table_1b_pob15_html</t>
+  </si>
+  <si>
+    <t>Población &lt;1 (%)*</t>
+  </si>
+  <si>
+    <t>Población &lt;5 (%)*</t>
+  </si>
+  <si>
+    <t>Población &lt;15 (%)*</t>
   </si>
 </sst>
 </file>
@@ -3062,7 +3102,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3372,10 +3433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3867,561 +3928,612 @@
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>955</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>956</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>957</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>865</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>867</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>869</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>871</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>873</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>874</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>875</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>958</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>959</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>960</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>877</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>878</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>879</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="64" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>880</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>948</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>762</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>764</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>765</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>132</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>137</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>697</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>793</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>793</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>161</v>
+        <v>762</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>165</v>
+        <v>763</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>764</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>691</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>32</v>
+        <v>789</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>765</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>36</v>
+        <v>790</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>690</v>
+        <v>133</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>42</v>
+        <v>463</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>43</v>
+        <v>464</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>44</v>
+        <v>465</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>45</v>
+        <v>466</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>166</v>
+        <v>697</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="D70"/>
-      <c r="E70"/>
+        <v>793</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>881</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>876</v>
+        <v>157</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>467</v>
+        <v>158</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>468</v>
+        <v>792</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>469</v>
+        <v>159</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>470</v>
+        <v>690</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>460</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>882</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D76"/>
+      <c r="E76"/>
+    </row>
+    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>884</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>885</v>
+        <v>167</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>881</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>467</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>469</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>460</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>882</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>884</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>942</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>887</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>888</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="87" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>890</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="88" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>889</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="89" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>677</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B89" s="17" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="C89" s="3" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>678</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>708</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>98</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="93" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>189</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>704</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>710</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="96" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>715</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="97" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>721</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="98" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>725</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+    <row r="99" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>729</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="100" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>733</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>734</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>940</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>894</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>896</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>943</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>912</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>337</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>339</v>
+        <v>940</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>341</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>894</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>343</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>896</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>345</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>346</v>
+        <v>943</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>944</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>912</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>337</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>339</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>341</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>343</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>345</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>917</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>916</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+    <row r="112" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>918</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>914</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+    <row r="113" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>919</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>915</v>
       </c>
     </row>
@@ -4431,6 +4543,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518FB3B-1B86-0649-AF4F-61022D4FE493}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DBD2-0F3F-5E4C-83A2-49E17C536753}">
   <dimension ref="A1:E74"/>
   <sheetViews>
@@ -5068,7 +5194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01EA010-864B-8746-BF5D-2E469295667F}">
   <dimension ref="A1:E291"/>
   <sheetViews>
@@ -8646,7 +8772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1088E479-CA72-964B-98C9-FB941DEE85DA}">
   <dimension ref="A1:E12"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat: agregue excel descargable con clave de como se calculan los punteos y las categorias de riesgo
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EE3ABE-4A92-874C-B1CF-459F1700A27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EB62BF-6306-8F43-B123-03EF16A350A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8480" yWindow="760" windowWidth="19080" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="680">
   <si>
     <t>LABEL</t>
   </si>
@@ -2079,6 +2079,18 @@
   </si>
   <si>
     <t>Resultado del análisis de riesgo</t>
+  </si>
+  <si>
+    <t>download_cutoffs_excel</t>
+  </si>
+  <si>
+    <t>Descargar clave de asignación de puntos de riesgo</t>
+  </si>
+  <si>
+    <t>cutoffs_excel_filename</t>
+  </si>
+  <si>
+    <t>clave_puntos_de_riesgo</t>
   </si>
 </sst>
 </file>
@@ -2176,7 +2188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2195,9 +2207,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2209,9 +2218,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -2225,7 +2231,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2554,7 +2577,7 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -2802,7 +2825,7 @@
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>642</v>
       </c>
     </row>
@@ -2818,7 +2841,7 @@
       <c r="A22" t="s">
         <v>565</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>537</v>
       </c>
     </row>
@@ -3395,7 +3418,7 @@
       <c r="A83" t="s">
         <v>594</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="14" t="s">
         <v>595</v>
       </c>
     </row>
@@ -3443,7 +3466,7 @@
       <c r="A89" t="s">
         <v>389</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="15" t="s">
         <v>658</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -3550,7 +3573,7 @@
       <c r="A102" t="s">
         <v>604</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="12" t="s">
         <v>605</v>
       </c>
     </row>
@@ -3558,7 +3581,7 @@
       <c r="A103" t="s">
         <v>606</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="12" t="s">
         <v>607</v>
       </c>
     </row>
@@ -3566,7 +3589,7 @@
       <c r="A104" t="s">
         <v>652</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="12" t="s">
         <v>653</v>
       </c>
     </row>
@@ -3665,7 +3688,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -3954,7 +3977,7 @@
       <c r="A36" t="s">
         <v>223</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -4287,1972 +4310,1823 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D19EDBB-2148-D941-8C67-E2C52C431560}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="5" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="34" style="19" customWidth="1"/>
+    <col min="2" max="5" width="28.5" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="19" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="21" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="21"/>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="C7" s="21"/>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="20" t="s">
         <v>608</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="20" t="s">
         <v>675</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="20" t="s">
         <v>610</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="C13" s="21"/>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="19" t="s">
         <v>631</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="20" t="s">
         <v>635</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="C14" s="21"/>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="19" t="s">
         <v>632</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="20" t="s">
         <v>636</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="21"/>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="19" t="s">
         <v>633</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="20" t="s">
         <v>637</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="C16" s="21"/>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="19" t="s">
         <v>634</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="21"/>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="21" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="19" t="s">
         <v>385</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="21" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="20" t="s">
         <v>640</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="21" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="21" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="C30" s="21"/>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="21" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="C32" s="21"/>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="21" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="21" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="C35" s="21"/>
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="C36" s="21"/>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+      <c r="C37" s="21"/>
     </row>
     <row r="38" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
+      <c r="C38" s="21"/>
     </row>
     <row r="39" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
+      <c r="C39" s="21"/>
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="21" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
+      <c r="C41" s="21"/>
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="A45" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
+      <c r="C46" s="21"/>
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="21" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="21" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="19" t="s">
         <v>409</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="20" t="s">
         <v>503</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="21" t="s">
         <v>503</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="21" t="s">
         <v>503</v>
       </c>
-      <c r="E49" s="3"/>
+      <c r="E49" s="21"/>
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="A50" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="21" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="A51" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="21" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="A52" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="21" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="A53" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="21" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
+      <c r="C54" s="21"/>
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
+      <c r="C55" s="21"/>
     </row>
     <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="21" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
+      <c r="C58" s="21"/>
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="A59" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="21" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
+      <c r="C60" s="21"/>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
+      <c r="C61" s="21"/>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="19" t="s">
         <v>322</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="21" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="21" t="s">
         <v>325</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="21" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
+      <c r="C64" s="21"/>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
+      <c r="C65" s="21"/>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="19" t="s">
         <v>332</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
+      <c r="C66" s="21"/>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
+      <c r="C67" s="21"/>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
+      <c r="C68" s="21"/>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
+      <c r="C69" s="21"/>
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="19" t="s">
         <v>340</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
+      <c r="C70" s="21"/>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
+      <c r="C71" s="21"/>
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
+      <c r="C72" s="21"/>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
+      <c r="C73" s="21"/>
     </row>
     <row r="74" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
+      <c r="C74" s="21"/>
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-    </row>
-    <row r="76" spans="1:5" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
+      <c r="C75" s="21"/>
+    </row>
+    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="20" t="s">
         <v>398</v>
       </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
     </row>
     <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
+      <c r="C77" s="21"/>
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="19" t="s">
         <v>399</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="20" t="s">
         <v>400</v>
       </c>
-      <c r="C78" s="8"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
+      <c r="C78" s="21"/>
     </row>
     <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="20" t="s">
         <v>611</v>
       </c>
-      <c r="C79" s="8"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
+      <c r="C79" s="21"/>
     </row>
     <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="19" t="s">
         <v>401</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="20" t="s">
         <v>612</v>
       </c>
-      <c r="C80" s="8"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
+      <c r="C80" s="21"/>
     </row>
     <row r="81" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="19" t="s">
         <v>394</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="20" t="s">
         <v>613</v>
       </c>
-      <c r="C81" s="8"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
+      <c r="C81" s="21"/>
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="C82" s="8"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
+      <c r="C82" s="21"/>
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="20" t="s">
         <v>504</v>
       </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
+      <c r="C83" s="21"/>
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="19" t="s">
         <v>456</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="20" t="s">
         <v>457</v>
       </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
+      <c r="C84" s="21"/>
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="19" t="s">
         <v>458</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B85" s="20" t="s">
         <v>615</v>
       </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
+      <c r="C85" s="21"/>
     </row>
     <row r="86" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
+      <c r="C86" s="21"/>
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="A87" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C87" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C88" s="8"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
+      <c r="C88" s="21"/>
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C89" s="8"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
+      <c r="C89" s="21"/>
     </row>
     <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="C90" s="8"/>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
+      <c r="C90" s="21"/>
     </row>
     <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="19" t="s">
         <v>353</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="C91" s="8"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
+      <c r="C91" s="21"/>
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C92" s="8"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
+      <c r="C92" s="21"/>
     </row>
     <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
+      <c r="C93" s="21"/>
     </row>
     <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="C94" s="8"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
+      <c r="C94" s="21"/>
     </row>
     <row r="95" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B95" s="20" t="s">
         <v>616</v>
       </c>
-      <c r="C95" s="8"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
+      <c r="C95" s="21"/>
     </row>
     <row r="96" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="19" t="s">
         <v>414</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-    </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
+      <c r="C96" s="21"/>
+    </row>
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="19" t="s">
         <v>416</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="C97" s="8"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
-    </row>
-    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="7" t="s">
+      <c r="C97" s="21"/>
+    </row>
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="19" t="s">
         <v>459</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B98" s="20" t="s">
         <v>460</v>
       </c>
-      <c r="C98" s="8"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-    </row>
-    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
+      <c r="C98" s="21"/>
+    </row>
+    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="19" t="s">
         <v>420</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-    </row>
-    <row r="100" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A100" s="7" t="s">
+      <c r="C99" s="21"/>
+    </row>
+    <row r="100" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A100" s="19" t="s">
         <v>421</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="20" t="s">
         <v>422</v>
       </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
-    </row>
-    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+      <c r="C100" s="21"/>
+    </row>
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="19" t="s">
         <v>423</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B101" s="20" t="s">
         <v>424</v>
       </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="7"/>
-      <c r="E101" s="7"/>
-    </row>
-    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="7" t="s">
+      <c r="C101" s="21"/>
+    </row>
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="19" t="s">
         <v>470</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B102" s="20" t="s">
         <v>461</v>
       </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-    </row>
-    <row r="103" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
+      <c r="C102" s="21"/>
+    </row>
+    <row r="103" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A103" s="19" t="s">
         <v>425</v>
       </c>
-      <c r="B103" s="9" t="s">
+      <c r="B103" s="20" t="s">
         <v>426</v>
       </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-    </row>
-    <row r="104" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
+      <c r="C103" s="21"/>
+    </row>
+    <row r="104" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="B104" s="9" t="s">
+      <c r="B104" s="20" t="s">
         <v>428</v>
       </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="7"/>
-      <c r="E104" s="7"/>
-    </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
+      <c r="C104" s="21"/>
+    </row>
+    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="20" t="s">
         <v>432</v>
       </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
-    </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
+      <c r="C105" s="21"/>
+    </row>
+    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="19" t="s">
         <v>462</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B106" s="20" t="s">
         <v>463</v>
       </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-    </row>
-    <row r="107" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
+      <c r="C106" s="21"/>
+    </row>
+    <row r="107" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A107" s="19" t="s">
         <v>431</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="B107" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
-    </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
+      <c r="C107" s="21"/>
+    </row>
+    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B108" s="20" t="s">
         <v>639</v>
       </c>
-      <c r="C108" s="8"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="7"/>
-    </row>
-    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
+      <c r="C108" s="21"/>
+    </row>
+    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="19" t="s">
         <v>464</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="C109" s="8"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="7"/>
-    </row>
-    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
+      <c r="C109" s="21"/>
+    </row>
+    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="19" t="s">
         <v>437</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B110" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C110" s="8"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-    </row>
-    <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
+      <c r="C110" s="21"/>
+    </row>
+    <row r="111" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A111" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="B111" s="20" t="s">
         <v>436</v>
       </c>
-      <c r="C111" s="8"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
-    </row>
-    <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
+      <c r="C111" s="21"/>
+    </row>
+    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="19" t="s">
         <v>438</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B112" s="20" t="s">
         <v>440</v>
       </c>
-      <c r="C112" s="8"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
+      <c r="C112" s="21"/>
     </row>
     <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
+      <c r="A113" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="B113" s="9" t="s">
+      <c r="B113" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="C113" s="8"/>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
+      <c r="C113" s="21"/>
     </row>
     <row r="114" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="19" t="s">
         <v>439</v>
       </c>
-      <c r="B114" s="9" t="s">
+      <c r="B114" s="20" t="s">
         <v>441</v>
       </c>
-      <c r="C114" s="8"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
+      <c r="C114" s="21"/>
     </row>
     <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="B115" s="20" t="s">
         <v>505</v>
       </c>
-      <c r="C115" s="8"/>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
+      <c r="C115" s="21"/>
     </row>
     <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
+      <c r="A116" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B116" s="20" t="s">
         <v>469</v>
       </c>
-      <c r="C116" s="8"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
+      <c r="C116" s="21"/>
     </row>
     <row r="117" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A117" s="7" t="s">
+      <c r="A117" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B117" s="20" t="s">
         <v>444</v>
       </c>
-      <c r="C117" s="8"/>
-      <c r="D117" s="7"/>
-      <c r="E117" s="7"/>
+      <c r="C117" s="21"/>
     </row>
     <row r="118" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
+      <c r="A118" s="19" t="s">
         <v>445</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B118" s="20" t="s">
         <v>446</v>
       </c>
-      <c r="C118" s="8"/>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
+      <c r="C118" s="21"/>
     </row>
     <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B119" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C119" s="8"/>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
+      <c r="C119" s="21"/>
     </row>
     <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
+      <c r="A120" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B120" s="9" t="s">
+      <c r="B120" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="C120" s="8"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
+      <c r="C120" s="21"/>
     </row>
     <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="A121" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="E121" s="3" t="s">
+      <c r="E121" s="21" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="A122" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C122" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="D122" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="E122" s="3" t="s">
+      <c r="E122" s="21" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="A123" s="19" t="s">
         <v>447</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="20" t="s">
         <v>451</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C123" s="21" t="s">
         <v>452</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="21" t="s">
         <v>453</v>
       </c>
-      <c r="E123" s="3" t="s">
+      <c r="E123" s="21" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+      <c r="A124" s="19" t="s">
         <v>448</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="20" t="s">
         <v>449</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="C124" s="21" t="s">
         <v>449</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D124" s="21" t="s">
         <v>455</v>
       </c>
-      <c r="E124" s="3" t="s">
+      <c r="E124" s="21" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="7" t="s">
+      <c r="A125" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
+      <c r="C125" s="21"/>
+      <c r="D125" s="21"/>
+      <c r="E125" s="21"/>
     </row>
     <row r="126" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="A126" s="19" t="s">
         <v>389</v>
       </c>
-      <c r="B126" s="13" t="s">
+      <c r="B126" s="22" t="s">
         <v>404</v>
       </c>
-      <c r="C126" s="3"/>
+      <c r="C126" s="21"/>
     </row>
     <row r="127" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="A127" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="20" t="s">
         <v>405</v>
       </c>
-      <c r="C127" s="3"/>
+      <c r="C127" s="21"/>
     </row>
     <row r="128" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="A128" s="19" t="s">
         <v>471</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="20" t="s">
         <v>641</v>
       </c>
-      <c r="C128" s="3"/>
+      <c r="C128" s="21"/>
     </row>
     <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="A129" s="19" t="s">
         <v>472</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="C129" s="3"/>
+      <c r="C129" s="21"/>
     </row>
     <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="A130" s="19" t="s">
         <v>474</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="20" t="s">
         <v>673</v>
       </c>
-      <c r="C130" s="3"/>
+      <c r="C130" s="21"/>
     </row>
     <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="A131" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="20" t="s">
         <v>674</v>
       </c>
-      <c r="C131" s="3"/>
+      <c r="C131" s="21"/>
     </row>
     <row r="132" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A132" s="7" t="s">
+      <c r="A132" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="B132" s="9" t="s">
+      <c r="B132" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="C132" s="3"/>
+      <c r="C132" s="21"/>
     </row>
     <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="A133" s="19" t="s">
         <v>379</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
-      <c r="E133" s="3"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="21"/>
     </row>
     <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="A134" s="19" t="s">
         <v>477</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="C134" s="3"/>
+      <c r="C134" s="21"/>
     </row>
     <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="A135" s="19" t="s">
         <v>478</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="C135" s="3"/>
+      <c r="C135" s="21"/>
     </row>
     <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="A136" s="19" t="s">
         <v>480</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="C136" s="3"/>
+      <c r="C136" s="21"/>
     </row>
     <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+      <c r="A137" s="19" t="s">
         <v>481</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="C137" s="3"/>
+      <c r="C137" s="21"/>
     </row>
     <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="A138" s="19" t="s">
         <v>483</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="C138" s="3"/>
+      <c r="C138" s="21"/>
     </row>
     <row r="139" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+      <c r="A139" s="19" t="s">
         <v>486</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B139" s="20" t="s">
         <v>490</v>
       </c>
-      <c r="C139" s="3"/>
+      <c r="C139" s="21"/>
     </row>
     <row r="140" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="A140" s="19" t="s">
         <v>487</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="20" t="s">
         <v>488</v>
       </c>
-      <c r="C140" s="3"/>
+      <c r="C140" s="21"/>
     </row>
     <row r="141" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="A141" s="19" t="s">
         <v>489</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="20" t="s">
         <v>491</v>
       </c>
-      <c r="C141" s="3"/>
+      <c r="C141" s="21"/>
     </row>
     <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="A142" s="19" t="s">
         <v>495</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B142" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="C142" s="3"/>
+      <c r="C142" s="21"/>
     </row>
     <row r="143" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="A143" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C143" s="3"/>
+      <c r="C143" s="21"/>
     </row>
     <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+      <c r="A144" s="19" t="s">
         <v>497</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="20" t="s">
         <v>498</v>
       </c>
-      <c r="C144" s="3"/>
+      <c r="C144" s="21"/>
     </row>
     <row r="145" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="A145" s="19" t="s">
         <v>493</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="C145" s="3"/>
+      <c r="C145" s="21"/>
     </row>
     <row r="146" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+      <c r="A146" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="C146" s="3"/>
+      <c r="C146" s="21"/>
     </row>
     <row r="147" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="A147" s="19" t="s">
         <v>506</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="C147" s="3"/>
+      <c r="C147" s="21"/>
     </row>
     <row r="148" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="A148" s="19" t="s">
         <v>507</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="20" t="s">
         <v>508</v>
       </c>
-      <c r="C148" s="3"/>
+      <c r="C148" s="21"/>
     </row>
     <row r="149" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="A149" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="C149" s="3"/>
+      <c r="C149" s="21"/>
     </row>
     <row r="150" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="A150" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B150" s="20" t="s">
         <v>523</v>
       </c>
-      <c r="C150" s="3"/>
+      <c r="C150" s="21"/>
     </row>
     <row r="151" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="A151" s="19" t="s">
         <v>512</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="C151" s="3"/>
+      <c r="C151" s="21"/>
     </row>
     <row r="152" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="A152" s="19" t="s">
         <v>513</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B152" s="20" t="s">
         <v>525</v>
       </c>
-      <c r="C152" s="3"/>
+      <c r="C152" s="21"/>
     </row>
     <row r="153" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="A153" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B153" s="20" t="s">
         <v>526</v>
       </c>
-      <c r="C153" s="3"/>
+      <c r="C153" s="21"/>
     </row>
     <row r="154" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="A154" s="19" t="s">
         <v>515</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="20" t="s">
         <v>527</v>
       </c>
-      <c r="C154" s="3"/>
+      <c r="C154" s="21"/>
     </row>
     <row r="155" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+      <c r="A155" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="20" t="s">
         <v>528</v>
       </c>
-      <c r="C155" s="3"/>
+      <c r="C155" s="21"/>
     </row>
     <row r="156" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+      <c r="A156" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B156" s="20" t="s">
         <v>529</v>
       </c>
-      <c r="C156" s="3"/>
+      <c r="C156" s="21"/>
     </row>
     <row r="157" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="A157" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B157" s="20" t="s">
         <v>530</v>
       </c>
-      <c r="C157" s="3"/>
+      <c r="C157" s="21"/>
     </row>
     <row r="158" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+      <c r="A158" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B158" s="20" t="s">
         <v>531</v>
       </c>
-      <c r="C158" s="3"/>
+      <c r="C158" s="21"/>
     </row>
     <row r="159" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+      <c r="A159" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B159" s="20" t="s">
         <v>532</v>
       </c>
-      <c r="C159" s="3"/>
+      <c r="C159" s="21"/>
     </row>
     <row r="160" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="A160" s="19" t="s">
         <v>521</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B160" s="20" t="s">
         <v>533</v>
       </c>
-      <c r="C160" s="3"/>
+      <c r="C160" s="21"/>
     </row>
     <row r="161" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+      <c r="A161" s="19" t="s">
         <v>522</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B161" s="20" t="s">
         <v>534</v>
       </c>
-      <c r="C161" s="3"/>
+      <c r="C161" s="21"/>
     </row>
     <row r="162" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+      <c r="A162" s="19" t="s">
         <v>535</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B162" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="C162" s="3"/>
+      <c r="C162" s="21"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
+      <c r="A163" s="19" t="s">
         <v>617</v>
       </c>
-      <c r="B163" s="18" t="s">
+      <c r="B163" s="23" t="s">
         <v>505</v>
       </c>
-      <c r="C163" s="3"/>
+      <c r="C163" s="21"/>
     </row>
     <row r="164" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
+      <c r="A164" s="19" t="s">
         <v>618</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B164" s="20" t="s">
         <v>619</v>
       </c>
-      <c r="C164" s="3"/>
+      <c r="C164" s="21"/>
     </row>
     <row r="165" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+      <c r="A165" s="19" t="s">
         <v>620</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B165" s="20" t="s">
         <v>621</v>
       </c>
-      <c r="C165" s="3"/>
+      <c r="C165" s="21"/>
+    </row>
+    <row r="166" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A167" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>679</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: Observaciones AR 22.12.2023
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EB62BF-6306-8F43-B123-03EF16A350A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB47310-C99A-2C42-880D-DFA33D840C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="760" windowWidth="19080" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="8480" yWindow="760" windowWidth="19080" windowHeight="18880" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="5" r:id="rId1"/>
@@ -2565,7 +2565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B573AB-F930-C946-836D-23C069CE4AE0}">
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4312,8 +4314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D19EDBB-2148-D941-8C67-E2C52C431560}">
   <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
refactor: agregue el titulo de Detalle por componente
</commit_message>
<xml_diff>
--- a/src/R/translations.xlsx
+++ b/src/R/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F733FBFF-1A9E-0F44-994A-6930968CD70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB96DC3-FFB7-334F-8D49-3E99CCCA363A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="760" windowWidth="19080" windowHeight="18880" activeTab="3" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
+    <workbookView xWindow="2360" yWindow="780" windowWidth="19080" windowHeight="18880" activeTab="2" xr2:uid="{41A3C097-9B5C-484B-88DA-6A6C7D19F152}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="5" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="1432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1434">
   <si>
     <t>LABEL</t>
   </si>
@@ -4383,6 +4383,12 @@
   </si>
   <si>
     <t>Fermer</t>
+  </si>
+  <si>
+    <t>sidebar_component_detail</t>
+  </si>
+  <si>
+    <t>Detalle por componente</t>
   </si>
 </sst>
 </file>
@@ -8108,10 +8114,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D19EDBB-2148-D941-8C67-E2C52C431560}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E168"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E165"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10942,6 +10948,14 @@
         <v>670</v>
       </c>
     </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="19" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B168" s="19" t="s">
+        <v>1433</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10952,7 +10966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1088E479-CA72-964B-98C9-FB941DEE85DA}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>